<commit_message>
Adding more XML functionality to Actor/Ability Databases.
</commit_message>
<xml_diff>
--- a/xml/Abilities.xlsx
+++ b/xml/Abilities.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="88">
   <si>
     <t>Name</t>
   </si>
@@ -253,13 +253,40 @@
   </si>
   <si>
     <t>Increase the Flexpoint drop rate of defeated enemies.</t>
+  </si>
+  <si>
+    <t>Spec</t>
+  </si>
+  <si>
+    <t>Damage</t>
+  </si>
+  <si>
+    <t>Support</t>
+  </si>
+  <si>
+    <t>Teleport</t>
+  </si>
+  <si>
+    <t>BS</t>
+  </si>
+  <si>
+    <t>Obstacle</t>
+  </si>
+  <si>
+    <t>Passive</t>
+  </si>
+  <si>
+    <t>Healing %</t>
+  </si>
+  <si>
+    <t>Stop</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -273,6 +300,13 @@
       <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -323,15 +357,6 @@
     </border>
     <border>
       <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color theme="0"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color theme="0"/>
       </right>
@@ -372,40 +397,53 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <border outline="0">
-        <bottom style="thick">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
+  <dxfs count="13">
     <dxf>
       <font>
         <b/>
@@ -437,6 +475,389 @@
         </right>
         <top/>
         <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top/>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top/>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top/>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top/>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top/>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top/>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top/>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top/>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top/>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thick">
+          <color theme="0"/>
+        </bottom>
       </border>
     </dxf>
   </dxfs>
@@ -545,43 +966,99 @@
       </xsd:element>
     </xsd:schema>
   </Schema>
+  <Schema ID="Schema5">
+    <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns="">
+      <xsd:element nillable="true" name="Abilities">
+        <xsd:complexType>
+          <xsd:sequence minOccurs="0">
+            <xsd:element minOccurs="0" maxOccurs="unbounded" nillable="true" name="Ability" form="unqualified">
+              <xsd:complexType>
+                <xsd:sequence minOccurs="0">
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Name" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Availability" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Spec" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="Range" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Cooldown" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="Uses" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="Activate" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="Value" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="Delay" form="unqualified"/>
+                </xsd:sequence>
+              </xsd:complexType>
+            </xsd:element>
+          </xsd:sequence>
+        </xsd:complexType>
+      </xsd:element>
+    </xsd:schema>
+  </Schema>
+  <Schema ID="Schema6">
+    <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns="">
+      <xsd:element nillable="true" name="Abilities">
+        <xsd:complexType>
+          <xsd:sequence minOccurs="0">
+            <xsd:element minOccurs="0" maxOccurs="unbounded" nillable="true" name="Ability" form="unqualified">
+              <xsd:complexType>
+                <xsd:sequence minOccurs="0">
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Name" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Availability" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Spec" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="Range" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Cooldown" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="Uses" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="Activate" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="Value" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="Delay" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Description" form="unqualified"/>
+                </xsd:sequence>
+              </xsd:complexType>
+            </xsd:element>
+          </xsd:sequence>
+        </xsd:complexType>
+      </xsd:element>
+    </xsd:schema>
+  </Schema>
   <Map ID="1" Name="Abilities_Map" RootElement="Abilities" SchemaID="Schema1" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true"/>
   <Map ID="2" Name="Abilities_Map1" RootElement="Abilities" SchemaID="Schema2" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true"/>
   <Map ID="3" Name="Abilities_Map2" RootElement="Abilities" SchemaID="Schema3" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true"/>
   <Map ID="4" Name="Abilities_Map3" RootElement="Abilities" SchemaID="Schema4" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true"/>
+  <Map ID="5" Name="Abilities_Map4" RootElement="Abilities" SchemaID="Schema5" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true"/>
+  <Map ID="6" Name="Abilities_Map5" RootElement="Abilities" SchemaID="Schema6" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true"/>
 </MapInfo>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A2:I32" tableType="xml" totalsRowShown="0" headerRowDxfId="1" headerRowBorderDxfId="0">
-  <autoFilter ref="A2:I32"/>
-  <tableColumns count="9">
-    <tableColumn id="1" uniqueName="Name" name="Name">
-      <xmlColumnPr mapId="4" xpath="/Abilities/Ability/Name" xmlDataType="string"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:J32" tableType="xml" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" headerRowBorderDxfId="12">
+  <autoFilter ref="A2:J32"/>
+  <tableColumns count="10">
+    <tableColumn id="1" uniqueName="Name" name="Name" dataDxfId="11">
+      <xmlColumnPr mapId="6" xpath="/Abilities/Ability/Name" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="Availability" name="Availability">
-      <xmlColumnPr mapId="4" xpath="/Abilities/Ability/Availability" xmlDataType="string"/>
+    <tableColumn id="2" uniqueName="Availability" name="Availability" dataDxfId="10">
+      <xmlColumnPr mapId="6" xpath="/Abilities/Ability/Availability" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="Range" name="Range">
-      <xmlColumnPr mapId="4" xpath="/Abilities/Ability/Range" xmlDataType="integer"/>
+    <tableColumn id="3" uniqueName="Spec" name="Spec" dataDxfId="9">
+      <xmlColumnPr mapId="6" xpath="/Abilities/Ability/Spec" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="4" uniqueName="Cooldown" name="Cooldown">
-      <xmlColumnPr mapId="4" xpath="/Abilities/Ability/Cooldown" xmlDataType="integer"/>
+    <tableColumn id="4" uniqueName="Range" name="Range" dataDxfId="8">
+      <xmlColumnPr mapId="6" xpath="/Abilities/Ability/Range" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="5" uniqueName="Uses" name="Uses">
-      <xmlColumnPr mapId="4" xpath="/Abilities/Ability/Uses" xmlDataType="integer"/>
+    <tableColumn id="5" uniqueName="Cooldown" name="Cooldown" dataDxfId="7">
+      <xmlColumnPr mapId="6" xpath="/Abilities/Ability/Cooldown" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="Activate" name="Activate">
-      <xmlColumnPr mapId="4" xpath="/Abilities/Ability/Activate" xmlDataType="integer"/>
+    <tableColumn id="6" uniqueName="Uses" name="Uses" dataDxfId="6">
+      <xmlColumnPr mapId="6" xpath="/Abilities/Ability/Uses" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="Value" name="Value">
-      <xmlColumnPr mapId="4" xpath="/Abilities/Ability/Value" xmlDataType="integer"/>
+    <tableColumn id="7" uniqueName="Activate" name="Activate" dataDxfId="5">
+      <xmlColumnPr mapId="6" xpath="/Abilities/Ability/Activate" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="8" uniqueName="Delay" name="Delay">
-      <xmlColumnPr mapId="4" xpath="/Abilities/Ability/Delay" xmlDataType="integer"/>
+    <tableColumn id="8" uniqueName="Value" name="Value" dataDxfId="4">
+      <xmlColumnPr mapId="6" xpath="/Abilities/Ability/Value" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="9" uniqueName="Description" name="Description">
-      <xmlColumnPr mapId="4" xpath="/Abilities/Ability/Description" xmlDataType="string"/>
+    <tableColumn id="9" uniqueName="Delay" name="Delay" dataDxfId="3">
+      <xmlColumnPr mapId="6" xpath="/Abilities/Ability/Delay" xmlDataType="integer"/>
+    </tableColumn>
+    <tableColumn id="10" uniqueName="Description" name="Description" dataDxfId="2">
+      <xmlColumnPr mapId="6" xpath="/Abilities/Ability/Description" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -873,10 +1350,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I32"/>
+  <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -884,909 +1361,1006 @@
     <col min="1" max="1" width="26.140625" customWidth="1"/>
     <col min="2" max="2" width="13.28515625" customWidth="1"/>
     <col min="3" max="3" width="13.140625" customWidth="1"/>
-    <col min="4" max="5" width="12.140625" customWidth="1"/>
-    <col min="6" max="7" width="10.42578125" customWidth="1"/>
-    <col min="9" max="9" width="106.7109375" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" customWidth="1"/>
+    <col min="9" max="9" width="8" customWidth="1"/>
+    <col min="10" max="10" width="108.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
-      <c r="F1" t="s">
+    <row r="1" spans="1:10">
+      <c r="G1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.75" thickBot="1">
+    <row r="2" spans="1:10" ht="15.75" thickBot="1">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="J2" s="10" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15.75" thickTop="1">
-      <c r="A3" s="16" t="s">
+    <row r="3" spans="1:10" ht="15.75" thickTop="1">
+      <c r="A3" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="3">
+        <v>80</v>
+      </c>
+      <c r="E3" s="14">
         <v>200</v>
       </c>
-      <c r="E3" s="16">
+      <c r="F3" s="8">
         <v>1</v>
       </c>
-      <c r="F3" s="16">
+      <c r="G3" s="8">
         <v>2</v>
       </c>
-      <c r="G3" s="16">
-        <v>0</v>
-      </c>
-      <c r="H3" s="16">
+      <c r="H3" s="8">
+        <v>0</v>
+      </c>
+      <c r="I3" s="8">
         <v>24</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" s="11" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="6" t="s">
+    <row r="4" spans="1:10">
+      <c r="A4" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" s="5">
         <v>140</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="15"/>
+      <c r="F4" s="5">
         <v>1</v>
       </c>
-      <c r="F4" s="6">
+      <c r="G4" s="5">
         <v>2</v>
       </c>
-      <c r="G4" s="6">
-        <v>0</v>
-      </c>
-      <c r="H4" s="6">
+      <c r="H4" s="5">
+        <v>0</v>
+      </c>
+      <c r="I4" s="5">
         <v>24</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" s="12" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:10">
+      <c r="A5" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D5" s="3">
         <v>30</v>
       </c>
-      <c r="D5">
+      <c r="E5" s="14">
         <v>150</v>
       </c>
-      <c r="E5" s="4">
+      <c r="F5" s="3">
         <v>1</v>
       </c>
-      <c r="F5" s="4">
+      <c r="G5" s="3">
         <v>2</v>
       </c>
-      <c r="G5" s="4">
-        <v>0</v>
-      </c>
-      <c r="H5" s="4">
+      <c r="H5" s="3">
+        <v>0</v>
+      </c>
+      <c r="I5" s="3">
         <v>12</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" s="11" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="13" t="s">
+    <row r="6" spans="1:10">
+      <c r="A6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D6" s="3">
         <v>400</v>
       </c>
-      <c r="D6" s="4">
+      <c r="E6" s="14">
         <v>16</v>
       </c>
-      <c r="E6" s="4">
+      <c r="F6" s="3">
         <v>1</v>
       </c>
-      <c r="F6" s="4">
+      <c r="G6" s="3">
         <v>1</v>
       </c>
-      <c r="G6" s="4">
-        <v>0</v>
-      </c>
-      <c r="H6" s="4">
+      <c r="H6" s="3">
+        <v>0</v>
+      </c>
+      <c r="I6" s="3">
         <v>6</v>
       </c>
-      <c r="I6" s="10" t="s">
+      <c r="J6" s="11" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:10">
+      <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="D7" s="4">
+      <c r="E7" s="14">
         <v>150</v>
       </c>
-      <c r="E7" s="4">
+      <c r="F7" s="3">
         <v>1</v>
       </c>
-      <c r="F7" s="4">
+      <c r="G7" s="3">
         <v>2</v>
       </c>
-      <c r="G7" s="4">
-        <v>0</v>
-      </c>
-      <c r="H7" s="4">
+      <c r="H7" s="3">
+        <v>0</v>
+      </c>
+      <c r="I7" s="3">
         <v>24</v>
       </c>
-      <c r="I7" s="10" t="s">
+      <c r="J7" s="11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="13" t="s">
+    <row r="8" spans="1:10">
+      <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D8" s="3">
         <v>500</v>
       </c>
-      <c r="D8" s="4">
+      <c r="E8" s="14">
         <v>72</v>
       </c>
-      <c r="E8" s="4">
+      <c r="F8" s="3">
         <v>1</v>
       </c>
-      <c r="F8" s="4">
+      <c r="G8" s="3">
         <v>2</v>
       </c>
-      <c r="G8" s="4">
-        <v>0</v>
-      </c>
-      <c r="H8" s="4">
+      <c r="H8" s="3">
+        <v>0</v>
+      </c>
+      <c r="I8" s="3">
         <v>24</v>
       </c>
-      <c r="I8" s="10" t="s">
+      <c r="J8" s="11" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="13" t="s">
+    <row r="9" spans="1:10">
+      <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="4">
-        <v>0</v>
-      </c>
-      <c r="D9" s="4">
-        <v>0</v>
-      </c>
-      <c r="E9" s="4">
+      <c r="C9" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0</v>
+      </c>
+      <c r="E9" s="14">
+        <v>0</v>
+      </c>
+      <c r="F9" s="3">
         <v>8</v>
       </c>
-      <c r="F9" s="4">
+      <c r="G9" s="3">
         <v>1</v>
       </c>
-      <c r="G9" s="4">
-        <v>0</v>
-      </c>
-      <c r="H9" s="4">
+      <c r="H9" s="3">
+        <v>0</v>
+      </c>
+      <c r="I9" s="3">
         <v>24</v>
       </c>
-      <c r="I9" s="10" t="s">
+      <c r="J9" s="11" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
-      <c r="A10" t="s">
+    <row r="10" spans="1:10">
+      <c r="A10" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="5">
+        <v>80</v>
+      </c>
+      <c r="E10" s="15">
         <v>12</v>
       </c>
-      <c r="E10">
+      <c r="F10" s="5">
         <v>1</v>
       </c>
-      <c r="F10">
+      <c r="G10" s="5">
         <v>1</v>
       </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10">
+      <c r="H10" s="5">
+        <v>0</v>
+      </c>
+      <c r="I10" s="5">
         <v>6</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" s="12" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
-      <c r="A11" t="s">
+    <row r="11" spans="1:10">
+      <c r="A11" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D11" s="3">
         <v>50</v>
       </c>
-      <c r="D11">
+      <c r="E11" s="14">
         <v>60</v>
       </c>
-      <c r="E11">
+      <c r="F11" s="3">
         <v>3</v>
       </c>
-      <c r="F11">
+      <c r="G11" s="3">
         <v>1</v>
       </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11">
+      <c r="H11" s="3">
+        <v>0</v>
+      </c>
+      <c r="I11" s="3">
         <v>24</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" s="11" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
-      <c r="A12" t="s">
+    <row r="12" spans="1:10">
+      <c r="A12" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D12" s="5">
         <v>100</v>
       </c>
-      <c r="D12">
+      <c r="E12" s="15">
         <v>70</v>
       </c>
-      <c r="E12">
+      <c r="F12" s="5">
         <v>1</v>
       </c>
-      <c r="F12">
+      <c r="G12" s="5">
         <v>2</v>
       </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="H12">
+      <c r="H12" s="5">
+        <v>0</v>
+      </c>
+      <c r="I12" s="5">
         <v>24</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" s="12" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
-      <c r="A13" t="s">
+    <row r="13" spans="1:10">
+      <c r="A13" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D13" s="3">
         <v>100</v>
       </c>
-      <c r="D13">
+      <c r="E13" s="14">
         <v>80</v>
       </c>
-      <c r="E13">
+      <c r="F13" s="3">
         <v>1</v>
       </c>
-      <c r="F13">
+      <c r="G13" s="3">
         <v>1</v>
       </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-      <c r="H13">
+      <c r="H13" s="3">
+        <v>0</v>
+      </c>
+      <c r="I13" s="3">
         <v>24</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" s="11" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
-      <c r="A14" t="s">
+    <row r="14" spans="1:10">
+      <c r="A14" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D14" s="5">
         <v>300</v>
       </c>
-      <c r="D14">
+      <c r="E14" s="15">
         <v>12</v>
       </c>
-      <c r="E14">
+      <c r="F14" s="5">
         <v>1</v>
       </c>
-      <c r="F14">
+      <c r="G14" s="5">
         <v>1</v>
       </c>
-      <c r="G14">
-        <v>0</v>
-      </c>
-      <c r="H14">
+      <c r="H14" s="5">
+        <v>0</v>
+      </c>
+      <c r="I14" s="5">
         <v>4</v>
       </c>
-      <c r="I14" t="s">
+      <c r="J14" s="12" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
-      <c r="A15" s="5" t="s">
+    <row r="15" spans="1:10">
+      <c r="A15" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D15" s="5">
         <v>200</v>
       </c>
-      <c r="D15" s="6">
+      <c r="E15" s="15">
         <v>80</v>
       </c>
-      <c r="E15" s="6">
+      <c r="F15" s="5">
         <v>2</v>
       </c>
-      <c r="F15" s="6">
+      <c r="G15" s="5">
         <v>2</v>
       </c>
-      <c r="G15" s="6">
-        <v>0</v>
-      </c>
-      <c r="H15" s="6">
+      <c r="H15" s="5">
+        <v>0</v>
+      </c>
+      <c r="I15" s="5">
         <v>24</v>
       </c>
-      <c r="I15" s="11" t="s">
+      <c r="J15" s="12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
-      <c r="A16" s="3" t="s">
+    <row r="16" spans="1:10">
+      <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D16" s="3">
         <v>500</v>
       </c>
-      <c r="D16" s="4">
+      <c r="E16" s="14">
         <v>120</v>
       </c>
-      <c r="E16" s="4">
+      <c r="F16" s="3">
         <v>5</v>
       </c>
-      <c r="F16" s="4">
+      <c r="G16" s="3">
         <v>2</v>
       </c>
-      <c r="G16" s="4">
-        <v>0</v>
-      </c>
-      <c r="H16" s="4">
+      <c r="H16" s="3">
+        <v>0</v>
+      </c>
+      <c r="I16" s="3">
         <v>8</v>
       </c>
-      <c r="I16" s="10" t="s">
+      <c r="J16" s="11" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
-      <c r="A17" s="7" t="s">
+    <row r="17" spans="1:10">
+      <c r="A17" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="8">
+      <c r="C17" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D17" s="5">
         <v>300</v>
       </c>
-      <c r="D17" s="8">
+      <c r="E17" s="15">
         <v>90</v>
       </c>
-      <c r="E17" s="8">
+      <c r="F17" s="5">
         <v>2</v>
       </c>
-      <c r="F17" s="8">
+      <c r="G17" s="5">
         <v>2</v>
       </c>
-      <c r="G17" s="8">
-        <v>0</v>
-      </c>
-      <c r="H17" s="8">
+      <c r="H17" s="5">
+        <v>0</v>
+      </c>
+      <c r="I17" s="5">
         <v>24</v>
       </c>
-      <c r="I17" s="12" t="s">
+      <c r="J17" s="12" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
-      <c r="A18" s="14" t="s">
+    <row r="18" spans="1:10">
+      <c r="A18" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="8">
-        <v>0</v>
-      </c>
-      <c r="D18" s="8">
-        <v>0</v>
-      </c>
-      <c r="E18" s="8">
-        <v>0</v>
-      </c>
-      <c r="F18" s="8">
-        <v>0</v>
-      </c>
-      <c r="G18" s="8">
-        <v>0</v>
-      </c>
-      <c r="H18" s="8">
-        <v>0</v>
-      </c>
-      <c r="I18" s="12" t="s">
+      <c r="C18" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D18" s="5">
+        <v>0</v>
+      </c>
+      <c r="E18" s="15">
+        <v>0</v>
+      </c>
+      <c r="F18" s="5">
+        <v>0</v>
+      </c>
+      <c r="G18" s="5">
+        <v>0</v>
+      </c>
+      <c r="H18" s="5">
+        <v>0</v>
+      </c>
+      <c r="I18" s="5">
+        <v>0</v>
+      </c>
+      <c r="J18" s="12" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
-      <c r="A19" s="15" t="s">
+    <row r="19" spans="1:10">
+      <c r="A19" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B19" s="15" t="s">
+      <c r="B19" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="15">
+      <c r="C19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D19" s="3">
         <v>60</v>
       </c>
-      <c r="D19" s="15">
+      <c r="E19" s="14">
         <v>8</v>
       </c>
-      <c r="E19" s="15">
+      <c r="F19" s="3">
         <v>1</v>
       </c>
-      <c r="F19" s="15">
+      <c r="G19" s="3">
         <v>1</v>
       </c>
-      <c r="G19" s="15">
-        <v>0</v>
-      </c>
-      <c r="H19" s="15">
+      <c r="H19" s="3">
+        <v>0</v>
+      </c>
+      <c r="I19" s="3">
         <v>4</v>
       </c>
-      <c r="I19" s="15" t="s">
+      <c r="J19" s="11" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
-      <c r="A20" t="s">
+    <row r="20" spans="1:10">
+      <c r="A20" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B20" s="15" t="s">
+      <c r="B20" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D20" s="5">
         <v>70</v>
       </c>
-      <c r="D20">
+      <c r="E20" s="15">
         <v>720</v>
       </c>
-      <c r="E20" s="15">
+      <c r="F20" s="5">
         <v>3</v>
       </c>
-      <c r="F20" s="15">
+      <c r="G20" s="5">
         <v>3</v>
       </c>
-      <c r="G20" s="15">
-        <v>0</v>
-      </c>
-      <c r="H20" s="15">
+      <c r="H20" s="5">
+        <v>0</v>
+      </c>
+      <c r="I20" s="5">
         <v>4</v>
       </c>
-      <c r="I20" t="s">
+      <c r="J20" s="12" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
-      <c r="A21" t="s">
+    <row r="21" spans="1:10">
+      <c r="A21" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B21" s="15" t="s">
+      <c r="B21" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D21" s="3">
         <v>50</v>
       </c>
-      <c r="D21">
+      <c r="E21" s="14">
         <v>720</v>
       </c>
-      <c r="E21" s="15">
+      <c r="F21" s="3">
         <v>3</v>
       </c>
-      <c r="F21" s="15">
+      <c r="G21" s="3">
         <v>1</v>
       </c>
-      <c r="G21" s="15">
-        <v>0</v>
-      </c>
-      <c r="H21" s="15">
+      <c r="H21" s="3">
+        <v>0</v>
+      </c>
+      <c r="I21" s="3">
         <v>72</v>
       </c>
-      <c r="I21" t="s">
+      <c r="J21" s="11" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
-      <c r="A22" t="s">
+    <row r="22" spans="1:10">
+      <c r="A22" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="5">
+        <v>80</v>
+      </c>
+      <c r="E22" s="15">
         <v>100</v>
       </c>
-      <c r="E22" s="15">
+      <c r="F22" s="5">
         <v>5</v>
       </c>
-      <c r="F22" s="15">
+      <c r="G22" s="5">
         <v>2</v>
       </c>
-      <c r="G22" s="15">
-        <v>0</v>
-      </c>
-      <c r="H22" s="15">
+      <c r="H22" s="5">
+        <v>0</v>
+      </c>
+      <c r="I22" s="5">
         <v>12</v>
       </c>
-      <c r="I22" t="s">
+      <c r="J22" s="12" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
-      <c r="A23" t="s">
+    <row r="23" spans="1:10">
+      <c r="A23" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C23">
-        <v>0</v>
-      </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-      <c r="E23">
-        <v>0</v>
-      </c>
-      <c r="F23">
-        <v>0</v>
-      </c>
-      <c r="G23">
-        <v>0</v>
-      </c>
-      <c r="H23">
-        <v>0</v>
-      </c>
-      <c r="I23" t="s">
+      <c r="C23" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D23" s="3">
+        <v>0</v>
+      </c>
+      <c r="E23" s="14">
+        <v>0</v>
+      </c>
+      <c r="F23" s="3">
+        <v>0</v>
+      </c>
+      <c r="G23" s="3">
+        <v>0</v>
+      </c>
+      <c r="H23" s="3">
+        <v>0</v>
+      </c>
+      <c r="I23" s="3">
+        <v>0</v>
+      </c>
+      <c r="J23" s="11" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
-      <c r="A24" t="s">
+    <row r="24" spans="1:10">
+      <c r="A24" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C24">
-        <v>0</v>
-      </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-      <c r="E24">
-        <v>0</v>
-      </c>
-      <c r="F24">
-        <v>0</v>
-      </c>
-      <c r="G24">
-        <v>0</v>
-      </c>
-      <c r="H24">
-        <v>0</v>
-      </c>
-      <c r="I24" t="s">
+      <c r="C24" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D24" s="5">
+        <v>0</v>
+      </c>
+      <c r="E24" s="15">
+        <v>0</v>
+      </c>
+      <c r="F24" s="5">
+        <v>0</v>
+      </c>
+      <c r="G24" s="5">
+        <v>0</v>
+      </c>
+      <c r="H24" s="5">
+        <v>0</v>
+      </c>
+      <c r="I24" s="5">
+        <v>0</v>
+      </c>
+      <c r="J24" s="12" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
-      <c r="A25" t="s">
+    <row r="25" spans="1:10">
+      <c r="A25" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B25" s="15" t="s">
+      <c r="B25" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C25">
-        <v>0</v>
-      </c>
-      <c r="D25">
+      <c r="C25" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D25" s="3">
+        <v>0</v>
+      </c>
+      <c r="E25" s="14">
         <v>720</v>
       </c>
-      <c r="E25" s="15">
+      <c r="F25" s="3">
         <v>1</v>
       </c>
-      <c r="F25" s="15">
+      <c r="G25" s="3">
         <v>1</v>
       </c>
-      <c r="G25" s="15">
+      <c r="H25" s="3">
         <v>20</v>
       </c>
-      <c r="H25" s="15">
+      <c r="I25" s="3">
         <v>12</v>
       </c>
-      <c r="I25" t="s">
+      <c r="J25" s="11" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
-      <c r="A26" t="s">
+    <row r="26" spans="1:10">
+      <c r="A26" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C26">
-        <v>0</v>
-      </c>
-      <c r="D26">
-        <v>0</v>
-      </c>
-      <c r="E26">
-        <v>0</v>
-      </c>
-      <c r="F26">
-        <v>0</v>
-      </c>
-      <c r="G26">
+      <c r="C26" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D26" s="5">
+        <v>0</v>
+      </c>
+      <c r="E26" s="15">
+        <v>0</v>
+      </c>
+      <c r="F26" s="5">
+        <v>0</v>
+      </c>
+      <c r="G26" s="5">
+        <v>0</v>
+      </c>
+      <c r="H26" s="5">
         <v>5</v>
       </c>
-      <c r="H26">
-        <v>0</v>
-      </c>
-      <c r="I26" t="s">
+      <c r="I26" s="5">
+        <v>0</v>
+      </c>
+      <c r="J26" s="12" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
-      <c r="A27" t="s">
+    <row r="27" spans="1:10">
+      <c r="A27" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C27">
-        <v>0</v>
-      </c>
-      <c r="D27">
-        <v>0</v>
-      </c>
-      <c r="E27">
-        <v>0</v>
-      </c>
-      <c r="F27">
-        <v>0</v>
-      </c>
-      <c r="G27">
+      <c r="C27" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D27" s="3">
+        <v>0</v>
+      </c>
+      <c r="E27" s="14">
+        <v>0</v>
+      </c>
+      <c r="F27" s="3">
+        <v>0</v>
+      </c>
+      <c r="G27" s="3">
+        <v>0</v>
+      </c>
+      <c r="H27" s="3">
         <v>5</v>
       </c>
-      <c r="H27">
-        <v>0</v>
-      </c>
-      <c r="I27" t="s">
+      <c r="I27" s="3">
+        <v>0</v>
+      </c>
+      <c r="J27" s="11" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
-      <c r="A28" t="s">
+    <row r="28" spans="1:10">
+      <c r="A28" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C28">
-        <v>0</v>
-      </c>
-      <c r="D28">
-        <v>0</v>
-      </c>
-      <c r="E28">
-        <v>0</v>
-      </c>
-      <c r="F28">
-        <v>0</v>
-      </c>
-      <c r="G28">
+      <c r="C28" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D28" s="5">
+        <v>0</v>
+      </c>
+      <c r="E28" s="15">
+        <v>0</v>
+      </c>
+      <c r="F28" s="5">
+        <v>0</v>
+      </c>
+      <c r="G28" s="5">
+        <v>0</v>
+      </c>
+      <c r="H28" s="5">
         <v>15</v>
       </c>
-      <c r="H28">
-        <v>0</v>
-      </c>
-      <c r="I28" t="s">
+      <c r="I28" s="5">
+        <v>0</v>
+      </c>
+      <c r="J28" s="12" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
-      <c r="A29" t="s">
+    <row r="29" spans="1:10">
+      <c r="A29" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C29">
-        <v>0</v>
-      </c>
-      <c r="D29">
-        <v>0</v>
-      </c>
-      <c r="E29">
-        <v>0</v>
-      </c>
-      <c r="F29">
-        <v>0</v>
-      </c>
-      <c r="G29">
+      <c r="C29" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D29" s="3">
+        <v>0</v>
+      </c>
+      <c r="E29" s="14">
+        <v>0</v>
+      </c>
+      <c r="F29" s="3">
+        <v>0</v>
+      </c>
+      <c r="G29" s="3">
+        <v>0</v>
+      </c>
+      <c r="H29" s="3">
         <v>30</v>
       </c>
-      <c r="H29">
-        <v>0</v>
-      </c>
-      <c r="I29" t="s">
+      <c r="I29" s="3">
+        <v>0</v>
+      </c>
+      <c r="J29" s="11" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
-      <c r="A30" t="s">
+    <row r="30" spans="1:10">
+      <c r="A30" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C30">
-        <v>0</v>
-      </c>
-      <c r="D30">
-        <v>0</v>
-      </c>
-      <c r="E30">
-        <v>0</v>
-      </c>
-      <c r="F30">
-        <v>0</v>
-      </c>
-      <c r="G30">
+      <c r="C30" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D30" s="5">
+        <v>0</v>
+      </c>
+      <c r="E30" s="15">
+        <v>0</v>
+      </c>
+      <c r="F30" s="5">
+        <v>0</v>
+      </c>
+      <c r="G30" s="5">
+        <v>0</v>
+      </c>
+      <c r="H30" s="5">
         <v>60</v>
       </c>
-      <c r="H30">
-        <v>0</v>
-      </c>
-      <c r="I30" t="s">
+      <c r="I30" s="5">
+        <v>0</v>
+      </c>
+      <c r="J30" s="12" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
-      <c r="A31" t="s">
+    <row r="31" spans="1:10">
+      <c r="A31" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B31" s="15" t="s">
+      <c r="B31" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D31" s="3">
         <v>400</v>
       </c>
-      <c r="D31">
+      <c r="E31" s="14">
         <v>48</v>
       </c>
-      <c r="E31" s="15">
+      <c r="F31" s="3">
         <v>1</v>
       </c>
-      <c r="F31" s="15">
+      <c r="G31" s="3">
         <v>2</v>
       </c>
-      <c r="G31" s="15">
-        <v>0</v>
-      </c>
-      <c r="H31" s="15">
+      <c r="H31" s="3">
+        <v>0</v>
+      </c>
+      <c r="I31" s="3">
         <v>12</v>
       </c>
-      <c r="I31" t="s">
+      <c r="J31" s="11" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
-      <c r="A32" s="15" t="s">
+    <row r="32" spans="1:10">
+      <c r="A32" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B32" s="15" t="s">
+      <c r="B32" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="C32" s="15">
+      <c r="C32" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D32" s="7">
         <v>400</v>
       </c>
-      <c r="D32" s="15">
+      <c r="E32" s="16">
         <v>48</v>
       </c>
-      <c r="E32" s="15">
+      <c r="F32" s="7">
         <v>1</v>
       </c>
-      <c r="F32" s="15">
+      <c r="G32" s="7">
         <v>2</v>
       </c>
-      <c r="G32" s="15">
-        <v>0</v>
-      </c>
-      <c r="H32" s="15">
+      <c r="H32" s="7">
+        <v>0</v>
+      </c>
+      <c r="I32" s="7">
         <v>12</v>
       </c>
-      <c r="I32" s="15" t="s">
+      <c r="J32" s="17" t="s">
         <v>57</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Random PlayerDisplay work. Will attempt more later today/tomorrow.
</commit_message>
<xml_diff>
--- a/xml/Abilities.xlsx
+++ b/xml/Abilities.xlsx
@@ -414,7 +414,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -439,67 +439,12 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="13">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -854,10 +799,66 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <border outline="0">
         <bottom style="thick">
           <color theme="0"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
   </dxfs>
@@ -1027,37 +1028,37 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:J32" tableType="xml" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" headerRowBorderDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:J32" tableType="xml" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11">
   <autoFilter ref="A2:J32"/>
   <tableColumns count="10">
-    <tableColumn id="1" uniqueName="Name" name="Name" dataDxfId="11">
+    <tableColumn id="1" uniqueName="Name" name="Name" dataDxfId="9">
       <xmlColumnPr mapId="6" xpath="/Abilities/Ability/Name" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="Availability" name="Availability" dataDxfId="10">
+    <tableColumn id="2" uniqueName="Availability" name="Availability" dataDxfId="8">
       <xmlColumnPr mapId="6" xpath="/Abilities/Ability/Availability" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="Spec" name="Spec" dataDxfId="9">
+    <tableColumn id="3" uniqueName="Spec" name="Spec" dataDxfId="7">
       <xmlColumnPr mapId="6" xpath="/Abilities/Ability/Spec" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="4" uniqueName="Range" name="Range" dataDxfId="8">
+    <tableColumn id="4" uniqueName="Range" name="Range" dataDxfId="6">
       <xmlColumnPr mapId="6" xpath="/Abilities/Ability/Range" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="5" uniqueName="Cooldown" name="Cooldown" dataDxfId="7">
+    <tableColumn id="5" uniqueName="Cooldown" name="Cooldown" dataDxfId="5">
       <xmlColumnPr mapId="6" xpath="/Abilities/Ability/Cooldown" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="Uses" name="Uses" dataDxfId="6">
+    <tableColumn id="6" uniqueName="Uses" name="Uses" dataDxfId="4">
       <xmlColumnPr mapId="6" xpath="/Abilities/Ability/Uses" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="Activate" name="Activate" dataDxfId="5">
+    <tableColumn id="7" uniqueName="Activate" name="Activate" dataDxfId="3">
       <xmlColumnPr mapId="6" xpath="/Abilities/Ability/Activate" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="8" uniqueName="Value" name="Value" dataDxfId="4">
+    <tableColumn id="8" uniqueName="Value" name="Value" dataDxfId="2">
       <xmlColumnPr mapId="6" xpath="/Abilities/Ability/Value" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="9" uniqueName="Delay" name="Delay" dataDxfId="3">
+    <tableColumn id="9" uniqueName="Delay" name="Delay" dataDxfId="1">
       <xmlColumnPr mapId="6" xpath="/Abilities/Ability/Delay" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="10" uniqueName="Description" name="Description" dataDxfId="2">
+    <tableColumn id="10" uniqueName="Description" name="Description" dataDxfId="0">
       <xmlColumnPr mapId="6" xpath="/Abilities/Ability/Description" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -1352,8 +1353,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:J32"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1891,7 +1892,7 @@
       <c r="B18" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="18" t="s">
         <v>85</v>
       </c>
       <c r="D18" s="5">

</xml_diff>

<commit_message>
Random Ability upgrading work and some other stuff I forget.
</commit_message>
<xml_diff>
--- a/xml/Abilities.xlsx
+++ b/xml/Abilities.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="118">
   <si>
     <t>Name</t>
   </si>
@@ -322,6 +322,54 @@
   </si>
   <si>
     <t>[Violation of Personal Space] Charge in a group of enemies, slowing and damaging them</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>Orgo Book Attack</t>
+  </si>
+  <si>
+    <t>Vivian H.</t>
+  </si>
+  <si>
+    <t>Basic Attack: Whack nearby enemies with an Orgo textbook.</t>
+  </si>
+  <si>
+    <t>HPPerc</t>
+  </si>
+  <si>
+    <t>HPLump</t>
+  </si>
+  <si>
+    <t>Voice Attack</t>
+  </si>
+  <si>
+    <t>Huong V.</t>
+  </si>
+  <si>
+    <t>Basic Attack: Creates a sound shockwave.</t>
+  </si>
+  <si>
+    <t>Tickle Fight</t>
+  </si>
+  <si>
+    <t>Awkward Turtle</t>
+  </si>
+  <si>
+    <t>Ramen!</t>
+  </si>
+  <si>
+    <t>Damages nearby enemies. If some are hit, friendship points appear</t>
+  </si>
+  <si>
+    <t>Damages and slows targeted enemy</t>
+  </si>
+  <si>
+    <t>Heals target</t>
   </si>
 </sst>
 </file>
@@ -473,7 +521,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -501,11 +549,73 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="19">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -532,6 +642,149 @@
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
+        <top/>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top/>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top/>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top/>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
         <top/>
         <bottom style="thin">
           <color theme="0"/>
@@ -897,72 +1150,16 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <bottom style="thick">
           <color theme="0"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="0"/>
-        </left>
+      <border outline="0">
         <right style="thin">
           <color theme="0"/>
         </right>
-        <top/>
-        <bottom/>
       </border>
     </dxf>
   </dxfs>
@@ -1175,6 +1372,65 @@
       </xsd:element>
     </xsd:schema>
   </Schema>
+  <Schema ID="Schema9">
+    <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns="">
+      <xsd:element nillable="true" name="Abilities">
+        <xsd:complexType>
+          <xsd:sequence minOccurs="0">
+            <xsd:element minOccurs="0" maxOccurs="unbounded" nillable="true" name="Ability" form="unqualified">
+              <xsd:complexType>
+                <xsd:sequence minOccurs="0">
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Name" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Availability" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Spec" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="Range" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="Cooldown" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="Uses" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="Activate" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="Value" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="Delay" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="Min" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="Max" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="Damage" form="unqualified"/>
+                </xsd:sequence>
+              </xsd:complexType>
+            </xsd:element>
+          </xsd:sequence>
+        </xsd:complexType>
+      </xsd:element>
+    </xsd:schema>
+  </Schema>
+  <Schema ID="Schema10">
+    <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns="">
+      <xsd:element nillable="true" name="Abilities">
+        <xsd:complexType>
+          <xsd:sequence minOccurs="0">
+            <xsd:element minOccurs="0" maxOccurs="unbounded" nillable="true" name="Ability" form="unqualified">
+              <xsd:complexType>
+                <xsd:sequence minOccurs="0">
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Name" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Availability" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Spec" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="Range" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="Cooldown" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="Uses" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="Activate" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="Value" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="Delay" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="Min" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="Max" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="Damage" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="HPPerc" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="HPLump" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Description" form="unqualified"/>
+                </xsd:sequence>
+              </xsd:complexType>
+            </xsd:element>
+          </xsd:sequence>
+        </xsd:complexType>
+      </xsd:element>
+    </xsd:schema>
+  </Schema>
   <Map ID="1" Name="Abilities_Map" RootElement="Abilities" SchemaID="Schema1" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true"/>
   <Map ID="2" Name="Abilities_Map1" RootElement="Abilities" SchemaID="Schema2" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true"/>
   <Map ID="3" Name="Abilities_Map2" RootElement="Abilities" SchemaID="Schema3" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true"/>
@@ -1183,45 +1439,59 @@
   <Map ID="6" Name="Abilities_Map5" RootElement="Abilities" SchemaID="Schema6" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true"/>
   <Map ID="7" Name="Abilities_Map6" RootElement="Abilities" SchemaID="Schema7" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true"/>
   <Map ID="8" Name="Abilities_Map7" RootElement="Abilities" SchemaID="Schema8" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true"/>
+  <Map ID="9" Name="Abilities_Map8" RootElement="Abilities" SchemaID="Schema9" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true"/>
+  <Map ID="10" Name="Abilities_Map9" RootElement="Abilities" SchemaID="Schema10" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true"/>
 </MapInfo>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:K38" tableType="xml" totalsRowShown="0" headerRowDxfId="14" dataDxfId="12" headerRowBorderDxfId="13" tableBorderDxfId="11">
-  <autoFilter ref="A2:K38"/>
-  <tableColumns count="11">
-    <tableColumn id="1" uniqueName="Name" name="Name" dataDxfId="10">
-      <xmlColumnPr mapId="8" xpath="/Abilities/Ability/Name" xmlDataType="string"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:O43" tableType="xml" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" headerRowBorderDxfId="17" tableBorderDxfId="18">
+  <autoFilter ref="A2:O43"/>
+  <tableColumns count="15">
+    <tableColumn id="1" uniqueName="Name" name="Name" dataDxfId="16">
+      <xmlColumnPr mapId="10" xpath="/Abilities/Ability/Name" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="Availability" name="Availability" dataDxfId="9">
-      <xmlColumnPr mapId="8" xpath="/Abilities/Ability/Availability" xmlDataType="string"/>
+    <tableColumn id="2" uniqueName="Availability" name="Availability" dataDxfId="15">
+      <xmlColumnPr mapId="10" xpath="/Abilities/Ability/Availability" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="Spec" name="Spec" dataDxfId="8">
-      <xmlColumnPr mapId="8" xpath="/Abilities/Ability/Spec" xmlDataType="string"/>
+    <tableColumn id="3" uniqueName="Spec" name="Spec" dataDxfId="14">
+      <xmlColumnPr mapId="10" xpath="/Abilities/Ability/Spec" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="4" uniqueName="Range" name="Range" dataDxfId="7">
-      <xmlColumnPr mapId="8" xpath="/Abilities/Ability/Range" xmlDataType="integer"/>
+    <tableColumn id="4" uniqueName="Range" name="Range" dataDxfId="13">
+      <xmlColumnPr mapId="10" xpath="/Abilities/Ability/Range" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="5" uniqueName="Cooldown" name="Cooldown" dataDxfId="6">
-      <xmlColumnPr mapId="8" xpath="/Abilities/Ability/Cooldown" xmlDataType="integer"/>
+    <tableColumn id="5" uniqueName="Cooldown" name="Cooldown" dataDxfId="12">
+      <xmlColumnPr mapId="10" xpath="/Abilities/Ability/Cooldown" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="Uses" name="Uses" dataDxfId="5">
-      <xmlColumnPr mapId="8" xpath="/Abilities/Ability/Uses" xmlDataType="integer"/>
+    <tableColumn id="6" uniqueName="Uses" name="Uses" dataDxfId="11">
+      <xmlColumnPr mapId="10" xpath="/Abilities/Ability/Uses" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="Activate" name="Activate" dataDxfId="4">
-      <xmlColumnPr mapId="8" xpath="/Abilities/Ability/Activate" xmlDataType="integer"/>
+    <tableColumn id="7" uniqueName="Activate" name="Activate" dataDxfId="10">
+      <xmlColumnPr mapId="10" xpath="/Abilities/Ability/Activate" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="8" uniqueName="Value" name="Value" dataDxfId="3">
-      <xmlColumnPr mapId="8" xpath="/Abilities/Ability/Value" xmlDataType="integer"/>
+    <tableColumn id="8" uniqueName="Value" name="Value" dataDxfId="9">
+      <xmlColumnPr mapId="10" xpath="/Abilities/Ability/Value" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="9" uniqueName="Delay" name="Delay" dataDxfId="2">
-      <xmlColumnPr mapId="8" xpath="/Abilities/Ability/Delay" xmlDataType="integer"/>
+    <tableColumn id="9" uniqueName="Delay" name="Delay" dataDxfId="8">
+      <xmlColumnPr mapId="10" xpath="/Abilities/Ability/Delay" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="10" uniqueName="Damage" name="Damage" dataDxfId="1">
-      <xmlColumnPr mapId="8" xpath="/Abilities/Ability/Damage" xmlDataType="integer"/>
+    <tableColumn id="10" uniqueName="Min" name="Min" dataDxfId="7">
+      <xmlColumnPr mapId="10" xpath="/Abilities/Ability/Min" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="11" uniqueName="Description" name="Description" dataDxfId="0">
-      <xmlColumnPr mapId="8" xpath="/Abilities/Ability/Description" xmlDataType="string"/>
+    <tableColumn id="11" uniqueName="Max" name="Max" dataDxfId="6">
+      <xmlColumnPr mapId="10" xpath="/Abilities/Ability/Max" xmlDataType="integer"/>
+    </tableColumn>
+    <tableColumn id="12" uniqueName="Damage" name="Damage" dataDxfId="5">
+      <xmlColumnPr mapId="10" xpath="/Abilities/Ability/Damage" xmlDataType="integer"/>
+    </tableColumn>
+    <tableColumn id="13" uniqueName="HPPerc" name="HPPerc" dataDxfId="4">
+      <xmlColumnPr mapId="10" xpath="/Abilities/Ability/HPPerc" xmlDataType="integer"/>
+    </tableColumn>
+    <tableColumn id="14" uniqueName="HPLump" name="HPLump" dataDxfId="3">
+      <xmlColumnPr mapId="10" xpath="/Abilities/Ability/HPLump" xmlDataType="integer"/>
+    </tableColumn>
+    <tableColumn id="15" uniqueName="Description" name="Description" dataDxfId="2">
+      <xmlColumnPr mapId="10" xpath="/Abilities/Ability/Description" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1513,32 +1783,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K38"/>
+  <dimension ref="A1:O43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
     <col min="2" max="2" width="13.28515625" customWidth="1"/>
-    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="3" max="3" width="10" customWidth="1"/>
     <col min="4" max="4" width="9.28515625" customWidth="1"/>
     <col min="5" max="5" width="11.42578125" customWidth="1"/>
     <col min="6" max="6" width="8" customWidth="1"/>
     <col min="7" max="7" width="10.42578125" customWidth="1"/>
     <col min="9" max="9" width="8" customWidth="1"/>
-    <col min="10" max="10" width="10.28515625" customWidth="1"/>
-    <col min="11" max="11" width="104.28515625" customWidth="1"/>
+    <col min="10" max="10" width="6.85546875" customWidth="1"/>
+    <col min="11" max="11" width="8" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" customWidth="1"/>
+    <col min="13" max="13" width="10" customWidth="1"/>
+    <col min="14" max="14" width="11" customWidth="1"/>
+    <col min="15" max="15" width="107" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:15">
       <c r="G1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15.75" thickBot="1">
+    <row r="2" spans="1:15" ht="15.75" thickBot="1">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1567,13 +1841,25 @@
         <v>8</v>
       </c>
       <c r="J2" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="L2" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="K2" s="18" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="15.75" thickTop="1">
+      <c r="M2" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="N2" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="O2" s="18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="15.75" thickTop="1">
       <c r="A3" s="11" t="s">
         <v>95</v>
       </c>
@@ -1602,13 +1888,25 @@
         <v>12</v>
       </c>
       <c r="J3" s="13">
-        <v>0</v>
-      </c>
-      <c r="K3" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="K3" s="13">
+        <v>5</v>
+      </c>
+      <c r="L3" s="22">
+        <v>0</v>
+      </c>
+      <c r="M3" s="22">
+        <v>0</v>
+      </c>
+      <c r="N3" s="22">
+        <v>0</v>
+      </c>
+      <c r="O3" s="19" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:15">
       <c r="A4" s="11" t="s">
         <v>44</v>
       </c>
@@ -1639,11 +1937,23 @@
       <c r="J4" s="13">
         <v>0</v>
       </c>
-      <c r="K4" s="19" t="s">
+      <c r="K4" s="13">
+        <v>5</v>
+      </c>
+      <c r="L4" s="22">
+        <v>0</v>
+      </c>
+      <c r="M4" s="22">
+        <v>0</v>
+      </c>
+      <c r="N4" s="22">
+        <v>0</v>
+      </c>
+      <c r="O4" s="19" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:15">
       <c r="A5" s="4" t="s">
         <v>45</v>
       </c>
@@ -1674,11 +1984,23 @@
       <c r="J5" s="13">
         <v>0</v>
       </c>
-      <c r="K5" s="19" t="s">
+      <c r="K5" s="13">
+        <v>5</v>
+      </c>
+      <c r="L5" s="22">
+        <v>0</v>
+      </c>
+      <c r="M5" s="22">
+        <v>0</v>
+      </c>
+      <c r="N5" s="22">
+        <v>0</v>
+      </c>
+      <c r="O5" s="19" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:15">
       <c r="A6" s="2" t="s">
         <v>46</v>
       </c>
@@ -1709,11 +2031,23 @@
       <c r="J6" s="13">
         <v>0</v>
       </c>
-      <c r="K6" s="19" t="s">
+      <c r="K6" s="13">
+        <v>5</v>
+      </c>
+      <c r="L6" s="22">
+        <v>0</v>
+      </c>
+      <c r="M6" s="22">
+        <v>0</v>
+      </c>
+      <c r="N6" s="22">
+        <v>0</v>
+      </c>
+      <c r="O6" s="19" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:15">
       <c r="A7" s="2" t="s">
         <v>86</v>
       </c>
@@ -1742,13 +2076,25 @@
         <v>6</v>
       </c>
       <c r="J7" s="13">
-        <v>0</v>
-      </c>
-      <c r="K7" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="K7" s="13">
+        <v>5</v>
+      </c>
+      <c r="L7" s="22">
+        <v>0</v>
+      </c>
+      <c r="M7" s="22">
+        <v>0</v>
+      </c>
+      <c r="N7" s="22">
+        <v>0</v>
+      </c>
+      <c r="O7" s="19" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:15">
       <c r="A8" s="2" t="s">
         <v>87</v>
       </c>
@@ -1779,11 +2125,23 @@
       <c r="J8" s="13">
         <v>0</v>
       </c>
-      <c r="K8" s="19" t="s">
+      <c r="K8" s="13">
+        <v>5</v>
+      </c>
+      <c r="L8" s="22">
+        <v>0</v>
+      </c>
+      <c r="M8" s="22">
+        <v>0</v>
+      </c>
+      <c r="N8" s="22">
+        <v>0</v>
+      </c>
+      <c r="O8" s="19" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:15">
       <c r="A9" s="2" t="s">
         <v>88</v>
       </c>
@@ -1814,11 +2172,23 @@
       <c r="J9" s="13">
         <v>0</v>
       </c>
-      <c r="K9" s="19" t="s">
+      <c r="K9" s="13">
+        <v>5</v>
+      </c>
+      <c r="L9" s="22">
+        <v>0</v>
+      </c>
+      <c r="M9" s="22">
+        <v>0</v>
+      </c>
+      <c r="N9" s="22">
+        <v>0</v>
+      </c>
+      <c r="O9" s="19" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:15">
       <c r="A10" s="2" t="s">
         <v>89</v>
       </c>
@@ -1849,11 +2219,23 @@
       <c r="J10" s="13">
         <v>0</v>
       </c>
-      <c r="K10" s="19" t="s">
+      <c r="K10" s="13">
+        <v>5</v>
+      </c>
+      <c r="L10" s="22">
+        <v>0</v>
+      </c>
+      <c r="M10" s="22">
+        <v>0</v>
+      </c>
+      <c r="N10" s="22">
+        <v>0</v>
+      </c>
+      <c r="O10" s="19" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:15">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
@@ -1882,13 +2264,25 @@
         <v>6</v>
       </c>
       <c r="J11" s="13">
-        <v>0</v>
-      </c>
-      <c r="K11" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="K11" s="13">
+        <v>5</v>
+      </c>
+      <c r="L11" s="22">
+        <v>0</v>
+      </c>
+      <c r="M11" s="22">
+        <v>0</v>
+      </c>
+      <c r="N11" s="22">
+        <v>0</v>
+      </c>
+      <c r="O11" s="19" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:15">
       <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
@@ -1919,11 +2313,23 @@
       <c r="J12" s="13">
         <v>0</v>
       </c>
-      <c r="K12" s="19" t="s">
+      <c r="K12" s="13">
+        <v>5</v>
+      </c>
+      <c r="L12" s="22">
+        <v>0</v>
+      </c>
+      <c r="M12" s="22">
+        <v>0</v>
+      </c>
+      <c r="N12" s="22">
+        <v>0</v>
+      </c>
+      <c r="O12" s="19" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:15">
       <c r="A13" s="2" t="s">
         <v>10</v>
       </c>
@@ -1954,11 +2360,23 @@
       <c r="J13" s="13">
         <v>0</v>
       </c>
-      <c r="K13" s="19" t="s">
+      <c r="K13" s="13">
+        <v>5</v>
+      </c>
+      <c r="L13" s="22">
+        <v>0</v>
+      </c>
+      <c r="M13" s="22">
+        <v>0</v>
+      </c>
+      <c r="N13" s="22">
+        <v>0</v>
+      </c>
+      <c r="O13" s="19" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:15">
       <c r="A14" s="2" t="s">
         <v>11</v>
       </c>
@@ -1989,11 +2407,23 @@
       <c r="J14" s="13">
         <v>0</v>
       </c>
-      <c r="K14" s="19" t="s">
+      <c r="K14" s="13">
+        <v>5</v>
+      </c>
+      <c r="L14" s="22">
+        <v>0</v>
+      </c>
+      <c r="M14" s="22">
+        <v>0</v>
+      </c>
+      <c r="N14" s="22">
+        <v>0</v>
+      </c>
+      <c r="O14" s="19" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:15">
       <c r="A15" s="4" t="s">
         <v>97</v>
       </c>
@@ -2022,13 +2452,25 @@
         <v>6</v>
       </c>
       <c r="J15" s="13">
-        <v>0</v>
-      </c>
-      <c r="K15" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="K15" s="13">
+        <v>5</v>
+      </c>
+      <c r="L15" s="22">
+        <v>0</v>
+      </c>
+      <c r="M15" s="22">
+        <v>0</v>
+      </c>
+      <c r="N15" s="22">
+        <v>0</v>
+      </c>
+      <c r="O15" s="19" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:15">
       <c r="A16" s="4" t="s">
         <v>33</v>
       </c>
@@ -2057,13 +2499,25 @@
         <v>6</v>
       </c>
       <c r="J16" s="13">
-        <v>0</v>
-      </c>
-      <c r="K16" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="K16" s="13">
+        <v>5</v>
+      </c>
+      <c r="L16" s="22">
+        <v>0</v>
+      </c>
+      <c r="M16" s="22">
+        <v>0</v>
+      </c>
+      <c r="N16" s="22">
+        <v>0</v>
+      </c>
+      <c r="O16" s="19" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:15">
       <c r="A17" s="2" t="s">
         <v>28</v>
       </c>
@@ -2094,11 +2548,23 @@
       <c r="J17" s="13">
         <v>0</v>
       </c>
-      <c r="K17" s="19" t="s">
+      <c r="K17" s="13">
+        <v>5</v>
+      </c>
+      <c r="L17" s="22">
+        <v>0</v>
+      </c>
+      <c r="M17" s="22">
+        <v>0</v>
+      </c>
+      <c r="N17" s="22">
+        <v>0</v>
+      </c>
+      <c r="O17" s="19" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:15">
       <c r="A18" s="4" t="s">
         <v>100</v>
       </c>
@@ -2129,11 +2595,23 @@
       <c r="J18" s="13">
         <v>0</v>
       </c>
-      <c r="K18" s="19" t="s">
+      <c r="K18" s="13">
+        <v>5</v>
+      </c>
+      <c r="L18" s="22">
+        <v>0</v>
+      </c>
+      <c r="M18" s="22">
+        <v>0</v>
+      </c>
+      <c r="N18" s="22">
+        <v>0</v>
+      </c>
+      <c r="O18" s="19" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:15">
       <c r="A19" s="2" t="s">
         <v>29</v>
       </c>
@@ -2164,11 +2642,23 @@
       <c r="J19" s="13">
         <v>0</v>
       </c>
-      <c r="K19" s="19" t="s">
+      <c r="K19" s="13">
+        <v>5</v>
+      </c>
+      <c r="L19" s="22">
+        <v>0</v>
+      </c>
+      <c r="M19" s="22">
+        <v>0</v>
+      </c>
+      <c r="N19" s="22">
+        <v>0</v>
+      </c>
+      <c r="O19" s="19" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:15">
       <c r="A20" s="4" t="s">
         <v>19</v>
       </c>
@@ -2197,13 +2687,25 @@
         <v>4</v>
       </c>
       <c r="J20" s="13">
-        <v>0</v>
-      </c>
-      <c r="K20" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="K20" s="13">
+        <v>5</v>
+      </c>
+      <c r="L20" s="22">
+        <v>0</v>
+      </c>
+      <c r="M20" s="22">
+        <v>0</v>
+      </c>
+      <c r="N20" s="22">
+        <v>0</v>
+      </c>
+      <c r="O20" s="19" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:15">
       <c r="A21" s="4" t="s">
         <v>13</v>
       </c>
@@ -2234,11 +2736,23 @@
       <c r="J21" s="13">
         <v>0</v>
       </c>
-      <c r="K21" s="19" t="s">
+      <c r="K21" s="13">
+        <v>5</v>
+      </c>
+      <c r="L21" s="22">
+        <v>0</v>
+      </c>
+      <c r="M21" s="22">
+        <v>0</v>
+      </c>
+      <c r="N21" s="22">
+        <v>0</v>
+      </c>
+      <c r="O21" s="19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:15">
       <c r="A22" s="2" t="s">
         <v>15</v>
       </c>
@@ -2269,11 +2783,23 @@
       <c r="J22" s="13">
         <v>0</v>
       </c>
-      <c r="K22" s="19" t="s">
+      <c r="K22" s="13">
+        <v>5</v>
+      </c>
+      <c r="L22" s="22">
+        <v>0</v>
+      </c>
+      <c r="M22" s="22">
+        <v>0</v>
+      </c>
+      <c r="N22" s="22">
+        <v>0</v>
+      </c>
+      <c r="O22" s="19" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:15">
       <c r="A23" s="4" t="s">
         <v>16</v>
       </c>
@@ -2304,11 +2830,23 @@
       <c r="J23" s="13">
         <v>0</v>
       </c>
-      <c r="K23" s="19" t="s">
+      <c r="K23" s="13">
+        <v>5</v>
+      </c>
+      <c r="L23" s="22">
+        <v>0</v>
+      </c>
+      <c r="M23" s="22">
+        <v>0</v>
+      </c>
+      <c r="N23" s="22">
+        <v>0</v>
+      </c>
+      <c r="O23" s="19" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:15">
       <c r="A24" s="4" t="s">
         <v>25</v>
       </c>
@@ -2339,296 +2877,404 @@
       <c r="J24" s="13">
         <v>0</v>
       </c>
-      <c r="K24" s="19" t="s">
+      <c r="K24" s="13">
+        <v>5</v>
+      </c>
+      <c r="L24" s="22">
+        <v>0</v>
+      </c>
+      <c r="M24" s="22">
+        <v>0</v>
+      </c>
+      <c r="N24" s="22">
+        <v>0</v>
+      </c>
+      <c r="O24" s="19" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
-      <c r="A25" s="2" t="s">
+    <row r="25" spans="1:15">
+      <c r="A25" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="B25" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="C25" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="D25" s="13">
+        <v>100</v>
+      </c>
+      <c r="E25" s="23">
+        <v>16</v>
+      </c>
+      <c r="F25" s="13">
+        <v>1</v>
+      </c>
+      <c r="G25" s="13">
+        <v>1</v>
+      </c>
+      <c r="H25" s="13">
+        <v>0</v>
+      </c>
+      <c r="I25" s="13">
+        <v>16</v>
+      </c>
+      <c r="J25" s="13">
+        <v>1</v>
+      </c>
+      <c r="K25" s="13">
+        <v>5</v>
+      </c>
+      <c r="L25" s="22">
+        <v>0</v>
+      </c>
+      <c r="M25" s="22">
+        <v>0</v>
+      </c>
+      <c r="N25" s="22">
+        <v>0</v>
+      </c>
+      <c r="O25" s="19" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15">
+      <c r="A26" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="B26" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="C26" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="D26" s="12">
+        <v>100</v>
+      </c>
+      <c r="E26">
+        <v>55</v>
+      </c>
+      <c r="F26" s="13">
+        <v>1</v>
+      </c>
+      <c r="G26" s="13">
+        <v>2</v>
+      </c>
+      <c r="H26" s="13">
+        <v>0</v>
+      </c>
+      <c r="I26" s="13">
+        <v>12</v>
+      </c>
+      <c r="J26" s="13">
+        <v>0</v>
+      </c>
+      <c r="K26" s="13">
+        <v>5</v>
+      </c>
+      <c r="L26" s="22">
+        <v>0</v>
+      </c>
+      <c r="M26" s="22">
+        <v>0</v>
+      </c>
+      <c r="N26" s="22">
+        <v>0</v>
+      </c>
+      <c r="O26" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15">
+      <c r="A27" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="B27" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="C27" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="D27" s="12">
+        <v>150</v>
+      </c>
+      <c r="E27">
+        <v>24</v>
+      </c>
+      <c r="F27" s="13">
+        <v>1</v>
+      </c>
+      <c r="G27" s="13">
+        <v>2</v>
+      </c>
+      <c r="H27" s="13">
+        <v>0</v>
+      </c>
+      <c r="I27" s="13">
+        <v>12</v>
+      </c>
+      <c r="J27" s="13">
+        <v>0</v>
+      </c>
+      <c r="K27" s="13">
+        <v>5</v>
+      </c>
+      <c r="L27" s="22">
+        <v>0</v>
+      </c>
+      <c r="M27" s="22">
+        <v>0</v>
+      </c>
+      <c r="N27" s="22">
+        <v>0</v>
+      </c>
+      <c r="O27" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15">
+      <c r="A28" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="B28" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="C28" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="D28" s="13">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>110</v>
+      </c>
+      <c r="F28" s="13">
+        <v>1</v>
+      </c>
+      <c r="G28" s="13">
+        <v>3</v>
+      </c>
+      <c r="H28" s="13">
+        <v>0</v>
+      </c>
+      <c r="I28" s="13">
+        <v>12</v>
+      </c>
+      <c r="J28" s="13">
+        <v>0</v>
+      </c>
+      <c r="K28" s="13">
+        <v>5</v>
+      </c>
+      <c r="L28" s="22">
+        <v>0</v>
+      </c>
+      <c r="M28" s="22">
+        <v>20</v>
+      </c>
+      <c r="N28" s="22">
+        <v>0</v>
+      </c>
+      <c r="O28" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15">
+      <c r="A29" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B29" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C29" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D25" s="3">
+      <c r="D29" s="3">
         <v>60</v>
       </c>
-      <c r="E25" s="15">
+      <c r="E29" s="15">
         <v>8</v>
       </c>
-      <c r="F25" s="3">
-        <v>1</v>
-      </c>
-      <c r="G25" s="3">
-        <v>1</v>
-      </c>
-      <c r="H25" s="3">
-        <v>0</v>
-      </c>
-      <c r="I25" s="3">
+      <c r="F29" s="3">
+        <v>1</v>
+      </c>
+      <c r="G29" s="3">
+        <v>1</v>
+      </c>
+      <c r="H29" s="3">
+        <v>0</v>
+      </c>
+      <c r="I29" s="3">
         <v>4</v>
       </c>
-      <c r="J25" s="13">
-        <v>0</v>
-      </c>
-      <c r="K25" s="19" t="s">
+      <c r="J29" s="13">
+        <v>1</v>
+      </c>
+      <c r="K29" s="13">
+        <v>5</v>
+      </c>
+      <c r="L29" s="22">
+        <v>0</v>
+      </c>
+      <c r="M29" s="22">
+        <v>0</v>
+      </c>
+      <c r="N29" s="22">
+        <v>0</v>
+      </c>
+      <c r="O29" s="19" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
-      <c r="A26" s="4" t="s">
+    <row r="30" spans="1:15">
+      <c r="A30" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B30" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C30" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="D26" s="5">
+      <c r="D30" s="5">
         <v>70</v>
       </c>
-      <c r="E26" s="16">
+      <c r="E30" s="16">
         <v>720</v>
       </c>
-      <c r="F26" s="5">
+      <c r="F30" s="5">
         <v>3</v>
       </c>
-      <c r="G26" s="5">
+      <c r="G30" s="5">
         <v>3</v>
       </c>
-      <c r="H26" s="5">
-        <v>0</v>
-      </c>
-      <c r="I26" s="5">
+      <c r="H30" s="5">
+        <v>0</v>
+      </c>
+      <c r="I30" s="5">
         <v>4</v>
       </c>
-      <c r="J26" s="13">
-        <v>0</v>
-      </c>
-      <c r="K26" s="19" t="s">
+      <c r="J30" s="13">
+        <v>0</v>
+      </c>
+      <c r="K30" s="13">
+        <v>5</v>
+      </c>
+      <c r="L30" s="22">
+        <v>0</v>
+      </c>
+      <c r="M30" s="22">
+        <v>0</v>
+      </c>
+      <c r="N30" s="22">
+        <v>0</v>
+      </c>
+      <c r="O30" s="19" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
-      <c r="A27" s="2" t="s">
+    <row r="31" spans="1:15">
+      <c r="A31" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B31" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C31" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D27" s="3">
+      <c r="D31" s="3">
         <v>50</v>
-      </c>
-      <c r="E27" s="15">
-        <v>720</v>
-      </c>
-      <c r="F27" s="3">
-        <v>3</v>
-      </c>
-      <c r="G27" s="3">
-        <v>1</v>
-      </c>
-      <c r="H27" s="3">
-        <v>0</v>
-      </c>
-      <c r="I27" s="3">
-        <v>72</v>
-      </c>
-      <c r="J27" s="13">
-        <v>0</v>
-      </c>
-      <c r="K27" s="19" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11">
-      <c r="A28" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="D28" s="5">
-        <v>80</v>
-      </c>
-      <c r="E28" s="16">
-        <v>100</v>
-      </c>
-      <c r="F28" s="5">
-        <v>5</v>
-      </c>
-      <c r="G28" s="5">
-        <v>2</v>
-      </c>
-      <c r="H28" s="5">
-        <v>0</v>
-      </c>
-      <c r="I28" s="5">
-        <v>12</v>
-      </c>
-      <c r="J28" s="13">
-        <v>0</v>
-      </c>
-      <c r="K28" s="19" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11">
-      <c r="A29" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="D29" s="3">
-        <v>0</v>
-      </c>
-      <c r="E29" s="15">
-        <v>0</v>
-      </c>
-      <c r="F29" s="3">
-        <v>0</v>
-      </c>
-      <c r="G29" s="3">
-        <v>0</v>
-      </c>
-      <c r="H29" s="3">
-        <v>0</v>
-      </c>
-      <c r="I29" s="3">
-        <v>0</v>
-      </c>
-      <c r="J29" s="13">
-        <v>0</v>
-      </c>
-      <c r="K29" s="19" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11">
-      <c r="A30" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="D30" s="5">
-        <v>0</v>
-      </c>
-      <c r="E30" s="16">
-        <v>0</v>
-      </c>
-      <c r="F30" s="5">
-        <v>0</v>
-      </c>
-      <c r="G30" s="5">
-        <v>0</v>
-      </c>
-      <c r="H30" s="5">
-        <v>0</v>
-      </c>
-      <c r="I30" s="5">
-        <v>0</v>
-      </c>
-      <c r="J30" s="13">
-        <v>0</v>
-      </c>
-      <c r="K30" s="19" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11">
-      <c r="A31" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D31" s="3">
-        <v>0</v>
       </c>
       <c r="E31" s="15">
         <v>720</v>
       </c>
       <c r="F31" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G31" s="3">
         <v>1</v>
       </c>
       <c r="H31" s="3">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="I31" s="3">
+        <v>72</v>
+      </c>
+      <c r="J31" s="13">
+        <v>0</v>
+      </c>
+      <c r="K31" s="13">
+        <v>5</v>
+      </c>
+      <c r="L31" s="22">
+        <v>0</v>
+      </c>
+      <c r="M31" s="22">
+        <v>0</v>
+      </c>
+      <c r="N31" s="22">
+        <v>0</v>
+      </c>
+      <c r="O31" s="19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15">
+      <c r="A32" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D32" s="5">
+        <v>80</v>
+      </c>
+      <c r="E32" s="16">
+        <v>100</v>
+      </c>
+      <c r="F32" s="5">
+        <v>5</v>
+      </c>
+      <c r="G32" s="5">
+        <v>2</v>
+      </c>
+      <c r="H32" s="5">
+        <v>0</v>
+      </c>
+      <c r="I32" s="5">
         <v>12</v>
       </c>
-      <c r="J31" s="13">
-        <v>0</v>
-      </c>
-      <c r="K31" s="19" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11">
-      <c r="A32" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="D32" s="5">
-        <v>0</v>
-      </c>
-      <c r="E32" s="16">
-        <v>0</v>
-      </c>
-      <c r="F32" s="5">
-        <v>0</v>
-      </c>
-      <c r="G32" s="5">
-        <v>0</v>
-      </c>
-      <c r="H32" s="5">
+      <c r="J32" s="13">
+        <v>0</v>
+      </c>
+      <c r="K32" s="13">
         <v>5</v>
       </c>
-      <c r="I32" s="5">
-        <v>0</v>
-      </c>
-      <c r="J32" s="13">
-        <v>0</v>
-      </c>
-      <c r="K32" s="19" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11">
+      <c r="L32" s="22">
+        <v>0</v>
+      </c>
+      <c r="M32" s="22">
+        <v>0</v>
+      </c>
+      <c r="N32" s="22">
+        <v>0</v>
+      </c>
+      <c r="O32" s="19" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15">
       <c r="A33" s="2" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>82</v>
@@ -2646,24 +3292,36 @@
         <v>0</v>
       </c>
       <c r="H33" s="3">
+        <v>0</v>
+      </c>
+      <c r="I33" s="3">
+        <v>0</v>
+      </c>
+      <c r="J33" s="13">
+        <v>0</v>
+      </c>
+      <c r="K33" s="13">
         <v>5</v>
       </c>
-      <c r="I33" s="3">
-        <v>0</v>
-      </c>
-      <c r="J33" s="13">
-        <v>0</v>
-      </c>
-      <c r="K33" s="19" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11">
+      <c r="L33" s="22">
+        <v>0</v>
+      </c>
+      <c r="M33" s="22">
+        <v>0</v>
+      </c>
+      <c r="N33" s="22">
+        <v>0</v>
+      </c>
+      <c r="O33" s="19" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15">
       <c r="A34" s="4" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>82</v>
@@ -2681,155 +3339,450 @@
         <v>0</v>
       </c>
       <c r="H34" s="5">
+        <v>0</v>
+      </c>
+      <c r="I34" s="5">
+        <v>0</v>
+      </c>
+      <c r="J34" s="13">
+        <v>0</v>
+      </c>
+      <c r="K34" s="13">
+        <v>5</v>
+      </c>
+      <c r="L34" s="22">
+        <v>0</v>
+      </c>
+      <c r="M34" s="22">
+        <v>0</v>
+      </c>
+      <c r="N34" s="22">
+        <v>0</v>
+      </c>
+      <c r="O34" s="19" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15">
+      <c r="A35" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D35" s="3">
+        <v>30</v>
+      </c>
+      <c r="E35" s="15">
+        <v>16</v>
+      </c>
+      <c r="F35" s="3">
+        <v>1</v>
+      </c>
+      <c r="G35" s="3">
+        <v>1</v>
+      </c>
+      <c r="H35" s="3">
+        <v>0</v>
+      </c>
+      <c r="I35" s="3">
+        <v>4</v>
+      </c>
+      <c r="J35" s="13">
+        <v>1</v>
+      </c>
+      <c r="K35" s="13">
+        <v>5</v>
+      </c>
+      <c r="L35" s="22">
+        <v>0</v>
+      </c>
+      <c r="M35" s="22">
+        <v>0</v>
+      </c>
+      <c r="N35" s="22">
+        <v>0</v>
+      </c>
+      <c r="O35" s="19" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15">
+      <c r="A36" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D36" s="3">
+        <v>0</v>
+      </c>
+      <c r="E36" s="15">
+        <v>720</v>
+      </c>
+      <c r="F36" s="3">
+        <v>1</v>
+      </c>
+      <c r="G36" s="3">
+        <v>1</v>
+      </c>
+      <c r="H36" s="3">
+        <v>20</v>
+      </c>
+      <c r="I36" s="3">
+        <v>12</v>
+      </c>
+      <c r="J36" s="13">
+        <v>1</v>
+      </c>
+      <c r="K36" s="13">
+        <v>1</v>
+      </c>
+      <c r="L36" s="22">
+        <v>0</v>
+      </c>
+      <c r="M36" s="22">
+        <v>0</v>
+      </c>
+      <c r="N36" s="22">
+        <v>0</v>
+      </c>
+      <c r="O36" s="19" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15">
+      <c r="A37" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D37" s="5">
+        <v>0</v>
+      </c>
+      <c r="E37" s="16">
+        <v>0</v>
+      </c>
+      <c r="F37" s="5">
+        <v>0</v>
+      </c>
+      <c r="G37" s="5">
+        <v>0</v>
+      </c>
+      <c r="H37" s="5">
+        <v>5</v>
+      </c>
+      <c r="I37" s="5">
+        <v>0</v>
+      </c>
+      <c r="J37" s="13">
+        <v>1</v>
+      </c>
+      <c r="K37" s="13">
+        <v>1</v>
+      </c>
+      <c r="L37" s="22">
+        <v>0</v>
+      </c>
+      <c r="M37" s="22">
+        <v>0</v>
+      </c>
+      <c r="N37" s="22">
+        <v>0</v>
+      </c>
+      <c r="O37" s="19" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15">
+      <c r="A38" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D38" s="3">
+        <v>0</v>
+      </c>
+      <c r="E38" s="15">
+        <v>0</v>
+      </c>
+      <c r="F38" s="3">
+        <v>0</v>
+      </c>
+      <c r="G38" s="3">
+        <v>0</v>
+      </c>
+      <c r="H38" s="3">
+        <v>5</v>
+      </c>
+      <c r="I38" s="3">
+        <v>0</v>
+      </c>
+      <c r="J38" s="13">
+        <v>1</v>
+      </c>
+      <c r="K38" s="13">
+        <v>1</v>
+      </c>
+      <c r="L38" s="22">
+        <v>0</v>
+      </c>
+      <c r="M38" s="22">
+        <v>0</v>
+      </c>
+      <c r="N38" s="22">
+        <v>0</v>
+      </c>
+      <c r="O38" s="19" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15">
+      <c r="A39" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D39" s="5">
+        <v>0</v>
+      </c>
+      <c r="E39" s="16">
+        <v>0</v>
+      </c>
+      <c r="F39" s="5">
+        <v>0</v>
+      </c>
+      <c r="G39" s="5">
+        <v>0</v>
+      </c>
+      <c r="H39" s="5">
         <v>15</v>
       </c>
-      <c r="I34" s="5">
-        <v>0</v>
-      </c>
-      <c r="J34" s="13">
-        <v>0</v>
-      </c>
-      <c r="K34" s="19" t="s">
+      <c r="I39" s="5">
+        <v>0</v>
+      </c>
+      <c r="J39" s="13">
+        <v>1</v>
+      </c>
+      <c r="K39" s="13">
+        <v>1</v>
+      </c>
+      <c r="L39" s="22">
+        <v>0</v>
+      </c>
+      <c r="M39" s="22">
+        <v>0</v>
+      </c>
+      <c r="N39" s="22">
+        <v>0</v>
+      </c>
+      <c r="O39" s="19" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="1:11">
-      <c r="A35" s="2" t="s">
+    <row r="40" spans="1:15">
+      <c r="A40" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B40" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C40" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D35" s="3">
-        <v>0</v>
-      </c>
-      <c r="E35" s="15">
-        <v>0</v>
-      </c>
-      <c r="F35" s="3">
-        <v>0</v>
-      </c>
-      <c r="G35" s="3">
-        <v>0</v>
-      </c>
-      <c r="H35" s="3">
+      <c r="D40" s="3">
+        <v>0</v>
+      </c>
+      <c r="E40" s="15">
+        <v>0</v>
+      </c>
+      <c r="F40" s="3">
+        <v>0</v>
+      </c>
+      <c r="G40" s="3">
+        <v>0</v>
+      </c>
+      <c r="H40" s="3">
         <v>30</v>
       </c>
-      <c r="I35" s="3">
-        <v>0</v>
-      </c>
-      <c r="J35" s="13">
-        <v>0</v>
-      </c>
-      <c r="K35" s="19" t="s">
+      <c r="I40" s="3">
+        <v>0</v>
+      </c>
+      <c r="J40" s="13">
+        <v>1</v>
+      </c>
+      <c r="K40" s="13">
+        <v>1</v>
+      </c>
+      <c r="L40" s="22">
+        <v>0</v>
+      </c>
+      <c r="M40" s="22">
+        <v>0</v>
+      </c>
+      <c r="N40" s="22">
+        <v>0</v>
+      </c>
+      <c r="O40" s="19" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="36" spans="1:11">
-      <c r="A36" s="4" t="s">
+    <row r="41" spans="1:15">
+      <c r="A41" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B41" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="C41" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="D36" s="5">
-        <v>0</v>
-      </c>
-      <c r="E36" s="16">
-        <v>0</v>
-      </c>
-      <c r="F36" s="5">
-        <v>0</v>
-      </c>
-      <c r="G36" s="5">
-        <v>0</v>
-      </c>
-      <c r="H36" s="5">
+      <c r="D41" s="5">
+        <v>0</v>
+      </c>
+      <c r="E41" s="16">
+        <v>0</v>
+      </c>
+      <c r="F41" s="5">
+        <v>0</v>
+      </c>
+      <c r="G41" s="5">
+        <v>0</v>
+      </c>
+      <c r="H41" s="5">
         <v>60</v>
       </c>
-      <c r="I36" s="5">
-        <v>0</v>
-      </c>
-      <c r="J36" s="13">
-        <v>0</v>
-      </c>
-      <c r="K36" s="19" t="s">
+      <c r="I41" s="5">
+        <v>0</v>
+      </c>
+      <c r="J41" s="13">
+        <v>1</v>
+      </c>
+      <c r="K41" s="13">
+        <v>1</v>
+      </c>
+      <c r="L41" s="22">
+        <v>0</v>
+      </c>
+      <c r="M41" s="22">
+        <v>0</v>
+      </c>
+      <c r="N41" s="22">
+        <v>0</v>
+      </c>
+      <c r="O41" s="19" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="37" spans="1:11">
-      <c r="A37" s="2" t="s">
+    <row r="42" spans="1:15">
+      <c r="A42" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B42" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C42" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D37" s="3">
+      <c r="D42" s="3">
         <v>400</v>
       </c>
-      <c r="E37" s="15">
+      <c r="E42" s="15">
         <v>48</v>
       </c>
-      <c r="F37" s="3">
-        <v>1</v>
-      </c>
-      <c r="G37" s="3">
+      <c r="F42" s="3">
+        <v>1</v>
+      </c>
+      <c r="G42" s="3">
         <v>2</v>
       </c>
-      <c r="H37" s="3">
-        <v>0</v>
-      </c>
-      <c r="I37" s="3">
+      <c r="H42" s="3">
+        <v>0</v>
+      </c>
+      <c r="I42" s="3">
         <v>12</v>
       </c>
-      <c r="J37" s="13">
-        <v>0</v>
-      </c>
-      <c r="K37" s="19" t="s">
+      <c r="J42" s="13">
+        <v>1</v>
+      </c>
+      <c r="K42" s="13">
+        <v>1</v>
+      </c>
+      <c r="L42" s="22">
+        <v>0</v>
+      </c>
+      <c r="M42" s="22">
+        <v>0</v>
+      </c>
+      <c r="N42" s="22">
+        <v>0</v>
+      </c>
+      <c r="O42" s="19" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="38" spans="1:11">
-      <c r="A38" s="6" t="s">
+    <row r="43" spans="1:15">
+      <c r="A43" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B38" s="6" t="s">
+      <c r="B43" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="C43" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="D38" s="7">
+      <c r="D43" s="7">
         <v>400</v>
       </c>
-      <c r="E38" s="17">
+      <c r="E43" s="17">
         <v>48</v>
       </c>
-      <c r="F38" s="7">
-        <v>1</v>
-      </c>
-      <c r="G38" s="7">
+      <c r="F43" s="7">
+        <v>1</v>
+      </c>
+      <c r="G43" s="7">
         <v>2</v>
       </c>
-      <c r="H38" s="7">
-        <v>0</v>
-      </c>
-      <c r="I38" s="7">
+      <c r="H43" s="7">
+        <v>0</v>
+      </c>
+      <c r="I43" s="7">
         <v>12</v>
       </c>
-      <c r="J38" s="12">
-        <v>0</v>
-      </c>
-      <c r="K38" s="20" t="s">
+      <c r="J43" s="12">
+        <v>1</v>
+      </c>
+      <c r="K43" s="12">
+        <v>1</v>
+      </c>
+      <c r="L43" s="24">
+        <v>0</v>
+      </c>
+      <c r="M43" s="22">
+        <v>0</v>
+      </c>
+      <c r="N43" s="22">
+        <v>0</v>
+      </c>
+      <c r="O43" s="20" t="s">
         <v>55</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Menu probably done now. New ability for C. Kata.
</commit_message>
<xml_diff>
--- a/xml/Abilities.xlsx
+++ b/xml/Abilities.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="147">
   <si>
     <t>Name</t>
   </si>
@@ -451,13 +451,19 @@
   </si>
   <si>
     <t>Self</t>
+  </si>
+  <si>
+    <t>Death Shout</t>
+  </si>
+  <si>
+    <t>Stuns all enemies within the shout's range for a second. gogoloudwhitegirl</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -471,6 +477,12 @@
       <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -589,7 +601,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -619,71 +631,18 @@
     <xf numFmtId="49" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="43">
-    <dxf>
-      <border outline="0">
-        <bottom style="thick">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2079,6 +2038,66 @@
         <vertical/>
         <horizontal/>
       </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thick">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -2438,124 +2457,124 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:AM43" tableType="xml" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2" headerRowBorderDxfId="0" tableBorderDxfId="1">
-  <autoFilter ref="A2:AM43"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:AM44" tableType="xml" totalsRowShown="0" headerRowDxfId="42" dataDxfId="40" headerRowBorderDxfId="41" tableBorderDxfId="39">
+  <autoFilter ref="A2:AM44"/>
   <tableColumns count="39">
-    <tableColumn id="1" uniqueName="Name" name="Name" dataDxfId="42">
+    <tableColumn id="1" uniqueName="Name" name="Name" dataDxfId="38">
       <xmlColumnPr mapId="12" xpath="/Abilities/Ability/Name" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="Availability" name="Availability" dataDxfId="41">
+    <tableColumn id="2" uniqueName="Availability" name="Availability" dataDxfId="37">
       <xmlColumnPr mapId="12" xpath="/Abilities/Ability/Availability" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="Spec" name="Spec" dataDxfId="40">
+    <tableColumn id="3" uniqueName="Spec" name="Spec" dataDxfId="36">
       <xmlColumnPr mapId="12" xpath="/Abilities/Ability/Spec" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="4" uniqueName="Range" name="Range" dataDxfId="39">
+    <tableColumn id="4" uniqueName="Range" name="Range" dataDxfId="35">
       <xmlColumnPr mapId="12" xpath="/Abilities/Ability/Range" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="5" uniqueName="Cooldown" name="Cooldown" dataDxfId="38">
+    <tableColumn id="5" uniqueName="Cooldown" name="Cooldown" dataDxfId="34">
       <xmlColumnPr mapId="12" xpath="/Abilities/Ability/Cooldown" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="Uses" name="Uses" dataDxfId="37">
+    <tableColumn id="6" uniqueName="Uses" name="Uses" dataDxfId="33">
       <xmlColumnPr mapId="12" xpath="/Abilities/Ability/Uses" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="Activate" name="Activate" dataDxfId="36">
+    <tableColumn id="7" uniqueName="Activate" name="Activate" dataDxfId="32">
       <xmlColumnPr mapId="12" xpath="/Abilities/Ability/Activate" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="8" uniqueName="Value" name="Value" dataDxfId="35">
+    <tableColumn id="8" uniqueName="Value" name="Value" dataDxfId="31">
       <xmlColumnPr mapId="12" xpath="/Abilities/Ability/Value" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="9" uniqueName="Delay" name="Delay" dataDxfId="34">
+    <tableColumn id="9" uniqueName="Delay" name="Delay" dataDxfId="30">
       <xmlColumnPr mapId="12" xpath="/Abilities/Ability/Delay" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="10" uniqueName="Min" name="Min" dataDxfId="33">
+    <tableColumn id="10" uniqueName="Min" name="Min" dataDxfId="29">
       <xmlColumnPr mapId="12" xpath="/Abilities/Ability/Min" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="11" uniqueName="Max" name="Max" dataDxfId="32">
+    <tableColumn id="11" uniqueName="Max" name="Max" dataDxfId="28">
       <xmlColumnPr mapId="12" xpath="/Abilities/Ability/Max" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="12" uniqueName="Damage" name="Damage" dataDxfId="31">
+    <tableColumn id="12" uniqueName="Damage" name="Damage" dataDxfId="27">
       <xmlColumnPr mapId="12" xpath="/Abilities/Ability/Damage" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="13" uniqueName="Speed" name="Speed" dataDxfId="30">
+    <tableColumn id="13" uniqueName="Speed" name="Speed" dataDxfId="26">
       <xmlColumnPr mapId="12" xpath="/Abilities/Ability/Speed" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="14" uniqueName="StunDur" name="StunDur" dataDxfId="29">
+    <tableColumn id="14" uniqueName="StunDur" name="StunDur" dataDxfId="25">
       <xmlColumnPr mapId="12" xpath="/Abilities/Ability/StunDur" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="15" uniqueName="SlowDur" name="SlowDur" dataDxfId="28">
+    <tableColumn id="15" uniqueName="SlowDur" name="SlowDur" dataDxfId="24">
       <xmlColumnPr mapId="12" xpath="/Abilities/Ability/SlowDur" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="16" uniqueName="SickDur" name="SickDur" dataDxfId="27">
+    <tableColumn id="16" uniqueName="SickDur" name="SickDur" dataDxfId="23">
       <xmlColumnPr mapId="12" xpath="/Abilities/Ability/SickDur" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="17" uniqueName="ExhaustDur" name="ExhaustDur" dataDxfId="26">
+    <tableColumn id="17" uniqueName="ExhaustDur" name="ExhaustDur" dataDxfId="22">
       <xmlColumnPr mapId="12" xpath="/Abilities/Ability/ExhaustDur" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="18" uniqueName="RegenDur" name="RegenDur" dataDxfId="25">
+    <tableColumn id="18" uniqueName="RegenDur" name="RegenDur" dataDxfId="21">
       <xmlColumnPr mapId="12" xpath="/Abilities/Ability/RegenDur" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="19" uniqueName="SlowPerc" name="SlowPerc" dataDxfId="24">
+    <tableColumn id="19" uniqueName="SlowPerc" name="SlowPerc" dataDxfId="20">
       <xmlColumnPr mapId="12" xpath="/Abilities/Ability/SlowPerc" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="20" uniqueName="SickPerc" name="SickPerc" dataDxfId="23">
+    <tableColumn id="20" uniqueName="SickPerc" name="SickPerc" dataDxfId="19">
       <xmlColumnPr mapId="12" xpath="/Abilities/Ability/SickPerc" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="21" uniqueName="RegenPerc" name="RegenPerc" dataDxfId="22">
+    <tableColumn id="21" uniqueName="RegenPerc" name="RegenPerc" dataDxfId="18">
       <xmlColumnPr mapId="12" xpath="/Abilities/Ability/RegenPerc" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="22" uniqueName="HPPerc" name="HPPerc" dataDxfId="21">
+    <tableColumn id="22" uniqueName="HPPerc" name="HPPerc" dataDxfId="17">
       <xmlColumnPr mapId="12" xpath="/Abilities/Ability/HPPerc" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="23" uniqueName="HPLump" name="HPLump" dataDxfId="20">
+    <tableColumn id="23" uniqueName="HPLump" name="HPLump" dataDxfId="16">
       <xmlColumnPr mapId="12" xpath="/Abilities/Ability/HPLump" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="24" uniqueName="APPerc" name="APPerc" dataDxfId="19">
+    <tableColumn id="24" uniqueName="APPerc" name="APPerc" dataDxfId="15">
       <xmlColumnPr mapId="12" xpath="/Abilities/Ability/APPerc" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="25" uniqueName="APLump" name="APLump" dataDxfId="18">
+    <tableColumn id="25" uniqueName="APLump" name="APLump" dataDxfId="14">
       <xmlColumnPr mapId="12" xpath="/Abilities/Ability/APLump" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="26" uniqueName="DPLump" name="DPLump" dataDxfId="17">
+    <tableColumn id="26" uniqueName="DPLump" name="DPLump" dataDxfId="13">
       <xmlColumnPr mapId="12" xpath="/Abilities/Ability/DPLump" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="27" uniqueName="SPPerc" name="SPPerc" dataDxfId="16">
+    <tableColumn id="27" uniqueName="SPPerc" name="SPPerc" dataDxfId="12">
       <xmlColumnPr mapId="12" xpath="/Abilities/Ability/SPPerc" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="28" uniqueName="SPLump" name="SPLump" dataDxfId="15">
+    <tableColumn id="28" uniqueName="SPLump" name="SPLump" dataDxfId="11">
       <xmlColumnPr mapId="12" xpath="/Abilities/Ability/SPLump" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="29" uniqueName="CDPerc" name="CDPerc" dataDxfId="14">
+    <tableColumn id="29" uniqueName="CDPerc" name="CDPerc" dataDxfId="10">
       <xmlColumnPr mapId="12" xpath="/Abilities/Ability/CDPerc" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="30" uniqueName="CDLump" name="CDLump" dataDxfId="13">
+    <tableColumn id="30" uniqueName="CDLump" name="CDLump" dataDxfId="9">
       <xmlColumnPr mapId="12" xpath="/Abilities/Ability/CDLump" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="31" uniqueName="Move" name="Move" dataDxfId="12">
+    <tableColumn id="31" uniqueName="Move" name="Move" dataDxfId="8">
       <xmlColumnPr mapId="12" xpath="/Abilities/Ability/Move" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="32" uniqueName="Tank" name="Tank" dataDxfId="11">
+    <tableColumn id="32" uniqueName="Tank" name="Tank" dataDxfId="7">
       <xmlColumnPr mapId="12" xpath="/Abilities/Ability/Tank" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="33" uniqueName="Sprite" name="Sprite" dataDxfId="10">
+    <tableColumn id="33" uniqueName="Sprite" name="Sprite" dataDxfId="6">
       <xmlColumnPr mapId="12" xpath="/Abilities/Ability/Sprite" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="34" uniqueName="HitAnimation" name="HitAnimation" dataDxfId="9">
+    <tableColumn id="34" uniqueName="HitAnimation" name="HitAnimation" dataDxfId="5">
       <xmlColumnPr mapId="12" xpath="/Abilities/Ability/HitAnimation" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="35" uniqueName="Bullet" name="Bullet" dataDxfId="8">
+    <tableColumn id="35" uniqueName="Bullet" name="Bullet" dataDxfId="4">
       <xmlColumnPr mapId="12" xpath="/Abilities/Ability/Bullet" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="36" uniqueName="BulletMovement" name="BulletMovement" dataDxfId="7">
+    <tableColumn id="36" uniqueName="BulletMovement" name="BulletMovement" dataDxfId="3">
       <xmlColumnPr mapId="12" xpath="/Abilities/Ability/BulletMovement" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="37" uniqueName="BulletRange" name="BulletRange" dataDxfId="6">
+    <tableColumn id="37" uniqueName="BulletRange" name="BulletRange" dataDxfId="2">
       <xmlColumnPr mapId="12" xpath="/Abilities/Ability/BulletRange" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="38" uniqueName="Target" name="Target" dataDxfId="5">
+    <tableColumn id="38" uniqueName="Target" name="Target" dataDxfId="1">
       <xmlColumnPr mapId="12" xpath="/Abilities/Ability/Target" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="39" uniqueName="Description" name="Description" dataDxfId="4">
+    <tableColumn id="39" uniqueName="Description" name="Description" dataDxfId="0">
       <xmlColumnPr mapId="12" xpath="/Abilities/Ability/Description" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -2848,11 +2867,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AM43"/>
+  <dimension ref="A1:AM44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="W1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AE44" sqref="AE44"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="AG1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AM14" sqref="AM14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4192,142 +4211,144 @@
       </c>
     </row>
     <row r="14" spans="1:39">
-      <c r="A14" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="B14" s="2" t="s">
+      <c r="A14" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="B14" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="D14" s="3">
-        <v>0</v>
-      </c>
-      <c r="E14" s="10">
-        <v>0</v>
-      </c>
-      <c r="F14" s="3">
-        <v>8</v>
-      </c>
-      <c r="G14" s="3">
-        <v>1</v>
-      </c>
-      <c r="H14" s="3">
-        <v>0</v>
-      </c>
-      <c r="I14" s="3">
+      <c r="C14" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="D14" s="24">
+        <v>200</v>
+      </c>
+      <c r="E14" s="25">
+        <v>120</v>
+      </c>
+      <c r="F14" s="24">
+        <v>1</v>
+      </c>
+      <c r="G14" s="24">
+        <v>1</v>
+      </c>
+      <c r="H14" s="24">
+        <v>0</v>
+      </c>
+      <c r="I14" s="24">
         <v>24</v>
       </c>
-      <c r="J14" s="5">
-        <v>0</v>
-      </c>
-      <c r="K14" s="5">
+      <c r="J14" s="24">
+        <v>0</v>
+      </c>
+      <c r="K14" s="24">
         <v>5</v>
       </c>
-      <c r="L14" s="17">
-        <v>0</v>
-      </c>
-      <c r="M14" s="17">
-        <v>0</v>
-      </c>
-      <c r="N14" s="17">
-        <v>0</v>
-      </c>
-      <c r="O14" s="17">
-        <v>0</v>
-      </c>
-      <c r="P14" s="17">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="17">
-        <v>0</v>
-      </c>
-      <c r="R14" s="17">
-        <v>0</v>
-      </c>
-      <c r="S14" s="17">
-        <v>0</v>
-      </c>
-      <c r="T14" s="17">
-        <v>0</v>
-      </c>
-      <c r="U14" s="17">
-        <v>0</v>
-      </c>
-      <c r="V14" s="17">
-        <v>0</v>
-      </c>
-      <c r="W14" s="17">
-        <v>0</v>
-      </c>
-      <c r="X14" s="17">
-        <v>0</v>
-      </c>
-      <c r="Y14" s="17">
-        <v>0</v>
-      </c>
-      <c r="Z14" s="17">
-        <v>0</v>
-      </c>
-      <c r="AA14" s="17">
-        <v>0</v>
-      </c>
-      <c r="AB14" s="17">
-        <v>0</v>
-      </c>
-      <c r="AC14" s="17">
-        <v>0</v>
-      </c>
-      <c r="AD14" s="17">
-        <v>0</v>
-      </c>
-      <c r="AE14" s="17">
-        <v>1</v>
-      </c>
-      <c r="AF14" s="4"/>
-      <c r="AG14" s="4"/>
-      <c r="AH14" s="4"/>
-      <c r="AI14" s="4"/>
-      <c r="AJ14" s="4"/>
-      <c r="AK14" s="4"/>
-      <c r="AL14" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="AM14" s="20" t="s">
-        <v>124</v>
+      <c r="L14" s="26">
+        <v>0</v>
+      </c>
+      <c r="M14" s="26">
+        <v>0</v>
+      </c>
+      <c r="N14" s="26">
+        <v>0</v>
+      </c>
+      <c r="O14" s="26">
+        <v>0</v>
+      </c>
+      <c r="P14" s="26">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="26">
+        <v>0</v>
+      </c>
+      <c r="R14" s="26">
+        <v>0</v>
+      </c>
+      <c r="S14" s="26">
+        <v>0</v>
+      </c>
+      <c r="T14" s="26">
+        <v>0</v>
+      </c>
+      <c r="U14" s="26">
+        <v>0</v>
+      </c>
+      <c r="V14" s="26">
+        <v>0</v>
+      </c>
+      <c r="W14" s="26">
+        <v>0</v>
+      </c>
+      <c r="X14" s="26">
+        <v>0</v>
+      </c>
+      <c r="Y14" s="26">
+        <v>0</v>
+      </c>
+      <c r="Z14" s="26">
+        <v>0</v>
+      </c>
+      <c r="AA14" s="26">
+        <v>0</v>
+      </c>
+      <c r="AB14" s="26">
+        <v>0</v>
+      </c>
+      <c r="AC14" s="26">
+        <v>0</v>
+      </c>
+      <c r="AD14" s="26">
+        <v>0</v>
+      </c>
+      <c r="AE14" s="26">
+        <v>0</v>
+      </c>
+      <c r="AF14" s="26">
+        <v>1</v>
+      </c>
+      <c r="AG14" s="26"/>
+      <c r="AH14" s="26"/>
+      <c r="AI14" s="26"/>
+      <c r="AJ14" s="26"/>
+      <c r="AK14" s="26"/>
+      <c r="AL14" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="AM14" s="27" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="15" spans="1:39">
-      <c r="A15" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="D15" s="5">
-        <v>400</v>
-      </c>
-      <c r="E15" s="11">
-        <v>12</v>
-      </c>
-      <c r="F15" s="5">
-        <v>1</v>
-      </c>
-      <c r="G15" s="5">
-        <v>1</v>
-      </c>
-      <c r="H15" s="5">
-        <v>0</v>
-      </c>
-      <c r="I15" s="5">
-        <v>6</v>
+      <c r="A15" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0</v>
+      </c>
+      <c r="E15" s="10">
+        <v>0</v>
+      </c>
+      <c r="F15" s="3">
+        <v>8</v>
+      </c>
+      <c r="G15" s="3">
+        <v>1</v>
+      </c>
+      <c r="H15" s="3">
+        <v>0</v>
+      </c>
+      <c r="I15" s="3">
+        <v>24</v>
       </c>
       <c r="J15" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K15" s="5">
         <v>5</v>
@@ -4399,24 +4420,24 @@
       <c r="AJ15" s="4"/>
       <c r="AK15" s="4"/>
       <c r="AL15" s="4" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="AM15" s="20" t="s">
-        <v>97</v>
+        <v>124</v>
       </c>
     </row>
     <row r="16" spans="1:39">
       <c r="A16" s="4" t="s">
-        <v>32</v>
+        <v>95</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>29</v>
+        <v>96</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>76</v>
       </c>
       <c r="D16" s="5">
-        <v>80</v>
+        <v>400</v>
       </c>
       <c r="E16" s="11">
         <v>12</v>
@@ -4509,39 +4530,39 @@
         <v>142</v>
       </c>
       <c r="AM16" s="20" t="s">
-        <v>33</v>
+        <v>97</v>
       </c>
     </row>
     <row r="17" spans="1:39">
-      <c r="A17" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B17" s="2" t="s">
+      <c r="A17" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="D17" s="3">
-        <v>50</v>
-      </c>
-      <c r="E17" s="10">
-        <v>60</v>
-      </c>
-      <c r="F17" s="3">
-        <v>3</v>
-      </c>
-      <c r="G17" s="3">
-        <v>1</v>
-      </c>
-      <c r="H17" s="3">
-        <v>0</v>
-      </c>
-      <c r="I17" s="3">
-        <v>24</v>
+      <c r="D17" s="5">
+        <v>80</v>
+      </c>
+      <c r="E17" s="11">
+        <v>12</v>
+      </c>
+      <c r="F17" s="5">
+        <v>1</v>
+      </c>
+      <c r="G17" s="5">
+        <v>1</v>
+      </c>
+      <c r="H17" s="5">
+        <v>0</v>
+      </c>
+      <c r="I17" s="5">
+        <v>6</v>
       </c>
       <c r="J17" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K17" s="5">
         <v>5</v>
@@ -4616,35 +4637,35 @@
         <v>142</v>
       </c>
       <c r="AM17" s="20" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:39">
-      <c r="A18" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="B18" s="4" t="s">
+      <c r="A18" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D18" s="5">
-        <v>100</v>
-      </c>
-      <c r="E18" s="11">
-        <v>70</v>
-      </c>
-      <c r="F18" s="5">
-        <v>1</v>
-      </c>
-      <c r="G18" s="5">
-        <v>2</v>
-      </c>
-      <c r="H18" s="5">
-        <v>0</v>
-      </c>
-      <c r="I18" s="5">
+      <c r="D18" s="3">
+        <v>50</v>
+      </c>
+      <c r="E18" s="10">
+        <v>60</v>
+      </c>
+      <c r="F18" s="3">
+        <v>3</v>
+      </c>
+      <c r="G18" s="3">
+        <v>1</v>
+      </c>
+      <c r="H18" s="3">
+        <v>0</v>
+      </c>
+      <c r="I18" s="3">
         <v>24</v>
       </c>
       <c r="J18" s="5">
@@ -4723,35 +4744,35 @@
         <v>142</v>
       </c>
       <c r="AM18" s="20" t="s">
-        <v>99</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:39">
-      <c r="A19" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B19" s="2" t="s">
+      <c r="A19" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B19" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D19" s="5">
         <v>100</v>
       </c>
-      <c r="E19" s="10">
-        <v>80</v>
-      </c>
-      <c r="F19" s="3">
-        <v>1</v>
-      </c>
-      <c r="G19" s="3">
-        <v>1</v>
-      </c>
-      <c r="H19" s="3">
-        <v>0</v>
-      </c>
-      <c r="I19" s="3">
+      <c r="E19" s="11">
+        <v>70</v>
+      </c>
+      <c r="F19" s="5">
+        <v>1</v>
+      </c>
+      <c r="G19" s="5">
+        <v>2</v>
+      </c>
+      <c r="H19" s="5">
+        <v>0</v>
+      </c>
+      <c r="I19" s="5">
         <v>24</v>
       </c>
       <c r="J19" s="5">
@@ -4830,39 +4851,39 @@
         <v>142</v>
       </c>
       <c r="AM19" s="20" t="s">
-        <v>31</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20" spans="1:39">
-      <c r="A20" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C20" s="4" t="s">
+      <c r="A20" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D20" s="5">
-        <v>300</v>
-      </c>
-      <c r="E20" s="11">
-        <v>12</v>
-      </c>
-      <c r="F20" s="5">
-        <v>1</v>
-      </c>
-      <c r="G20" s="5">
-        <v>1</v>
-      </c>
-      <c r="H20" s="5">
-        <v>0</v>
-      </c>
-      <c r="I20" s="5">
-        <v>4</v>
+      <c r="D20" s="3">
+        <v>100</v>
+      </c>
+      <c r="E20" s="10">
+        <v>80</v>
+      </c>
+      <c r="F20" s="3">
+        <v>1</v>
+      </c>
+      <c r="G20" s="3">
+        <v>1</v>
+      </c>
+      <c r="H20" s="3">
+        <v>0</v>
+      </c>
+      <c r="I20" s="3">
+        <v>24</v>
       </c>
       <c r="J20" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K20" s="5">
         <v>5</v>
@@ -4937,39 +4958,39 @@
         <v>142</v>
       </c>
       <c r="AM20" s="20" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:39">
       <c r="A21" s="4" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="4" t="s">
         <v>76</v>
       </c>
       <c r="D21" s="5">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="E21" s="11">
-        <v>80</v>
+        <v>12</v>
       </c>
       <c r="F21" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G21" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H21" s="5">
         <v>0</v>
       </c>
       <c r="I21" s="5">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="J21" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K21" s="5">
         <v>5</v>
@@ -5044,36 +5065,36 @@
         <v>142</v>
       </c>
       <c r="AM21" s="20" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:39">
-      <c r="A22" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B22" s="2" t="s">
+      <c r="A22" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D22" s="3">
-        <v>500</v>
-      </c>
-      <c r="E22" s="10">
-        <v>120</v>
-      </c>
-      <c r="F22" s="3">
-        <v>5</v>
-      </c>
-      <c r="G22" s="3">
+      <c r="D22" s="5">
+        <v>200</v>
+      </c>
+      <c r="E22" s="11">
+        <v>80</v>
+      </c>
+      <c r="F22" s="5">
         <v>2</v>
       </c>
-      <c r="H22" s="3">
-        <v>0</v>
-      </c>
-      <c r="I22" s="3">
-        <v>8</v>
+      <c r="G22" s="5">
+        <v>2</v>
+      </c>
+      <c r="H22" s="5">
+        <v>0</v>
+      </c>
+      <c r="I22" s="5">
+        <v>24</v>
       </c>
       <c r="J22" s="5">
         <v>0</v>
@@ -5141,9 +5162,7 @@
       <c r="AE22" s="17">
         <v>1</v>
       </c>
-      <c r="AF22" s="4">
-        <v>1</v>
-      </c>
+      <c r="AF22" s="4"/>
       <c r="AG22" s="4"/>
       <c r="AH22" s="4"/>
       <c r="AI22" s="4"/>
@@ -5153,36 +5172,36 @@
         <v>142</v>
       </c>
       <c r="AM22" s="20" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:39">
-      <c r="A23" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B23" s="4" t="s">
+      <c r="A23" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D23" s="5">
-        <v>300</v>
-      </c>
-      <c r="E23" s="11">
-        <v>90</v>
-      </c>
-      <c r="F23" s="5">
+      <c r="C23" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D23" s="3">
+        <v>500</v>
+      </c>
+      <c r="E23" s="10">
+        <v>120</v>
+      </c>
+      <c r="F23" s="3">
+        <v>5</v>
+      </c>
+      <c r="G23" s="3">
         <v>2</v>
       </c>
-      <c r="G23" s="5">
-        <v>2</v>
-      </c>
-      <c r="H23" s="5">
-        <v>0</v>
-      </c>
-      <c r="I23" s="5">
-        <v>24</v>
+      <c r="H23" s="3">
+        <v>0</v>
+      </c>
+      <c r="I23" s="3">
+        <v>8</v>
       </c>
       <c r="J23" s="5">
         <v>0</v>
@@ -5250,7 +5269,9 @@
       <c r="AE23" s="17">
         <v>1</v>
       </c>
-      <c r="AF23" s="4"/>
+      <c r="AF23" s="4">
+        <v>1</v>
+      </c>
       <c r="AG23" s="4"/>
       <c r="AH23" s="4"/>
       <c r="AI23" s="4"/>
@@ -5260,36 +5281,36 @@
         <v>142</v>
       </c>
       <c r="AM23" s="20" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:39">
       <c r="A24" s="4" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="4" t="s">
-        <v>80</v>
+      <c r="C24" s="2" t="s">
+        <v>79</v>
       </c>
       <c r="D24" s="5">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="E24" s="11">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="F24" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G24" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H24" s="5">
         <v>0</v>
       </c>
       <c r="I24" s="5">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="J24" s="5">
         <v>0</v>
@@ -5364,42 +5385,42 @@
       <c r="AJ24" s="4"/>
       <c r="AK24" s="4"/>
       <c r="AL24" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="AM24" s="20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:39">
       <c r="A25" s="4" t="s">
-        <v>107</v>
+        <v>24</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>108</v>
+        <v>13</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="D25" s="5">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="E25" s="11">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="F25" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G25" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H25" s="5">
         <v>0</v>
       </c>
       <c r="I25" s="5">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="J25" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K25" s="5">
         <v>5</v>
@@ -5471,15 +5492,15 @@
       <c r="AJ25" s="4"/>
       <c r="AK25" s="4"/>
       <c r="AL25" s="4" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="AM25" s="20" t="s">
-        <v>109</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:39">
       <c r="A26" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>108</v>
@@ -5490,23 +5511,23 @@
       <c r="D26" s="5">
         <v>100</v>
       </c>
-      <c r="E26" s="5">
-        <v>55</v>
+      <c r="E26" s="11">
+        <v>16</v>
       </c>
       <c r="F26" s="5">
         <v>1</v>
       </c>
       <c r="G26" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H26" s="5">
         <v>0</v>
       </c>
       <c r="I26" s="5">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="J26" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K26" s="5">
         <v>5</v>
@@ -5581,12 +5602,12 @@
         <v>142</v>
       </c>
       <c r="AM26" s="20" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="27" spans="1:39">
       <c r="A27" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>108</v>
@@ -5595,10 +5616,10 @@
         <v>76</v>
       </c>
       <c r="D27" s="5">
-        <v>150</v>
-      </c>
-      <c r="E27" s="3">
-        <v>24</v>
+        <v>100</v>
+      </c>
+      <c r="E27" s="5">
+        <v>55</v>
       </c>
       <c r="F27" s="5">
         <v>1</v>
@@ -5687,31 +5708,31 @@
       <c r="AL27" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="AM27" s="22" t="s">
-        <v>114</v>
+      <c r="AM27" s="20" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="28" spans="1:39">
       <c r="A28" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>108</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D28" s="5">
-        <v>0</v>
-      </c>
-      <c r="E28" s="5">
-        <v>110</v>
+        <v>150</v>
+      </c>
+      <c r="E28" s="3">
+        <v>24</v>
       </c>
       <c r="F28" s="5">
         <v>1</v>
       </c>
       <c r="G28" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H28" s="5">
         <v>0</v>
@@ -5756,7 +5777,7 @@
         <v>0</v>
       </c>
       <c r="V28" s="17">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="W28" s="17">
         <v>0</v>
@@ -5792,42 +5813,42 @@
       <c r="AJ28" s="4"/>
       <c r="AK28" s="4"/>
       <c r="AL28" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="AM28" s="20" t="s">
-        <v>115</v>
+        <v>142</v>
+      </c>
+      <c r="AM28" s="22" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="29" spans="1:39">
-      <c r="A29" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D29" s="3">
-        <v>60</v>
-      </c>
-      <c r="E29" s="10">
-        <v>8</v>
-      </c>
-      <c r="F29" s="3">
-        <v>1</v>
-      </c>
-      <c r="G29" s="3">
-        <v>1</v>
-      </c>
-      <c r="H29" s="3">
-        <v>0</v>
-      </c>
-      <c r="I29" s="3">
-        <v>4</v>
+      <c r="A29" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D29" s="5">
+        <v>0</v>
+      </c>
+      <c r="E29" s="5">
+        <v>110</v>
+      </c>
+      <c r="F29" s="5">
+        <v>1</v>
+      </c>
+      <c r="G29" s="5">
+        <v>3</v>
+      </c>
+      <c r="H29" s="5">
+        <v>0</v>
+      </c>
+      <c r="I29" s="5">
+        <v>12</v>
       </c>
       <c r="J29" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K29" s="5">
         <v>5</v>
@@ -5863,7 +5884,7 @@
         <v>0</v>
       </c>
       <c r="V29" s="17">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="W29" s="17">
         <v>0</v>
@@ -5899,42 +5920,42 @@
       <c r="AJ29" s="4"/>
       <c r="AK29" s="4"/>
       <c r="AL29" s="4" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="AM29" s="20" t="s">
-        <v>36</v>
+        <v>115</v>
       </c>
     </row>
     <row r="30" spans="1:39">
-      <c r="A30" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B30" s="4" t="s">
+      <c r="A30" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C30" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="D30" s="5">
-        <v>70</v>
-      </c>
-      <c r="E30" s="11">
-        <v>720</v>
-      </c>
-      <c r="F30" s="5">
-        <v>3</v>
-      </c>
-      <c r="G30" s="5">
-        <v>3</v>
-      </c>
-      <c r="H30" s="5">
-        <v>0</v>
-      </c>
-      <c r="I30" s="5">
+      <c r="C30" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D30" s="3">
+        <v>60</v>
+      </c>
+      <c r="E30" s="10">
+        <v>8</v>
+      </c>
+      <c r="F30" s="3">
+        <v>1</v>
+      </c>
+      <c r="G30" s="3">
+        <v>1</v>
+      </c>
+      <c r="H30" s="3">
+        <v>0</v>
+      </c>
+      <c r="I30" s="3">
         <v>4</v>
       </c>
       <c r="J30" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K30" s="5">
         <v>5</v>
@@ -6006,39 +6027,39 @@
       <c r="AJ30" s="4"/>
       <c r="AK30" s="4"/>
       <c r="AL30" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AM30" s="20" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="31" spans="1:39">
-      <c r="A31" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B31" s="2" t="s">
+      <c r="A31" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B31" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C31" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D31" s="3">
-        <v>50</v>
-      </c>
-      <c r="E31" s="10">
+      <c r="C31" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D31" s="5">
+        <v>70</v>
+      </c>
+      <c r="E31" s="11">
         <v>720</v>
       </c>
-      <c r="F31" s="3">
+      <c r="F31" s="5">
         <v>3</v>
       </c>
-      <c r="G31" s="3">
-        <v>1</v>
-      </c>
-      <c r="H31" s="3">
-        <v>0</v>
-      </c>
-      <c r="I31" s="3">
-        <v>72</v>
+      <c r="G31" s="5">
+        <v>3</v>
+      </c>
+      <c r="H31" s="5">
+        <v>0</v>
+      </c>
+      <c r="I31" s="5">
+        <v>4</v>
       </c>
       <c r="J31" s="5">
         <v>0</v>
@@ -6113,39 +6134,39 @@
       <c r="AJ31" s="4"/>
       <c r="AK31" s="4"/>
       <c r="AL31" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AM31" s="20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="32" spans="1:39">
-      <c r="A32" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B32" s="4" t="s">
+      <c r="A32" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C32" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="D32" s="5">
-        <v>80</v>
-      </c>
-      <c r="E32" s="11">
-        <v>100</v>
-      </c>
-      <c r="F32" s="5">
-        <v>5</v>
-      </c>
-      <c r="G32" s="5">
-        <v>2</v>
-      </c>
-      <c r="H32" s="5">
-        <v>0</v>
-      </c>
-      <c r="I32" s="5">
-        <v>12</v>
+      <c r="C32" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D32" s="3">
+        <v>50</v>
+      </c>
+      <c r="E32" s="10">
+        <v>720</v>
+      </c>
+      <c r="F32" s="3">
+        <v>3</v>
+      </c>
+      <c r="G32" s="3">
+        <v>1</v>
+      </c>
+      <c r="H32" s="3">
+        <v>0</v>
+      </c>
+      <c r="I32" s="3">
+        <v>72</v>
       </c>
       <c r="J32" s="5">
         <v>0</v>
@@ -6220,39 +6241,39 @@
       <c r="AJ32" s="4"/>
       <c r="AK32" s="4"/>
       <c r="AL32" s="4" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="AM32" s="20" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="33" spans="1:39">
-      <c r="A33" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C33" s="2" t="s">
+      <c r="A33" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D33" s="5">
         <v>80</v>
       </c>
-      <c r="D33" s="3">
-        <v>0</v>
-      </c>
-      <c r="E33" s="10">
-        <v>0</v>
-      </c>
-      <c r="F33" s="3">
-        <v>0</v>
-      </c>
-      <c r="G33" s="3">
-        <v>0</v>
-      </c>
-      <c r="H33" s="3">
-        <v>0</v>
-      </c>
-      <c r="I33" s="3">
-        <v>0</v>
+      <c r="E33" s="11">
+        <v>100</v>
+      </c>
+      <c r="F33" s="5">
+        <v>5</v>
+      </c>
+      <c r="G33" s="5">
+        <v>2</v>
+      </c>
+      <c r="H33" s="5">
+        <v>0</v>
+      </c>
+      <c r="I33" s="5">
+        <v>12</v>
       </c>
       <c r="J33" s="5">
         <v>0</v>
@@ -6326,37 +6347,39 @@
       <c r="AI33" s="4"/>
       <c r="AJ33" s="4"/>
       <c r="AK33" s="4"/>
-      <c r="AL33" s="4"/>
+      <c r="AL33" s="4" t="s">
+        <v>142</v>
+      </c>
       <c r="AM33" s="20" t="s">
-        <v>66</v>
+        <v>39</v>
       </c>
     </row>
     <row r="34" spans="1:39">
-      <c r="A34" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C34" s="4" t="s">
+      <c r="A34" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D34" s="5">
-        <v>0</v>
-      </c>
-      <c r="E34" s="11">
-        <v>0</v>
-      </c>
-      <c r="F34" s="5">
-        <v>0</v>
-      </c>
-      <c r="G34" s="5">
-        <v>0</v>
-      </c>
-      <c r="H34" s="5">
-        <v>0</v>
-      </c>
-      <c r="I34" s="5">
+      <c r="D34" s="3">
+        <v>0</v>
+      </c>
+      <c r="E34" s="10">
+        <v>0</v>
+      </c>
+      <c r="F34" s="3">
+        <v>0</v>
+      </c>
+      <c r="G34" s="3">
+        <v>0</v>
+      </c>
+      <c r="H34" s="3">
+        <v>0</v>
+      </c>
+      <c r="I34" s="3">
         <v>0</v>
       </c>
       <c r="J34" s="5">
@@ -6433,39 +6456,39 @@
       <c r="AK34" s="4"/>
       <c r="AL34" s="4"/>
       <c r="AM34" s="20" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="35" spans="1:39">
-      <c r="A35" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D35" s="3">
-        <v>30</v>
-      </c>
-      <c r="E35" s="10">
-        <v>16</v>
-      </c>
-      <c r="F35" s="3">
-        <v>1</v>
-      </c>
-      <c r="G35" s="3">
-        <v>1</v>
-      </c>
-      <c r="H35" s="3">
-        <v>0</v>
-      </c>
-      <c r="I35" s="3">
-        <v>4</v>
+      <c r="A35" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D35" s="5">
+        <v>0</v>
+      </c>
+      <c r="E35" s="11">
+        <v>0</v>
+      </c>
+      <c r="F35" s="5">
+        <v>0</v>
+      </c>
+      <c r="G35" s="5">
+        <v>0</v>
+      </c>
+      <c r="H35" s="5">
+        <v>0</v>
+      </c>
+      <c r="I35" s="5">
+        <v>0</v>
       </c>
       <c r="J35" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K35" s="5">
         <v>5</v>
@@ -6536,28 +6559,26 @@
       <c r="AI35" s="4"/>
       <c r="AJ35" s="4"/>
       <c r="AK35" s="4"/>
-      <c r="AL35" s="4" t="s">
-        <v>142</v>
-      </c>
+      <c r="AL35" s="4"/>
       <c r="AM35" s="20" t="s">
-        <v>104</v>
+        <v>70</v>
       </c>
     </row>
     <row r="36" spans="1:39">
       <c r="A36" s="2" t="s">
-        <v>55</v>
+        <v>102</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>56</v>
+        <v>103</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D36" s="3">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="E36" s="10">
-        <v>720</v>
+        <v>16</v>
       </c>
       <c r="F36" s="3">
         <v>1</v>
@@ -6566,16 +6587,16 @@
         <v>1</v>
       </c>
       <c r="H36" s="3">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="I36" s="3">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="J36" s="5">
         <v>1</v>
       </c>
       <c r="K36" s="5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="L36" s="17">
         <v>0</v>
@@ -6647,36 +6668,36 @@
         <v>142</v>
       </c>
       <c r="AM36" s="20" t="s">
-        <v>57</v>
+        <v>104</v>
       </c>
     </row>
     <row r="37" spans="1:39">
-      <c r="A37" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B37" s="4" t="s">
+      <c r="A37" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C37" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="D37" s="5">
-        <v>0</v>
-      </c>
-      <c r="E37" s="11">
-        <v>0</v>
-      </c>
-      <c r="F37" s="5">
-        <v>0</v>
-      </c>
-      <c r="G37" s="5">
-        <v>0</v>
-      </c>
-      <c r="H37" s="5">
-        <v>5</v>
-      </c>
-      <c r="I37" s="5">
-        <v>0</v>
+      <c r="C37" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D37" s="3">
+        <v>0</v>
+      </c>
+      <c r="E37" s="10">
+        <v>720</v>
+      </c>
+      <c r="F37" s="3">
+        <v>1</v>
+      </c>
+      <c r="G37" s="3">
+        <v>1</v>
+      </c>
+      <c r="H37" s="3">
+        <v>20</v>
+      </c>
+      <c r="I37" s="3">
+        <v>12</v>
       </c>
       <c r="J37" s="5">
         <v>1</v>
@@ -6750,37 +6771,39 @@
       <c r="AI37" s="4"/>
       <c r="AJ37" s="4"/>
       <c r="AK37" s="4"/>
-      <c r="AL37" s="4"/>
+      <c r="AL37" s="4" t="s">
+        <v>142</v>
+      </c>
       <c r="AM37" s="20" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
     </row>
     <row r="38" spans="1:39">
-      <c r="A38" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B38" s="2" t="s">
+      <c r="A38" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B38" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C38" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="D38" s="3">
-        <v>0</v>
-      </c>
-      <c r="E38" s="10">
-        <v>0</v>
-      </c>
-      <c r="F38" s="3">
-        <v>0</v>
-      </c>
-      <c r="G38" s="3">
-        <v>0</v>
-      </c>
-      <c r="H38" s="3">
+      <c r="D38" s="5">
+        <v>0</v>
+      </c>
+      <c r="E38" s="11">
+        <v>0</v>
+      </c>
+      <c r="F38" s="5">
+        <v>0</v>
+      </c>
+      <c r="G38" s="5">
+        <v>0</v>
+      </c>
+      <c r="H38" s="5">
         <v>5</v>
       </c>
-      <c r="I38" s="3">
+      <c r="I38" s="5">
         <v>0</v>
       </c>
       <c r="J38" s="5">
@@ -6857,35 +6880,35 @@
       <c r="AK38" s="4"/>
       <c r="AL38" s="4"/>
       <c r="AM38" s="20" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="39" spans="1:39">
-      <c r="A39" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="B39" s="4" t="s">
+      <c r="A39" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B39" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C39" s="4" t="s">
+      <c r="C39" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D39" s="5">
-        <v>0</v>
-      </c>
-      <c r="E39" s="11">
-        <v>0</v>
-      </c>
-      <c r="F39" s="5">
-        <v>0</v>
-      </c>
-      <c r="G39" s="5">
-        <v>0</v>
-      </c>
-      <c r="H39" s="5">
-        <v>15</v>
-      </c>
-      <c r="I39" s="5">
+      <c r="D39" s="3">
+        <v>0</v>
+      </c>
+      <c r="E39" s="10">
+        <v>0</v>
+      </c>
+      <c r="F39" s="3">
+        <v>0</v>
+      </c>
+      <c r="G39" s="3">
+        <v>0</v>
+      </c>
+      <c r="H39" s="3">
+        <v>5</v>
+      </c>
+      <c r="I39" s="3">
         <v>0</v>
       </c>
       <c r="J39" s="5">
@@ -6962,35 +6985,35 @@
       <c r="AK39" s="4"/>
       <c r="AL39" s="4"/>
       <c r="AM39" s="20" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
     </row>
     <row r="40" spans="1:39">
-      <c r="A40" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B40" s="2" t="s">
+      <c r="A40" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B40" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C40" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="D40" s="3">
-        <v>0</v>
-      </c>
-      <c r="E40" s="10">
-        <v>0</v>
-      </c>
-      <c r="F40" s="3">
-        <v>0</v>
-      </c>
-      <c r="G40" s="3">
-        <v>0</v>
-      </c>
-      <c r="H40" s="3">
-        <v>30</v>
-      </c>
-      <c r="I40" s="3">
+      <c r="D40" s="5">
+        <v>0</v>
+      </c>
+      <c r="E40" s="11">
+        <v>0</v>
+      </c>
+      <c r="F40" s="5">
+        <v>0</v>
+      </c>
+      <c r="G40" s="5">
+        <v>0</v>
+      </c>
+      <c r="H40" s="5">
+        <v>15</v>
+      </c>
+      <c r="I40" s="5">
         <v>0</v>
       </c>
       <c r="J40" s="5">
@@ -7067,35 +7090,35 @@
       <c r="AK40" s="4"/>
       <c r="AL40" s="4"/>
       <c r="AM40" s="20" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="41" spans="1:39">
-      <c r="A41" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B41" s="4" t="s">
+      <c r="A41" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B41" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C41" s="4" t="s">
+      <c r="C41" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D41" s="5">
-        <v>0</v>
-      </c>
-      <c r="E41" s="11">
-        <v>0</v>
-      </c>
-      <c r="F41" s="5">
-        <v>0</v>
-      </c>
-      <c r="G41" s="5">
-        <v>0</v>
-      </c>
-      <c r="H41" s="5">
-        <v>60</v>
-      </c>
-      <c r="I41" s="5">
+      <c r="D41" s="3">
+        <v>0</v>
+      </c>
+      <c r="E41" s="10">
+        <v>0</v>
+      </c>
+      <c r="F41" s="3">
+        <v>0</v>
+      </c>
+      <c r="G41" s="3">
+        <v>0</v>
+      </c>
+      <c r="H41" s="3">
+        <v>30</v>
+      </c>
+      <c r="I41" s="3">
         <v>0</v>
       </c>
       <c r="J41" s="5">
@@ -7172,36 +7195,36 @@
       <c r="AK41" s="4"/>
       <c r="AL41" s="4"/>
       <c r="AM41" s="20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="42" spans="1:39">
-      <c r="A42" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D42" s="3">
-        <v>400</v>
-      </c>
-      <c r="E42" s="10">
-        <v>48</v>
-      </c>
-      <c r="F42" s="3">
-        <v>1</v>
-      </c>
-      <c r="G42" s="3">
-        <v>2</v>
-      </c>
-      <c r="H42" s="3">
-        <v>0</v>
-      </c>
-      <c r="I42" s="3">
-        <v>12</v>
+      <c r="A42" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D42" s="5">
+        <v>0</v>
+      </c>
+      <c r="E42" s="11">
+        <v>0</v>
+      </c>
+      <c r="F42" s="5">
+        <v>0</v>
+      </c>
+      <c r="G42" s="5">
+        <v>0</v>
+      </c>
+      <c r="H42" s="5">
+        <v>60</v>
+      </c>
+      <c r="I42" s="5">
+        <v>0</v>
       </c>
       <c r="J42" s="5">
         <v>1</v>
@@ -7277,111 +7300,216 @@
       <c r="AK42" s="4"/>
       <c r="AL42" s="4"/>
       <c r="AM42" s="20" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
     </row>
     <row r="43" spans="1:39">
-      <c r="A43" s="6" t="s">
+      <c r="A43" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D43" s="3">
+        <v>400</v>
+      </c>
+      <c r="E43" s="10">
+        <v>48</v>
+      </c>
+      <c r="F43" s="3">
+        <v>1</v>
+      </c>
+      <c r="G43" s="3">
+        <v>2</v>
+      </c>
+      <c r="H43" s="3">
+        <v>0</v>
+      </c>
+      <c r="I43" s="3">
+        <v>12</v>
+      </c>
+      <c r="J43" s="5">
+        <v>1</v>
+      </c>
+      <c r="K43" s="5">
+        <v>1</v>
+      </c>
+      <c r="L43" s="17">
+        <v>0</v>
+      </c>
+      <c r="M43" s="17">
+        <v>0</v>
+      </c>
+      <c r="N43" s="17">
+        <v>0</v>
+      </c>
+      <c r="O43" s="17">
+        <v>0</v>
+      </c>
+      <c r="P43" s="17">
+        <v>0</v>
+      </c>
+      <c r="Q43" s="17">
+        <v>0</v>
+      </c>
+      <c r="R43" s="17">
+        <v>0</v>
+      </c>
+      <c r="S43" s="17">
+        <v>0</v>
+      </c>
+      <c r="T43" s="17">
+        <v>0</v>
+      </c>
+      <c r="U43" s="17">
+        <v>0</v>
+      </c>
+      <c r="V43" s="17">
+        <v>0</v>
+      </c>
+      <c r="W43" s="17">
+        <v>0</v>
+      </c>
+      <c r="X43" s="17">
+        <v>0</v>
+      </c>
+      <c r="Y43" s="17">
+        <v>0</v>
+      </c>
+      <c r="Z43" s="17">
+        <v>0</v>
+      </c>
+      <c r="AA43" s="17">
+        <v>0</v>
+      </c>
+      <c r="AB43" s="17">
+        <v>0</v>
+      </c>
+      <c r="AC43" s="17">
+        <v>0</v>
+      </c>
+      <c r="AD43" s="17">
+        <v>0</v>
+      </c>
+      <c r="AE43" s="17">
+        <v>1</v>
+      </c>
+      <c r="AF43" s="4"/>
+      <c r="AG43" s="4"/>
+      <c r="AH43" s="4"/>
+      <c r="AI43" s="4"/>
+      <c r="AJ43" s="4"/>
+      <c r="AK43" s="4"/>
+      <c r="AL43" s="4"/>
+      <c r="AM43" s="20" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="44" spans="1:39">
+      <c r="A44" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B43" s="6" t="s">
+      <c r="B44" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C43" s="6" t="s">
+      <c r="C44" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="D43" s="7">
+      <c r="D44" s="7">
         <v>400</v>
       </c>
-      <c r="E43" s="12">
+      <c r="E44" s="12">
         <v>48</v>
       </c>
-      <c r="F43" s="7">
-        <v>1</v>
-      </c>
-      <c r="G43" s="7">
+      <c r="F44" s="7">
+        <v>1</v>
+      </c>
+      <c r="G44" s="7">
         <v>2</v>
       </c>
-      <c r="H43" s="7">
-        <v>0</v>
-      </c>
-      <c r="I43" s="7">
+      <c r="H44" s="7">
+        <v>0</v>
+      </c>
+      <c r="I44" s="7">
         <v>12</v>
       </c>
-      <c r="J43" s="7">
-        <v>1</v>
-      </c>
-      <c r="K43" s="7">
-        <v>1</v>
-      </c>
-      <c r="L43" s="18">
-        <v>0</v>
-      </c>
-      <c r="M43" s="17">
-        <v>0</v>
-      </c>
-      <c r="N43" s="17">
-        <v>0</v>
-      </c>
-      <c r="O43" s="17">
-        <v>0</v>
-      </c>
-      <c r="P43" s="17">
-        <v>0</v>
-      </c>
-      <c r="Q43" s="17">
-        <v>0</v>
-      </c>
-      <c r="R43" s="17">
-        <v>0</v>
-      </c>
-      <c r="S43" s="17">
-        <v>0</v>
-      </c>
-      <c r="T43" s="17">
-        <v>0</v>
-      </c>
-      <c r="U43" s="17">
-        <v>0</v>
-      </c>
-      <c r="V43" s="17">
-        <v>0</v>
-      </c>
-      <c r="W43" s="17">
-        <v>0</v>
-      </c>
-      <c r="X43" s="17">
-        <v>0</v>
-      </c>
-      <c r="Y43" s="17">
-        <v>0</v>
-      </c>
-      <c r="Z43" s="17">
-        <v>0</v>
-      </c>
-      <c r="AA43" s="17">
-        <v>0</v>
-      </c>
-      <c r="AB43" s="17">
-        <v>0</v>
-      </c>
-      <c r="AC43" s="17">
-        <v>0</v>
-      </c>
-      <c r="AD43" s="17">
-        <v>0</v>
-      </c>
-      <c r="AE43" s="18">
-        <v>1</v>
-      </c>
-      <c r="AF43" s="6"/>
-      <c r="AG43" s="6"/>
-      <c r="AH43" s="6"/>
-      <c r="AI43" s="6"/>
-      <c r="AJ43" s="6"/>
-      <c r="AK43" s="6"/>
-      <c r="AL43" s="6"/>
-      <c r="AM43" s="21" t="s">
+      <c r="J44" s="7">
+        <v>1</v>
+      </c>
+      <c r="K44" s="7">
+        <v>1</v>
+      </c>
+      <c r="L44" s="18">
+        <v>0</v>
+      </c>
+      <c r="M44" s="17">
+        <v>0</v>
+      </c>
+      <c r="N44" s="17">
+        <v>0</v>
+      </c>
+      <c r="O44" s="17">
+        <v>0</v>
+      </c>
+      <c r="P44" s="17">
+        <v>0</v>
+      </c>
+      <c r="Q44" s="17">
+        <v>0</v>
+      </c>
+      <c r="R44" s="17">
+        <v>0</v>
+      </c>
+      <c r="S44" s="17">
+        <v>0</v>
+      </c>
+      <c r="T44" s="17">
+        <v>0</v>
+      </c>
+      <c r="U44" s="17">
+        <v>0</v>
+      </c>
+      <c r="V44" s="17">
+        <v>0</v>
+      </c>
+      <c r="W44" s="17">
+        <v>0</v>
+      </c>
+      <c r="X44" s="17">
+        <v>0</v>
+      </c>
+      <c r="Y44" s="17">
+        <v>0</v>
+      </c>
+      <c r="Z44" s="17">
+        <v>0</v>
+      </c>
+      <c r="AA44" s="17">
+        <v>0</v>
+      </c>
+      <c r="AB44" s="17">
+        <v>0</v>
+      </c>
+      <c r="AC44" s="17">
+        <v>0</v>
+      </c>
+      <c r="AD44" s="17">
+        <v>0</v>
+      </c>
+      <c r="AE44" s="18">
+        <v>1</v>
+      </c>
+      <c r="AF44" s="6"/>
+      <c r="AG44" s="6"/>
+      <c r="AH44" s="6"/>
+      <c r="AI44" s="6"/>
+      <c r="AJ44" s="6"/>
+      <c r="AK44" s="6"/>
+      <c r="AL44" s="6"/>
+      <c r="AM44" s="21" t="s">
         <v>54</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Some attack movement implemented. GOTTA FIX MOVEMENT BUGS SOON.
</commit_message>
<xml_diff>
--- a/xml/Abilities.xlsx
+++ b/xml/Abilities.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="180">
   <si>
     <t>Name</t>
   </si>
@@ -54,9 +54,6 @@
     <t>C. Kata</t>
   </si>
   <si>
-    <t>Stomping Ground</t>
-  </si>
-  <si>
     <t>John T.</t>
   </si>
   <si>
@@ -66,21 +63,12 @@
     <t>Mediation</t>
   </si>
   <si>
-    <t>Stuns an enemy for two seconds.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shoots four arrows toward a target. </t>
-  </si>
-  <si>
     <t>Hoverpad Attack</t>
   </si>
   <si>
     <t>Railgun Attack</t>
   </si>
   <si>
-    <t>Throws a random shoe toward a target out of anger.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Dashes in a straight line, inflicting Stun. </t>
   </si>
   <si>
@@ -96,9 +84,6 @@
     <t>Creates a magic and apologetic wall that lasts for four seconds.</t>
   </si>
   <si>
-    <t>Restores 1 HP per second. But really, he stopped doing this a few months ago. No REALLY. OMG SHUT UP, YOU HATER.</t>
-  </si>
-  <si>
     <t>Perk-kulate</t>
   </si>
   <si>
@@ -165,9 +150,6 @@
     <t>Improve self and ally's attack speeds</t>
   </si>
   <si>
-    <t>Teleport self and ally to a point</t>
-  </si>
-  <si>
     <t>Girly Swirl</t>
   </si>
   <si>
@@ -195,12 +177,6 @@
     <t>Second Chance</t>
   </si>
   <si>
-    <t>Revives this Unit to 1 HP after he/she reaches 0 HP. Can only be used once per stage.</t>
-  </si>
-  <si>
-    <t>Second Wind</t>
-  </si>
-  <si>
     <t>Second World</t>
   </si>
   <si>
@@ -249,9 +225,6 @@
     <t>Damage</t>
   </si>
   <si>
-    <t>Support</t>
-  </si>
-  <si>
     <t>Teleport</t>
   </si>
   <si>
@@ -267,9 +240,6 @@
     <t>Stop</t>
   </si>
   <si>
-    <t>Nothing</t>
-  </si>
-  <si>
     <t>Claw Attack</t>
   </si>
   <si>
@@ -339,9 +309,6 @@
     <t>HPLump</t>
   </si>
   <si>
-    <t>Voice Attack</t>
-  </si>
-  <si>
     <t>Huong V.</t>
   </si>
   <si>
@@ -390,9 +357,6 @@
     <t>A. Mediation</t>
   </si>
   <si>
-    <t>[Aggressive Mediation] Jump up and down violently, which solves nothing at all. HA TAKE THAT KATA</t>
-  </si>
-  <si>
     <t>SlowPerc</t>
   </si>
   <si>
@@ -457,6 +421,141 @@
   </si>
   <si>
     <t>Stuns all enemies within the shout's range for a second. gogoloudwhitegirl</t>
+  </si>
+  <si>
+    <t>Beatrice C.</t>
+  </si>
+  <si>
+    <t>Happiness</t>
+  </si>
+  <si>
+    <t>Sunshine</t>
+  </si>
+  <si>
+    <t>Tevin J.</t>
+  </si>
+  <si>
+    <t>Lung Crusher</t>
+  </si>
+  <si>
+    <t>Deep Sleep</t>
+  </si>
+  <si>
+    <t>Sonic Laugh</t>
+  </si>
+  <si>
+    <t>Basic Attack: Charge toward an enemy and overpower it.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Restores HP over time. Tevin cannot move nor use abilities during this time. </t>
+  </si>
+  <si>
+    <t>Launches a conical sound blast in front of him, damaging and slowing down enemies.</t>
+  </si>
+  <si>
+    <t>Crushes the enemy through the power of hugging at close-range.</t>
+  </si>
+  <si>
+    <t>Raymon B.</t>
+  </si>
+  <si>
+    <t>Siphon</t>
+  </si>
+  <si>
+    <t>Shockwave</t>
+  </si>
+  <si>
+    <t>Bio-Leech</t>
+  </si>
+  <si>
+    <t>Overload</t>
+  </si>
+  <si>
+    <t>Machine Gun Attack</t>
+  </si>
+  <si>
+    <t>Strength Attack</t>
+  </si>
+  <si>
+    <t>Seals an enemy in a magical circlet, which slows the enemy and siphons HP after a few seconds.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Creates a temporary aura of circles that heals Cia and deals damage to closeby enemies. </t>
+  </si>
+  <si>
+    <t>Cheer</t>
+  </si>
+  <si>
+    <t>C. Kata restores some HP every few seconds.</t>
+  </si>
+  <si>
+    <t>Upgrade</t>
+  </si>
+  <si>
+    <t>Downgrade</t>
+  </si>
+  <si>
+    <t>Nearby enemies surrounding Cia are slowed for a few seconds.</t>
+  </si>
+  <si>
+    <t>Stuns an enemy for a few seconds.</t>
+  </si>
+  <si>
+    <t>Restores a small amount of HP per second. But really, he stopped doing this a few months ago. REALLY. OMG SHUT UP, YOU HATER.</t>
+  </si>
+  <si>
+    <t>Logic Puzzle</t>
+  </si>
+  <si>
+    <t>Bling Bling</t>
+  </si>
+  <si>
+    <t>Taking Heart</t>
+  </si>
+  <si>
+    <t>Damages enemies in a wave</t>
+  </si>
+  <si>
+    <t>Drain HP from target enemy</t>
+  </si>
+  <si>
+    <t>After channeling, unleash massive damage to nearby enemies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Basic Attack: Shoot down an enemy with rapid gunfire. </t>
+  </si>
+  <si>
+    <t>Creates a ray of solar energy.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gains one solar charge every few seconds. After gaining three charges and activating again, sends forth bursts of solar energy. </t>
+  </si>
+  <si>
+    <t>Teleports Charles and Nate to a point. Afterwards, shoots kunais outward that temporarily stuns nearby enemies.</t>
+  </si>
+  <si>
+    <t>Ananya A.</t>
+  </si>
+  <si>
+    <t>Final Destination</t>
+  </si>
+  <si>
+    <t>Change X's and Ananya's Friendship Finale to Destination Zero.</t>
+  </si>
+  <si>
+    <t>[Aggressive Mediation] Jump up and down violently. Probably does nothing at all. HA TAKE THAT KATA</t>
+  </si>
+  <si>
+    <t>Arrow Control</t>
+  </si>
+  <si>
+    <t>Megaphone Attack</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Throws a random shoe toward a target out of anger. </t>
+  </si>
+  <si>
+    <t>Shoots arrows toward a target.</t>
   </si>
 </sst>
 </file>
@@ -601,7 +700,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -638,6 +737,10 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2457,8 +2560,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:AM44" tableType="xml" totalsRowShown="0" headerRowDxfId="42" dataDxfId="40" headerRowBorderDxfId="41" tableBorderDxfId="39">
-  <autoFilter ref="A2:AM44"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:AM58" tableType="xml" totalsRowShown="0" headerRowDxfId="42" dataDxfId="40" headerRowBorderDxfId="41" tableBorderDxfId="39">
+  <autoFilter ref="A2:AM58"/>
   <tableColumns count="39">
     <tableColumn id="1" uniqueName="Name" name="Name" dataDxfId="38">
       <xmlColumnPr mapId="12" xpath="/Abilities/Ability/Name" xmlDataType="string"/>
@@ -2867,18 +2970,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AM44"/>
+  <dimension ref="A1:AM58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AG1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AM14" sqref="AM14"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="1" max="1" width="19" customWidth="1"/>
     <col min="2" max="2" width="13.28515625" customWidth="1"/>
-    <col min="3" max="3" width="10" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" customWidth="1"/>
     <col min="4" max="4" width="9.28515625" customWidth="1"/>
     <col min="5" max="5" width="11.42578125" customWidth="1"/>
     <col min="6" max="6" width="8" customWidth="1"/>
@@ -2904,12 +3007,12 @@
     <col min="35" max="35" width="9" customWidth="1"/>
     <col min="36" max="37" width="17.42578125" customWidth="1"/>
     <col min="38" max="38" width="10.42578125" customWidth="1"/>
-    <col min="39" max="39" width="107" customWidth="1"/>
+    <col min="39" max="39" width="119.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:39">
       <c r="G1" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:39" ht="15.75" thickBot="1">
@@ -2920,7 +3023,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="D2" s="15" t="s">
         <v>2</v>
@@ -2941,91 +3044,91 @@
         <v>8</v>
       </c>
       <c r="J2" s="15" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="K2" s="15" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="L2" s="15" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="M2" s="15" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="N2" s="15" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="O2" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="P2" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q2" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="R2" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="S2" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="T2" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="U2" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="V2" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="W2" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="X2" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="Y2" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="Z2" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="AA2" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="AB2" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="AC2" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="AD2" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="AE2" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="AF2" s="19" t="s">
         <v>129</v>
       </c>
-      <c r="P2" s="15" t="s">
+      <c r="AG2" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="AH2" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="AI2" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="AJ2" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="AK2" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="AL2" s="19" t="s">
         <v>128</v>
-      </c>
-      <c r="Q2" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="R2" s="15" t="s">
-        <v>138</v>
-      </c>
-      <c r="S2" s="15" t="s">
-        <v>125</v>
-      </c>
-      <c r="T2" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="U2" s="15" t="s">
-        <v>139</v>
-      </c>
-      <c r="V2" s="15" t="s">
-        <v>105</v>
-      </c>
-      <c r="W2" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="X2" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="Y2" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="Z2" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="AA2" s="13" t="s">
-        <v>121</v>
-      </c>
-      <c r="AB2" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="AC2" s="13" t="s">
-        <v>116</v>
-      </c>
-      <c r="AD2" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="AE2" s="13" t="s">
-        <v>131</v>
-      </c>
-      <c r="AF2" s="19" t="s">
-        <v>141</v>
-      </c>
-      <c r="AG2" s="19" t="s">
-        <v>132</v>
-      </c>
-      <c r="AH2" s="19" t="s">
-        <v>133</v>
-      </c>
-      <c r="AI2" s="19" t="s">
-        <v>134</v>
-      </c>
-      <c r="AJ2" s="19" t="s">
-        <v>135</v>
-      </c>
-      <c r="AK2" s="19" t="s">
-        <v>136</v>
-      </c>
-      <c r="AL2" s="19" t="s">
-        <v>140</v>
       </c>
       <c r="AM2" s="19" t="s">
         <v>1</v>
@@ -3033,13 +3136,13 @@
     </row>
     <row r="3" spans="1:39" ht="15.75" thickTop="1">
       <c r="A3" s="9" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="D3" s="3">
         <v>80</v>
@@ -3066,10 +3169,10 @@
         <v>5</v>
       </c>
       <c r="L3" s="17">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M3" s="17">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="N3" s="17">
         <v>0</v>
@@ -3132,21 +3235,21 @@
       <c r="AJ3" s="4"/>
       <c r="AK3" s="4"/>
       <c r="AL3" s="4" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="AM3" s="20" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:39">
       <c r="A4" s="9" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="D4" s="3">
         <v>80</v>
@@ -3173,7 +3276,7 @@
         <v>5</v>
       </c>
       <c r="L4" s="17">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="M4" s="17">
         <v>0</v>
@@ -3241,21 +3344,21 @@
       <c r="AJ4" s="4"/>
       <c r="AK4" s="4"/>
       <c r="AL4" s="4" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="AM4" s="20" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:39">
       <c r="A5" s="4" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>77</v>
+        <v>41</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>157</v>
       </c>
       <c r="D5" s="5">
         <v>140</v>
@@ -3348,21 +3451,21 @@
       <c r="AJ5" s="4"/>
       <c r="AK5" s="4"/>
       <c r="AL5" s="4" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="AM5" s="20" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:39">
       <c r="A6" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="D6" s="3">
         <v>30</v>
@@ -3389,10 +3492,10 @@
         <v>5</v>
       </c>
       <c r="L6" s="17">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="M6" s="17">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N6" s="17">
         <v>0</v>
@@ -3455,21 +3558,21 @@
       <c r="AJ6" s="4"/>
       <c r="AK6" s="4"/>
       <c r="AL6" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="AM6" s="20" t="s">
-        <v>49</v>
+        <v>131</v>
+      </c>
+      <c r="AM6" s="30" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="7" spans="1:39">
       <c r="A7" s="2" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="D7" s="3">
         <v>20</v>
@@ -3496,10 +3599,10 @@
         <v>5</v>
       </c>
       <c r="L7" s="17">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M7" s="17">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="N7" s="17">
         <v>0</v>
@@ -3562,21 +3665,21 @@
       <c r="AJ7" s="4"/>
       <c r="AK7" s="4"/>
       <c r="AL7" s="4" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="AM7" s="20" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:39">
       <c r="A8" s="2" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
+      </c>
+      <c r="C8" s="29" t="s">
+        <v>157</v>
       </c>
       <c r="D8" s="3">
         <v>0</v>
@@ -3669,21 +3772,21 @@
       <c r="AJ8" s="4"/>
       <c r="AK8" s="4"/>
       <c r="AL8" s="4" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="AM8" s="20" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:39">
       <c r="A9" s="2" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="D9" s="3">
         <v>120</v>
@@ -3710,10 +3813,10 @@
         <v>5</v>
       </c>
       <c r="L9" s="17">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M9" s="17">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="N9" s="17">
         <v>0</v>
@@ -3776,21 +3879,21 @@
       <c r="AJ9" s="4"/>
       <c r="AK9" s="4"/>
       <c r="AL9" s="4" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="AM9" s="20" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:39">
       <c r="A10" s="2" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
+      </c>
+      <c r="C10" s="29" t="s">
+        <v>157</v>
       </c>
       <c r="D10" s="5">
         <v>50</v>
@@ -3883,21 +3986,21 @@
       <c r="AJ10" s="4"/>
       <c r="AK10" s="4"/>
       <c r="AL10" s="4" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="AM10" s="20" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:39">
       <c r="A11" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="D11" s="3">
         <v>400</v>
@@ -3924,10 +4027,10 @@
         <v>5</v>
       </c>
       <c r="L11" s="17">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M11" s="17">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="N11" s="17">
         <v>0</v>
@@ -3990,10 +4093,10 @@
       <c r="AJ11" s="4"/>
       <c r="AK11" s="4"/>
       <c r="AL11" s="4" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="AM11" s="20" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:39">
@@ -4004,7 +4107,7 @@
         <v>11</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="D12" s="3">
         <v>500</v>
@@ -4031,10 +4134,10 @@
         <v>5</v>
       </c>
       <c r="L12" s="17">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M12" s="17">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="N12" s="17">
         <v>0</v>
@@ -4097,10 +4200,10 @@
       <c r="AJ12" s="4"/>
       <c r="AK12" s="4"/>
       <c r="AL12" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="AM12" s="20" t="s">
-        <v>16</v>
+        <v>130</v>
+      </c>
+      <c r="AM12" s="30" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="13" spans="1:39">
@@ -4111,7 +4214,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="D13" s="3">
         <v>500</v>
@@ -4138,10 +4241,10 @@
         <v>5</v>
       </c>
       <c r="L13" s="17">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M13" s="17">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="N13" s="17">
         <v>0</v>
@@ -4204,21 +4307,21 @@
       <c r="AJ13" s="4"/>
       <c r="AK13" s="4"/>
       <c r="AL13" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="AM13" s="20" t="s">
-        <v>20</v>
+        <v>130</v>
+      </c>
+      <c r="AM13" s="30" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="14" spans="1:39">
       <c r="A14" s="23" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="B14" s="23" t="s">
         <v>11</v>
       </c>
       <c r="C14" s="23" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="D14" s="24">
         <v>200</v>
@@ -4245,10 +4348,10 @@
         <v>5</v>
       </c>
       <c r="L14" s="26">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="M14" s="26">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="N14" s="26">
         <v>0</v>
@@ -4313,30 +4416,30 @@
       <c r="AJ14" s="26"/>
       <c r="AK14" s="26"/>
       <c r="AL14" s="23" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="AM14" s="27" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
     </row>
     <row r="15" spans="1:39">
       <c r="A15" s="2" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>83</v>
+      <c r="C15" s="29" t="s">
+        <v>68</v>
       </c>
       <c r="D15" s="3">
         <v>0</v>
       </c>
       <c r="E15" s="10">
-        <v>0</v>
+        <v>240</v>
       </c>
       <c r="F15" s="3">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="G15" s="3">
         <v>1</v>
@@ -4351,13 +4454,13 @@
         <v>0</v>
       </c>
       <c r="K15" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="L15" s="17">
         <v>0</v>
       </c>
       <c r="M15" s="17">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="N15" s="17">
         <v>0</v>
@@ -4419,22 +4522,22 @@
       <c r="AI15" s="4"/>
       <c r="AJ15" s="4"/>
       <c r="AK15" s="4"/>
-      <c r="AL15" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="AM15" s="20" t="s">
-        <v>124</v>
+      <c r="AL15" s="28" t="s">
+        <v>130</v>
+      </c>
+      <c r="AM15" s="30" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="16" spans="1:39">
       <c r="A16" s="4" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="D16" s="5">
         <v>400</v>
@@ -4461,10 +4564,10 @@
         <v>5</v>
       </c>
       <c r="L16" s="17">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M16" s="17">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="N16" s="17">
         <v>0</v>
@@ -4527,51 +4630,51 @@
       <c r="AJ16" s="4"/>
       <c r="AK16" s="4"/>
       <c r="AL16" s="4" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="AM16" s="20" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17" spans="1:39">
-      <c r="A17" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="D17" s="5">
-        <v>80</v>
-      </c>
-      <c r="E17" s="11">
+      <c r="A17" s="23" t="s">
+        <v>163</v>
+      </c>
+      <c r="B17" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="C17" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="D17" s="24">
+        <v>50</v>
+      </c>
+      <c r="E17" s="25">
+        <v>120</v>
+      </c>
+      <c r="F17" s="24">
+        <v>1</v>
+      </c>
+      <c r="G17" s="24">
+        <v>1</v>
+      </c>
+      <c r="H17" s="24">
+        <v>0</v>
+      </c>
+      <c r="I17" s="24">
         <v>12</v>
       </c>
-      <c r="F17" s="5">
-        <v>1</v>
-      </c>
-      <c r="G17" s="5">
-        <v>1</v>
-      </c>
-      <c r="H17" s="5">
-        <v>0</v>
-      </c>
-      <c r="I17" s="5">
-        <v>6</v>
-      </c>
-      <c r="J17" s="5">
-        <v>1</v>
-      </c>
-      <c r="K17" s="5">
+      <c r="J17" s="24">
+        <v>0</v>
+      </c>
+      <c r="K17" s="24">
         <v>5</v>
       </c>
       <c r="L17" s="17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M17" s="17">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="N17" s="17">
         <v>0</v>
@@ -4627,55 +4730,55 @@
       <c r="AE17" s="17">
         <v>1</v>
       </c>
-      <c r="AF17" s="4"/>
-      <c r="AG17" s="4"/>
-      <c r="AH17" s="4"/>
-      <c r="AI17" s="4"/>
-      <c r="AJ17" s="4"/>
-      <c r="AK17" s="4"/>
-      <c r="AL17" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="AM17" s="20" t="s">
-        <v>33</v>
+      <c r="AF17" s="26"/>
+      <c r="AG17" s="26"/>
+      <c r="AH17" s="26"/>
+      <c r="AI17" s="26"/>
+      <c r="AJ17" s="26"/>
+      <c r="AK17" s="26"/>
+      <c r="AL17" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="AM17" s="27" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="18" spans="1:39">
-      <c r="A18" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D18" s="3">
-        <v>50</v>
-      </c>
-      <c r="E18" s="10">
-        <v>60</v>
-      </c>
-      <c r="F18" s="3">
-        <v>3</v>
-      </c>
-      <c r="G18" s="3">
-        <v>1</v>
-      </c>
-      <c r="H18" s="3">
-        <v>0</v>
-      </c>
-      <c r="I18" s="3">
-        <v>24</v>
-      </c>
-      <c r="J18" s="5">
-        <v>0</v>
-      </c>
-      <c r="K18" s="5">
+      <c r="A18" s="23" t="s">
+        <v>164</v>
+      </c>
+      <c r="B18" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="C18" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="D18" s="24">
+        <v>800</v>
+      </c>
+      <c r="E18" s="25">
+        <v>120</v>
+      </c>
+      <c r="F18" s="24">
+        <v>1</v>
+      </c>
+      <c r="G18" s="24">
+        <v>2</v>
+      </c>
+      <c r="H18" s="24">
+        <v>0</v>
+      </c>
+      <c r="I18" s="24">
+        <v>12</v>
+      </c>
+      <c r="J18" s="24">
+        <v>0</v>
+      </c>
+      <c r="K18" s="24">
         <v>5</v>
       </c>
       <c r="L18" s="17">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M18" s="17">
         <v>0</v>
@@ -4732,60 +4835,60 @@
         <v>0</v>
       </c>
       <c r="AE18" s="17">
-        <v>1</v>
-      </c>
-      <c r="AF18" s="4"/>
-      <c r="AG18" s="4"/>
-      <c r="AH18" s="4"/>
-      <c r="AI18" s="4"/>
-      <c r="AJ18" s="4"/>
-      <c r="AK18" s="4"/>
-      <c r="AL18" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="AM18" s="20" t="s">
-        <v>30</v>
+        <v>0</v>
+      </c>
+      <c r="AF18" s="26"/>
+      <c r="AG18" s="26"/>
+      <c r="AH18" s="26"/>
+      <c r="AI18" s="26"/>
+      <c r="AJ18" s="26"/>
+      <c r="AK18" s="26"/>
+      <c r="AL18" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="AM18" s="27" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="19" spans="1:39">
-      <c r="A19" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="D19" s="5">
+      <c r="A19" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="B19" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="C19" s="23" t="s">
+        <v>158</v>
+      </c>
+      <c r="D19" s="24">
         <v>100</v>
       </c>
-      <c r="E19" s="11">
-        <v>70</v>
-      </c>
-      <c r="F19" s="5">
-        <v>1</v>
-      </c>
-      <c r="G19" s="5">
-        <v>2</v>
-      </c>
-      <c r="H19" s="5">
-        <v>0</v>
-      </c>
-      <c r="I19" s="5">
-        <v>24</v>
-      </c>
-      <c r="J19" s="5">
-        <v>0</v>
-      </c>
-      <c r="K19" s="5">
+      <c r="E19" s="25">
+        <v>120</v>
+      </c>
+      <c r="F19" s="24">
+        <v>1</v>
+      </c>
+      <c r="G19" s="24">
+        <v>1</v>
+      </c>
+      <c r="H19" s="24">
+        <v>0</v>
+      </c>
+      <c r="I19" s="24">
+        <v>12</v>
+      </c>
+      <c r="J19" s="24">
+        <v>0</v>
+      </c>
+      <c r="K19" s="24">
         <v>5</v>
       </c>
       <c r="L19" s="17">
         <v>0</v>
       </c>
       <c r="M19" s="17">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="N19" s="17">
         <v>0</v>
@@ -4839,53 +4942,53 @@
         <v>0</v>
       </c>
       <c r="AE19" s="17">
-        <v>1</v>
-      </c>
-      <c r="AF19" s="4"/>
-      <c r="AG19" s="4"/>
-      <c r="AH19" s="4"/>
-      <c r="AI19" s="4"/>
-      <c r="AJ19" s="4"/>
-      <c r="AK19" s="4"/>
-      <c r="AL19" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="AM19" s="20" t="s">
-        <v>99</v>
+        <v>0</v>
+      </c>
+      <c r="AF19" s="26"/>
+      <c r="AG19" s="26"/>
+      <c r="AH19" s="26"/>
+      <c r="AI19" s="26"/>
+      <c r="AJ19" s="26"/>
+      <c r="AK19" s="26"/>
+      <c r="AL19" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="AM19" s="27" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="20" spans="1:39">
-      <c r="A20" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D20" s="3">
-        <v>100</v>
-      </c>
-      <c r="E20" s="10">
-        <v>80</v>
-      </c>
-      <c r="F20" s="3">
-        <v>1</v>
-      </c>
-      <c r="G20" s="3">
-        <v>1</v>
-      </c>
-      <c r="H20" s="3">
-        <v>0</v>
-      </c>
-      <c r="I20" s="3">
-        <v>24</v>
-      </c>
-      <c r="J20" s="5">
-        <v>0</v>
-      </c>
-      <c r="K20" s="5">
+      <c r="A20" s="23" t="s">
+        <v>155</v>
+      </c>
+      <c r="B20" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="C20" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="D20" s="24">
+        <v>0</v>
+      </c>
+      <c r="E20" s="25">
+        <v>0</v>
+      </c>
+      <c r="F20" s="24">
+        <v>0</v>
+      </c>
+      <c r="G20" s="24">
+        <v>0</v>
+      </c>
+      <c r="H20" s="24">
+        <v>0</v>
+      </c>
+      <c r="I20" s="24">
+        <v>0</v>
+      </c>
+      <c r="J20" s="24">
+        <v>0</v>
+      </c>
+      <c r="K20" s="24">
         <v>5</v>
       </c>
       <c r="L20" s="17">
@@ -4946,33 +5049,33 @@
         <v>0</v>
       </c>
       <c r="AE20" s="17">
-        <v>1</v>
-      </c>
-      <c r="AF20" s="4"/>
-      <c r="AG20" s="4"/>
-      <c r="AH20" s="4"/>
-      <c r="AI20" s="4"/>
-      <c r="AJ20" s="4"/>
-      <c r="AK20" s="4"/>
-      <c r="AL20" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="AM20" s="20" t="s">
-        <v>31</v>
+        <v>0</v>
+      </c>
+      <c r="AF20" s="26"/>
+      <c r="AG20" s="26"/>
+      <c r="AH20" s="26"/>
+      <c r="AI20" s="26"/>
+      <c r="AJ20" s="26"/>
+      <c r="AK20" s="26"/>
+      <c r="AL20" s="23" t="s">
+        <v>131</v>
+      </c>
+      <c r="AM20" s="27" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="21" spans="1:39">
       <c r="A21" s="4" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="D21" s="5">
-        <v>300</v>
+        <v>80</v>
       </c>
       <c r="E21" s="11">
         <v>12</v>
@@ -4987,7 +5090,7 @@
         <v>0</v>
       </c>
       <c r="I21" s="5">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J21" s="5">
         <v>1</v>
@@ -4996,10 +5099,10 @@
         <v>5</v>
       </c>
       <c r="L21" s="17">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="M21" s="17">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="N21" s="17">
         <v>0</v>
@@ -5062,38 +5165,38 @@
       <c r="AJ21" s="4"/>
       <c r="AK21" s="4"/>
       <c r="AL21" s="4" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="AM21" s="20" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:39">
-      <c r="A22" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>13</v>
+      <c r="A22" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D22" s="5">
-        <v>200</v>
-      </c>
-      <c r="E22" s="11">
-        <v>80</v>
-      </c>
-      <c r="F22" s="5">
-        <v>2</v>
-      </c>
-      <c r="G22" s="5">
-        <v>2</v>
-      </c>
-      <c r="H22" s="5">
-        <v>0</v>
-      </c>
-      <c r="I22" s="5">
+        <v>68</v>
+      </c>
+      <c r="D22" s="3">
+        <v>50</v>
+      </c>
+      <c r="E22" s="10">
+        <v>60</v>
+      </c>
+      <c r="F22" s="3">
+        <v>3</v>
+      </c>
+      <c r="G22" s="3">
+        <v>1</v>
+      </c>
+      <c r="H22" s="3">
+        <v>0</v>
+      </c>
+      <c r="I22" s="3">
         <v>24</v>
       </c>
       <c r="J22" s="5">
@@ -5103,10 +5206,10 @@
         <v>5</v>
       </c>
       <c r="L22" s="17">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="M22" s="17">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="N22" s="17">
         <v>0</v>
@@ -5169,39 +5272,39 @@
       <c r="AJ22" s="4"/>
       <c r="AK22" s="4"/>
       <c r="AL22" s="4" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="AM22" s="20" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:39">
-      <c r="A23" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>13</v>
+      <c r="A23" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="D23" s="3">
-        <v>500</v>
-      </c>
-      <c r="E23" s="10">
-        <v>120</v>
-      </c>
-      <c r="F23" s="3">
-        <v>5</v>
-      </c>
-      <c r="G23" s="3">
+        <v>68</v>
+      </c>
+      <c r="D23" s="5">
+        <v>100</v>
+      </c>
+      <c r="E23" s="11">
+        <v>70</v>
+      </c>
+      <c r="F23" s="5">
+        <v>1</v>
+      </c>
+      <c r="G23" s="5">
         <v>2</v>
       </c>
-      <c r="H23" s="3">
-        <v>0</v>
-      </c>
-      <c r="I23" s="3">
-        <v>8</v>
+      <c r="H23" s="5">
+        <v>0</v>
+      </c>
+      <c r="I23" s="5">
+        <v>24</v>
       </c>
       <c r="J23" s="5">
         <v>0</v>
@@ -5210,10 +5313,10 @@
         <v>5</v>
       </c>
       <c r="L23" s="17">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="M23" s="17">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="N23" s="17">
         <v>0</v>
@@ -5269,47 +5372,45 @@
       <c r="AE23" s="17">
         <v>1</v>
       </c>
-      <c r="AF23" s="4">
-        <v>1</v>
-      </c>
+      <c r="AF23" s="4"/>
       <c r="AG23" s="4"/>
       <c r="AH23" s="4"/>
       <c r="AI23" s="4"/>
       <c r="AJ23" s="4"/>
       <c r="AK23" s="4"/>
       <c r="AL23" s="4" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="AM23" s="20" t="s">
-        <v>21</v>
+        <v>89</v>
       </c>
     </row>
     <row r="24" spans="1:39">
-      <c r="A24" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>13</v>
+      <c r="A24" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D24" s="5">
-        <v>300</v>
-      </c>
-      <c r="E24" s="11">
-        <v>90</v>
-      </c>
-      <c r="F24" s="5">
-        <v>2</v>
-      </c>
-      <c r="G24" s="5">
-        <v>2</v>
-      </c>
-      <c r="H24" s="5">
-        <v>0</v>
-      </c>
-      <c r="I24" s="5">
+        <v>68</v>
+      </c>
+      <c r="D24" s="3">
+        <v>100</v>
+      </c>
+      <c r="E24" s="10">
+        <v>80</v>
+      </c>
+      <c r="F24" s="3">
+        <v>1</v>
+      </c>
+      <c r="G24" s="3">
+        <v>1</v>
+      </c>
+      <c r="H24" s="3">
+        <v>0</v>
+      </c>
+      <c r="I24" s="3">
         <v>24</v>
       </c>
       <c r="J24" s="5">
@@ -5319,10 +5420,10 @@
         <v>5</v>
       </c>
       <c r="L24" s="17">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="M24" s="17">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="N24" s="17">
         <v>0</v>
@@ -5385,48 +5486,48 @@
       <c r="AJ24" s="4"/>
       <c r="AK24" s="4"/>
       <c r="AL24" s="4" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="AM24" s="20" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:39">
       <c r="A25" s="4" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="D25" s="5">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="E25" s="11">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="F25" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G25" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H25" s="5">
         <v>0</v>
       </c>
       <c r="I25" s="5">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J25" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K25" s="5">
         <v>5</v>
       </c>
       <c r="L25" s="17">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M25" s="17">
         <v>0</v>
@@ -5492,48 +5593,48 @@
       <c r="AJ25" s="4"/>
       <c r="AK25" s="4"/>
       <c r="AL25" s="4" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="AM25" s="20" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26" spans="1:39">
-      <c r="A26" s="4" t="s">
-        <v>107</v>
+      <c r="A26" s="28" t="s">
+        <v>176</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>76</v>
+        <v>12</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>68</v>
       </c>
       <c r="D26" s="5">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="E26" s="11">
-        <v>16</v>
+        <v>80</v>
       </c>
       <c r="F26" s="5">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="G26" s="5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H26" s="5">
         <v>0</v>
       </c>
       <c r="I26" s="5">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="J26" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K26" s="5">
         <v>5</v>
       </c>
       <c r="L26" s="17">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M26" s="17">
         <v>0</v>
@@ -5599,39 +5700,39 @@
       <c r="AJ26" s="4"/>
       <c r="AK26" s="4"/>
       <c r="AL26" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="AM26" s="20" t="s">
-        <v>109</v>
+        <v>130</v>
+      </c>
+      <c r="AM26" s="30" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="27" spans="1:39">
-      <c r="A27" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>108</v>
+      <c r="A27" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="D27" s="5">
-        <v>100</v>
-      </c>
-      <c r="E27" s="5">
-        <v>55</v>
-      </c>
-      <c r="F27" s="5">
-        <v>1</v>
-      </c>
-      <c r="G27" s="5">
+        <v>68</v>
+      </c>
+      <c r="D27" s="3">
+        <v>500</v>
+      </c>
+      <c r="E27" s="10">
+        <v>120</v>
+      </c>
+      <c r="F27" s="3">
+        <v>5</v>
+      </c>
+      <c r="G27" s="3">
         <v>2</v>
       </c>
-      <c r="H27" s="5">
-        <v>0</v>
-      </c>
-      <c r="I27" s="5">
-        <v>12</v>
+      <c r="H27" s="3">
+        <v>0</v>
+      </c>
+      <c r="I27" s="3">
+        <v>8</v>
       </c>
       <c r="J27" s="5">
         <v>0</v>
@@ -5640,7 +5741,7 @@
         <v>5</v>
       </c>
       <c r="L27" s="17">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="M27" s="17">
         <v>0</v>
@@ -5699,37 +5800,39 @@
       <c r="AE27" s="17">
         <v>1</v>
       </c>
-      <c r="AF27" s="4"/>
+      <c r="AF27" s="4">
+        <v>1</v>
+      </c>
       <c r="AG27" s="4"/>
       <c r="AH27" s="4"/>
       <c r="AI27" s="4"/>
       <c r="AJ27" s="4"/>
       <c r="AK27" s="4"/>
       <c r="AL27" s="4" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="AM27" s="20" t="s">
-        <v>113</v>
+        <v>17</v>
       </c>
     </row>
     <row r="28" spans="1:39">
       <c r="A28" s="4" t="s">
-        <v>111</v>
+        <v>14</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>76</v>
+        <v>12</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="D28" s="5">
-        <v>150</v>
-      </c>
-      <c r="E28" s="3">
-        <v>24</v>
+        <v>300</v>
+      </c>
+      <c r="E28" s="11">
+        <v>90</v>
       </c>
       <c r="F28" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G28" s="5">
         <v>2</v>
@@ -5738,7 +5841,7 @@
         <v>0</v>
       </c>
       <c r="I28" s="5">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="J28" s="5">
         <v>0</v>
@@ -5813,39 +5916,39 @@
       <c r="AJ28" s="4"/>
       <c r="AK28" s="4"/>
       <c r="AL28" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="AM28" s="22" t="s">
-        <v>114</v>
+        <v>130</v>
+      </c>
+      <c r="AM28" s="20" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="29" spans="1:39">
       <c r="A29" s="4" t="s">
-        <v>112</v>
+        <v>20</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>108</v>
+        <v>12</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="D29" s="5">
         <v>0</v>
       </c>
-      <c r="E29" s="5">
-        <v>110</v>
+      <c r="E29" s="11">
+        <v>0</v>
       </c>
       <c r="F29" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G29" s="5">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H29" s="5">
         <v>0</v>
       </c>
       <c r="I29" s="5">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="J29" s="5">
         <v>0</v>
@@ -5884,7 +5987,7 @@
         <v>0</v>
       </c>
       <c r="V29" s="17">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="W29" s="17">
         <v>0</v>
@@ -5920,39 +6023,39 @@
       <c r="AJ29" s="4"/>
       <c r="AK29" s="4"/>
       <c r="AL29" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="AM29" s="20" t="s">
-        <v>115</v>
+        <v>132</v>
+      </c>
+      <c r="AM29" s="30" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="30" spans="1:39">
-      <c r="A30" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D30" s="3">
-        <v>60</v>
-      </c>
-      <c r="E30" s="10">
-        <v>8</v>
-      </c>
-      <c r="F30" s="3">
-        <v>1</v>
-      </c>
-      <c r="G30" s="3">
-        <v>1</v>
-      </c>
-      <c r="H30" s="3">
-        <v>0</v>
-      </c>
-      <c r="I30" s="3">
-        <v>4</v>
+      <c r="A30" s="28" t="s">
+        <v>177</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D30" s="5">
+        <v>100</v>
+      </c>
+      <c r="E30" s="11">
+        <v>16</v>
+      </c>
+      <c r="F30" s="5">
+        <v>1</v>
+      </c>
+      <c r="G30" s="5">
+        <v>1</v>
+      </c>
+      <c r="H30" s="5">
+        <v>0</v>
+      </c>
+      <c r="I30" s="5">
+        <v>16</v>
       </c>
       <c r="J30" s="5">
         <v>1</v>
@@ -5961,7 +6064,7 @@
         <v>5</v>
       </c>
       <c r="L30" s="17">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M30" s="17">
         <v>0</v>
@@ -6027,39 +6130,39 @@
       <c r="AJ30" s="4"/>
       <c r="AK30" s="4"/>
       <c r="AL30" s="4" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="AM30" s="20" t="s">
-        <v>36</v>
+        <v>98</v>
       </c>
     </row>
     <row r="31" spans="1:39">
       <c r="A31" s="4" t="s">
-        <v>40</v>
+        <v>99</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>34</v>
+        <v>97</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="D31" s="5">
-        <v>70</v>
-      </c>
-      <c r="E31" s="11">
-        <v>720</v>
+        <v>100</v>
+      </c>
+      <c r="E31" s="5">
+        <v>55</v>
       </c>
       <c r="F31" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G31" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H31" s="5">
         <v>0</v>
       </c>
       <c r="I31" s="5">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="J31" s="5">
         <v>0</v>
@@ -6068,7 +6171,7 @@
         <v>5</v>
       </c>
       <c r="L31" s="17">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="M31" s="17">
         <v>0</v>
@@ -6134,39 +6237,39 @@
       <c r="AJ31" s="4"/>
       <c r="AK31" s="4"/>
       <c r="AL31" s="4" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="AM31" s="20" t="s">
-        <v>41</v>
+        <v>102</v>
       </c>
     </row>
     <row r="32" spans="1:39">
-      <c r="A32" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D32" s="3">
-        <v>50</v>
-      </c>
-      <c r="E32" s="10">
-        <v>720</v>
-      </c>
-      <c r="F32" s="3">
-        <v>3</v>
-      </c>
-      <c r="G32" s="3">
-        <v>1</v>
-      </c>
-      <c r="H32" s="3">
-        <v>0</v>
-      </c>
-      <c r="I32" s="3">
-        <v>72</v>
+      <c r="A32" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D32" s="5">
+        <v>150</v>
+      </c>
+      <c r="E32" s="3">
+        <v>24</v>
+      </c>
+      <c r="F32" s="5">
+        <v>1</v>
+      </c>
+      <c r="G32" s="5">
+        <v>2</v>
+      </c>
+      <c r="H32" s="5">
+        <v>0</v>
+      </c>
+      <c r="I32" s="5">
+        <v>12</v>
       </c>
       <c r="J32" s="5">
         <v>0</v>
@@ -6175,7 +6278,7 @@
         <v>5</v>
       </c>
       <c r="L32" s="17">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="M32" s="17">
         <v>0</v>
@@ -6241,33 +6344,33 @@
       <c r="AJ32" s="4"/>
       <c r="AK32" s="4"/>
       <c r="AL32" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="AM32" s="20" t="s">
-        <v>42</v>
+        <v>130</v>
+      </c>
+      <c r="AM32" s="22" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="33" spans="1:39">
       <c r="A33" s="4" t="s">
-        <v>38</v>
+        <v>101</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>34</v>
+        <v>97</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D33" s="5">
-        <v>80</v>
-      </c>
-      <c r="E33" s="11">
-        <v>100</v>
+        <v>0</v>
+      </c>
+      <c r="E33" s="5">
+        <v>110</v>
       </c>
       <c r="F33" s="5">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G33" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H33" s="5">
         <v>0</v>
@@ -6312,7 +6415,7 @@
         <v>0</v>
       </c>
       <c r="V33" s="17">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="W33" s="17">
         <v>0</v>
@@ -6341,55 +6444,55 @@
       <c r="AE33" s="17">
         <v>1</v>
       </c>
-      <c r="AF33" s="4"/>
+      <c r="AF33" s="28"/>
       <c r="AG33" s="4"/>
       <c r="AH33" s="4"/>
       <c r="AI33" s="4"/>
       <c r="AJ33" s="4"/>
       <c r="AK33" s="4"/>
       <c r="AL33" s="4" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="AM33" s="20" t="s">
-        <v>39</v>
+        <v>104</v>
       </c>
     </row>
     <row r="34" spans="1:39">
-      <c r="A34" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D34" s="3">
-        <v>0</v>
-      </c>
-      <c r="E34" s="10">
-        <v>0</v>
-      </c>
-      <c r="F34" s="3">
-        <v>0</v>
-      </c>
-      <c r="G34" s="3">
-        <v>0</v>
-      </c>
-      <c r="H34" s="3">
-        <v>0</v>
-      </c>
-      <c r="I34" s="3">
-        <v>0</v>
-      </c>
-      <c r="J34" s="5">
-        <v>0</v>
-      </c>
-      <c r="K34" s="5">
+      <c r="A34" s="23" t="s">
+        <v>152</v>
+      </c>
+      <c r="B34" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="C34" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="D34" s="24">
+        <v>30</v>
+      </c>
+      <c r="E34" s="25">
+        <v>24</v>
+      </c>
+      <c r="F34" s="24">
+        <v>1</v>
+      </c>
+      <c r="G34" s="24">
+        <v>1</v>
+      </c>
+      <c r="H34" s="24">
+        <v>0</v>
+      </c>
+      <c r="I34" s="24">
+        <v>12</v>
+      </c>
+      <c r="J34" s="24">
+        <v>1</v>
+      </c>
+      <c r="K34" s="24">
         <v>5</v>
       </c>
       <c r="L34" s="17">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="M34" s="17">
         <v>0</v>
@@ -6419,7 +6522,7 @@
         <v>0</v>
       </c>
       <c r="V34" s="17">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="W34" s="17">
         <v>0</v>
@@ -6448,53 +6551,57 @@
       <c r="AE34" s="17">
         <v>1</v>
       </c>
-      <c r="AF34" s="4"/>
-      <c r="AG34" s="4"/>
-      <c r="AH34" s="4"/>
-      <c r="AI34" s="4"/>
-      <c r="AJ34" s="4"/>
-      <c r="AK34" s="4"/>
-      <c r="AL34" s="4"/>
-      <c r="AM34" s="20" t="s">
-        <v>66</v>
+      <c r="AF34" s="26">
+        <v>1</v>
+      </c>
+      <c r="AG34" s="26"/>
+      <c r="AH34" s="26"/>
+      <c r="AI34" s="26"/>
+      <c r="AJ34" s="26"/>
+      <c r="AK34" s="26"/>
+      <c r="AL34" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="AM34" s="27" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="35" spans="1:39">
-      <c r="A35" s="4" t="s">
+      <c r="A35" t="s">
+        <v>139</v>
+      </c>
+      <c r="B35" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="C35" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="B35" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="D35" s="5">
-        <v>0</v>
-      </c>
-      <c r="E35" s="11">
-        <v>0</v>
-      </c>
-      <c r="F35" s="5">
-        <v>0</v>
-      </c>
-      <c r="G35" s="5">
-        <v>0</v>
-      </c>
-      <c r="H35" s="5">
-        <v>0</v>
-      </c>
-      <c r="I35" s="5">
-        <v>0</v>
-      </c>
-      <c r="J35" s="5">
-        <v>0</v>
-      </c>
-      <c r="K35" s="5">
+      <c r="D35" s="24">
+        <v>50</v>
+      </c>
+      <c r="E35" s="25">
+        <v>50</v>
+      </c>
+      <c r="F35" s="24">
+        <v>3</v>
+      </c>
+      <c r="G35" s="24">
+        <v>2</v>
+      </c>
+      <c r="H35" s="24">
+        <v>0</v>
+      </c>
+      <c r="I35" s="24">
+        <v>12</v>
+      </c>
+      <c r="J35" s="24">
+        <v>0</v>
+      </c>
+      <c r="K35" s="24">
         <v>5</v>
       </c>
       <c r="L35" s="17">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="M35" s="17">
         <v>0</v>
@@ -6524,7 +6631,7 @@
         <v>0</v>
       </c>
       <c r="V35" s="17">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="W35" s="17">
         <v>0</v>
@@ -6553,49 +6660,51 @@
       <c r="AE35" s="17">
         <v>1</v>
       </c>
-      <c r="AF35" s="4"/>
-      <c r="AG35" s="4"/>
-      <c r="AH35" s="4"/>
-      <c r="AI35" s="4"/>
-      <c r="AJ35" s="4"/>
-      <c r="AK35" s="4"/>
-      <c r="AL35" s="4"/>
-      <c r="AM35" s="20" t="s">
-        <v>70</v>
+      <c r="AF35" s="26"/>
+      <c r="AG35" s="26"/>
+      <c r="AH35" s="26"/>
+      <c r="AI35" s="26"/>
+      <c r="AJ35" s="26"/>
+      <c r="AK35" s="26"/>
+      <c r="AL35" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="AM35" s="27" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="36" spans="1:39">
-      <c r="A36" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D36" s="3">
-        <v>30</v>
-      </c>
-      <c r="E36" s="10">
-        <v>16</v>
-      </c>
-      <c r="F36" s="3">
-        <v>1</v>
-      </c>
-      <c r="G36" s="3">
-        <v>1</v>
-      </c>
-      <c r="H36" s="3">
-        <v>0</v>
-      </c>
-      <c r="I36" s="3">
-        <v>4</v>
-      </c>
-      <c r="J36" s="5">
-        <v>1</v>
-      </c>
-      <c r="K36" s="5">
+      <c r="A36" t="s">
+        <v>140</v>
+      </c>
+      <c r="B36" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="C36" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="D36" s="24">
+        <v>0</v>
+      </c>
+      <c r="E36" s="25">
+        <v>230</v>
+      </c>
+      <c r="F36" s="24">
+        <v>1</v>
+      </c>
+      <c r="G36" s="24">
+        <v>1</v>
+      </c>
+      <c r="H36" s="24">
+        <v>0</v>
+      </c>
+      <c r="I36" s="24">
+        <v>12</v>
+      </c>
+      <c r="J36" s="24">
+        <v>0</v>
+      </c>
+      <c r="K36" s="24">
         <v>5</v>
       </c>
       <c r="L36" s="17">
@@ -6629,7 +6738,7 @@
         <v>0</v>
       </c>
       <c r="V36" s="17">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="W36" s="17">
         <v>0</v>
@@ -6658,86 +6767,86 @@
       <c r="AE36" s="17">
         <v>1</v>
       </c>
-      <c r="AF36" s="4"/>
-      <c r="AG36" s="4"/>
-      <c r="AH36" s="4"/>
-      <c r="AI36" s="4"/>
-      <c r="AJ36" s="4"/>
-      <c r="AK36" s="4"/>
-      <c r="AL36" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="AM36" s="20" t="s">
-        <v>104</v>
+      <c r="AF36" s="26"/>
+      <c r="AG36" s="26"/>
+      <c r="AH36" s="26"/>
+      <c r="AI36" s="26"/>
+      <c r="AJ36" s="26"/>
+      <c r="AK36" s="26"/>
+      <c r="AL36" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="AM36" s="27" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="37" spans="1:39">
-      <c r="A37" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="D37" s="3">
-        <v>0</v>
-      </c>
-      <c r="E37" s="10">
-        <v>720</v>
-      </c>
-      <c r="F37" s="3">
-        <v>1</v>
-      </c>
-      <c r="G37" s="3">
-        <v>1</v>
-      </c>
-      <c r="H37" s="3">
+      <c r="A37" t="s">
+        <v>141</v>
+      </c>
+      <c r="B37" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="C37" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="D37" s="24">
+        <v>100</v>
+      </c>
+      <c r="E37" s="25">
+        <v>48</v>
+      </c>
+      <c r="F37" s="24">
+        <v>3</v>
+      </c>
+      <c r="G37" s="24">
+        <v>2</v>
+      </c>
+      <c r="H37" s="24">
+        <v>0</v>
+      </c>
+      <c r="I37" s="24">
+        <v>12</v>
+      </c>
+      <c r="J37" s="24">
+        <v>0</v>
+      </c>
+      <c r="K37" s="24">
+        <v>5</v>
+      </c>
+      <c r="L37" s="17">
+        <v>12</v>
+      </c>
+      <c r="M37" s="17">
+        <v>0</v>
+      </c>
+      <c r="N37" s="17">
+        <v>0</v>
+      </c>
+      <c r="O37" s="17">
+        <v>0</v>
+      </c>
+      <c r="P37" s="17">
+        <v>0</v>
+      </c>
+      <c r="Q37" s="17">
+        <v>0</v>
+      </c>
+      <c r="R37" s="17">
+        <v>0</v>
+      </c>
+      <c r="S37" s="17">
+        <v>0</v>
+      </c>
+      <c r="T37" s="17">
+        <v>0</v>
+      </c>
+      <c r="U37" s="17">
+        <v>0</v>
+      </c>
+      <c r="V37" s="17">
         <v>20</v>
       </c>
-      <c r="I37" s="3">
-        <v>12</v>
-      </c>
-      <c r="J37" s="5">
-        <v>1</v>
-      </c>
-      <c r="K37" s="5">
-        <v>1</v>
-      </c>
-      <c r="L37" s="17">
-        <v>0</v>
-      </c>
-      <c r="M37" s="17">
-        <v>0</v>
-      </c>
-      <c r="N37" s="17">
-        <v>0</v>
-      </c>
-      <c r="O37" s="17">
-        <v>0</v>
-      </c>
-      <c r="P37" s="17">
-        <v>0</v>
-      </c>
-      <c r="Q37" s="17">
-        <v>0</v>
-      </c>
-      <c r="R37" s="17">
-        <v>0</v>
-      </c>
-      <c r="S37" s="17">
-        <v>0</v>
-      </c>
-      <c r="T37" s="17">
-        <v>0</v>
-      </c>
-      <c r="U37" s="17">
-        <v>0</v>
-      </c>
-      <c r="V37" s="17">
-        <v>0</v>
-      </c>
       <c r="W37" s="17">
         <v>0</v>
       </c>
@@ -6765,55 +6874,55 @@
       <c r="AE37" s="17">
         <v>1</v>
       </c>
-      <c r="AF37" s="4"/>
-      <c r="AG37" s="4"/>
-      <c r="AH37" s="4"/>
-      <c r="AI37" s="4"/>
-      <c r="AJ37" s="4"/>
-      <c r="AK37" s="4"/>
-      <c r="AL37" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="AM37" s="20" t="s">
-        <v>57</v>
+      <c r="AF37" s="26"/>
+      <c r="AG37" s="26"/>
+      <c r="AH37" s="26"/>
+      <c r="AI37" s="26"/>
+      <c r="AJ37" s="26"/>
+      <c r="AK37" s="26"/>
+      <c r="AL37" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="AM37" s="27" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="38" spans="1:39">
-      <c r="A38" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="D38" s="5">
-        <v>0</v>
-      </c>
-      <c r="E38" s="11">
-        <v>0</v>
-      </c>
-      <c r="F38" s="5">
-        <v>0</v>
-      </c>
-      <c r="G38" s="5">
-        <v>0</v>
-      </c>
-      <c r="H38" s="5">
+      <c r="A38" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D38" s="3">
+        <v>60</v>
+      </c>
+      <c r="E38" s="10">
+        <v>8</v>
+      </c>
+      <c r="F38" s="3">
+        <v>1</v>
+      </c>
+      <c r="G38" s="3">
+        <v>1</v>
+      </c>
+      <c r="H38" s="3">
+        <v>0</v>
+      </c>
+      <c r="I38" s="3">
+        <v>4</v>
+      </c>
+      <c r="J38" s="5">
+        <v>1</v>
+      </c>
+      <c r="K38" s="5">
         <v>5</v>
       </c>
-      <c r="I38" s="5">
-        <v>0</v>
-      </c>
-      <c r="J38" s="5">
-        <v>1</v>
-      </c>
-      <c r="K38" s="5">
-        <v>1</v>
-      </c>
       <c r="L38" s="17">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M38" s="17">
         <v>0</v>
@@ -6878,44 +6987,46 @@
       <c r="AI38" s="4"/>
       <c r="AJ38" s="4"/>
       <c r="AK38" s="4"/>
-      <c r="AL38" s="4"/>
+      <c r="AL38" s="4" t="s">
+        <v>130</v>
+      </c>
       <c r="AM38" s="20" t="s">
-        <v>74</v>
+        <v>31</v>
       </c>
     </row>
     <row r="39" spans="1:39">
-      <c r="A39" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D39" s="3">
-        <v>0</v>
-      </c>
-      <c r="E39" s="10">
-        <v>0</v>
-      </c>
-      <c r="F39" s="3">
-        <v>0</v>
-      </c>
-      <c r="G39" s="3">
-        <v>0</v>
-      </c>
-      <c r="H39" s="3">
+      <c r="A39" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D39" s="5">
+        <v>70</v>
+      </c>
+      <c r="E39" s="11">
+        <v>720</v>
+      </c>
+      <c r="F39" s="5">
+        <v>3</v>
+      </c>
+      <c r="G39" s="5">
+        <v>3</v>
+      </c>
+      <c r="H39" s="5">
+        <v>0</v>
+      </c>
+      <c r="I39" s="5">
+        <v>4</v>
+      </c>
+      <c r="J39" s="5">
+        <v>0</v>
+      </c>
+      <c r="K39" s="5">
         <v>5</v>
-      </c>
-      <c r="I39" s="3">
-        <v>0</v>
-      </c>
-      <c r="J39" s="5">
-        <v>1</v>
-      </c>
-      <c r="K39" s="5">
-        <v>1</v>
       </c>
       <c r="L39" s="17">
         <v>0</v>
@@ -6983,44 +7094,46 @@
       <c r="AI39" s="4"/>
       <c r="AJ39" s="4"/>
       <c r="AK39" s="4"/>
-      <c r="AL39" s="4"/>
+      <c r="AL39" s="4" t="s">
+        <v>131</v>
+      </c>
       <c r="AM39" s="20" t="s">
-        <v>72</v>
+        <v>36</v>
       </c>
     </row>
     <row r="40" spans="1:39">
-      <c r="A40" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="D40" s="5">
-        <v>0</v>
-      </c>
-      <c r="E40" s="11">
-        <v>0</v>
-      </c>
-      <c r="F40" s="5">
-        <v>0</v>
-      </c>
-      <c r="G40" s="5">
-        <v>0</v>
-      </c>
-      <c r="H40" s="5">
-        <v>15</v>
-      </c>
-      <c r="I40" s="5">
-        <v>0</v>
+      <c r="A40" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D40" s="3">
+        <v>50</v>
+      </c>
+      <c r="E40" s="10">
+        <v>720</v>
+      </c>
+      <c r="F40" s="3">
+        <v>3</v>
+      </c>
+      <c r="G40" s="3">
+        <v>1</v>
+      </c>
+      <c r="H40" s="3">
+        <v>0</v>
+      </c>
+      <c r="I40" s="3">
+        <v>72</v>
       </c>
       <c r="J40" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K40" s="5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="L40" s="17">
         <v>0</v>
@@ -7088,47 +7201,49 @@
       <c r="AI40" s="4"/>
       <c r="AJ40" s="4"/>
       <c r="AK40" s="4"/>
-      <c r="AL40" s="4"/>
+      <c r="AL40" s="4" t="s">
+        <v>132</v>
+      </c>
       <c r="AM40" s="20" t="s">
-        <v>59</v>
+        <v>37</v>
       </c>
     </row>
     <row r="41" spans="1:39">
-      <c r="A41" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C41" s="2" t="s">
+      <c r="A41" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D41" s="5">
         <v>80</v>
       </c>
-      <c r="D41" s="3">
-        <v>0</v>
-      </c>
-      <c r="E41" s="10">
-        <v>0</v>
-      </c>
-      <c r="F41" s="3">
-        <v>0</v>
-      </c>
-      <c r="G41" s="3">
-        <v>0</v>
-      </c>
-      <c r="H41" s="3">
-        <v>30</v>
-      </c>
-      <c r="I41" s="3">
-        <v>0</v>
+      <c r="E41" s="11">
+        <v>100</v>
+      </c>
+      <c r="F41" s="5">
+        <v>5</v>
+      </c>
+      <c r="G41" s="5">
+        <v>2</v>
+      </c>
+      <c r="H41" s="5">
+        <v>0</v>
+      </c>
+      <c r="I41" s="5">
+        <v>12</v>
       </c>
       <c r="J41" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K41" s="5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="L41" s="17">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="M41" s="17">
         <v>0</v>
@@ -7193,44 +7308,46 @@
       <c r="AI41" s="4"/>
       <c r="AJ41" s="4"/>
       <c r="AK41" s="4"/>
-      <c r="AL41" s="4"/>
+      <c r="AL41" s="4" t="s">
+        <v>130</v>
+      </c>
       <c r="AM41" s="20" t="s">
-        <v>62</v>
+        <v>34</v>
       </c>
     </row>
     <row r="42" spans="1:39">
-      <c r="A42" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B42" s="4" t="s">
+      <c r="A42" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C42" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="D42" s="5">
-        <v>0</v>
-      </c>
-      <c r="E42" s="11">
-        <v>0</v>
-      </c>
-      <c r="F42" s="5">
-        <v>0</v>
-      </c>
-      <c r="G42" s="5">
-        <v>0</v>
-      </c>
-      <c r="H42" s="5">
-        <v>60</v>
-      </c>
-      <c r="I42" s="5">
+      <c r="B42" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D42" s="3">
+        <v>0</v>
+      </c>
+      <c r="E42" s="10">
+        <v>0</v>
+      </c>
+      <c r="F42" s="3">
+        <v>0</v>
+      </c>
+      <c r="G42" s="3">
+        <v>0</v>
+      </c>
+      <c r="H42" s="3">
+        <v>0</v>
+      </c>
+      <c r="I42" s="3">
         <v>0</v>
       </c>
       <c r="J42" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K42" s="5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="L42" s="17">
         <v>0</v>
@@ -7298,44 +7415,46 @@
       <c r="AI42" s="4"/>
       <c r="AJ42" s="4"/>
       <c r="AK42" s="4"/>
-      <c r="AL42" s="4"/>
+      <c r="AL42" s="28" t="s">
+        <v>132</v>
+      </c>
       <c r="AM42" s="20" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="43" spans="1:39">
-      <c r="A43" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D43" s="3">
-        <v>400</v>
-      </c>
-      <c r="E43" s="10">
-        <v>48</v>
-      </c>
-      <c r="F43" s="3">
-        <v>1</v>
-      </c>
-      <c r="G43" s="3">
-        <v>2</v>
-      </c>
-      <c r="H43" s="3">
-        <v>0</v>
-      </c>
-      <c r="I43" s="3">
-        <v>12</v>
+      <c r="A43" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D43" s="5">
+        <v>0</v>
+      </c>
+      <c r="E43" s="11">
+        <v>0</v>
+      </c>
+      <c r="F43" s="5">
+        <v>0</v>
+      </c>
+      <c r="G43" s="5">
+        <v>0</v>
+      </c>
+      <c r="H43" s="5">
+        <v>0</v>
+      </c>
+      <c r="I43" s="5">
+        <v>0</v>
       </c>
       <c r="J43" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K43" s="5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="L43" s="17">
         <v>0</v>
@@ -7403,114 +7522,1618 @@
       <c r="AI43" s="4"/>
       <c r="AJ43" s="4"/>
       <c r="AK43" s="4"/>
-      <c r="AL43" s="4"/>
+      <c r="AL43" s="28" t="s">
+        <v>131</v>
+      </c>
       <c r="AM43" s="20" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
     </row>
     <row r="44" spans="1:39">
-      <c r="A44" s="6" t="s">
+      <c r="A44" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D44" s="3">
+        <v>30</v>
+      </c>
+      <c r="E44" s="10">
+        <v>16</v>
+      </c>
+      <c r="F44" s="3">
+        <v>1</v>
+      </c>
+      <c r="G44" s="3">
+        <v>1</v>
+      </c>
+      <c r="H44" s="3">
+        <v>0</v>
+      </c>
+      <c r="I44" s="3">
+        <v>4</v>
+      </c>
+      <c r="J44" s="5">
+        <v>1</v>
+      </c>
+      <c r="K44" s="5">
+        <v>5</v>
+      </c>
+      <c r="L44" s="17">
+        <v>5</v>
+      </c>
+      <c r="M44" s="17">
+        <v>0</v>
+      </c>
+      <c r="N44" s="17">
+        <v>0</v>
+      </c>
+      <c r="O44" s="17">
+        <v>0</v>
+      </c>
+      <c r="P44" s="17">
+        <v>0</v>
+      </c>
+      <c r="Q44" s="17">
+        <v>0</v>
+      </c>
+      <c r="R44" s="17">
+        <v>0</v>
+      </c>
+      <c r="S44" s="17">
+        <v>0</v>
+      </c>
+      <c r="T44" s="17">
+        <v>0</v>
+      </c>
+      <c r="U44" s="17">
+        <v>0</v>
+      </c>
+      <c r="V44" s="17">
+        <v>0</v>
+      </c>
+      <c r="W44" s="17">
+        <v>0</v>
+      </c>
+      <c r="X44" s="17">
+        <v>0</v>
+      </c>
+      <c r="Y44" s="17">
+        <v>0</v>
+      </c>
+      <c r="Z44" s="17">
+        <v>0</v>
+      </c>
+      <c r="AA44" s="17">
+        <v>0</v>
+      </c>
+      <c r="AB44" s="17">
+        <v>0</v>
+      </c>
+      <c r="AC44" s="17">
+        <v>0</v>
+      </c>
+      <c r="AD44" s="17">
+        <v>0</v>
+      </c>
+      <c r="AE44" s="17">
+        <v>1</v>
+      </c>
+      <c r="AF44" s="4"/>
+      <c r="AG44" s="4"/>
+      <c r="AH44" s="4"/>
+      <c r="AI44" s="4"/>
+      <c r="AJ44" s="4"/>
+      <c r="AK44" s="4"/>
+      <c r="AL44" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="AM44" s="20" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="45" spans="1:39">
+      <c r="A45" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="B45" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D45" s="5">
+        <v>0</v>
+      </c>
+      <c r="E45" s="11">
+        <v>0</v>
+      </c>
+      <c r="F45" s="5">
+        <v>0</v>
+      </c>
+      <c r="G45" s="5">
+        <v>0</v>
+      </c>
+      <c r="H45" s="5">
+        <v>0</v>
+      </c>
+      <c r="I45" s="5">
+        <v>0</v>
+      </c>
+      <c r="J45" s="5">
+        <v>1</v>
+      </c>
+      <c r="K45" s="5">
+        <v>1</v>
+      </c>
+      <c r="L45" s="17">
+        <v>0</v>
+      </c>
+      <c r="M45" s="17">
+        <v>0</v>
+      </c>
+      <c r="N45" s="17">
+        <v>0</v>
+      </c>
+      <c r="O45" s="17">
+        <v>0</v>
+      </c>
+      <c r="P45" s="17">
+        <v>0</v>
+      </c>
+      <c r="Q45" s="17">
+        <v>0</v>
+      </c>
+      <c r="R45" s="17">
+        <v>0</v>
+      </c>
+      <c r="S45" s="17">
+        <v>0</v>
+      </c>
+      <c r="T45" s="17">
+        <v>0</v>
+      </c>
+      <c r="U45" s="17">
+        <v>0</v>
+      </c>
+      <c r="V45" s="17">
+        <v>0</v>
+      </c>
+      <c r="W45" s="17">
+        <v>0</v>
+      </c>
+      <c r="X45" s="17">
+        <v>0</v>
+      </c>
+      <c r="Y45" s="17">
+        <v>0</v>
+      </c>
+      <c r="Z45" s="17">
+        <v>0</v>
+      </c>
+      <c r="AA45" s="17">
+        <v>0</v>
+      </c>
+      <c r="AB45" s="17">
+        <v>0</v>
+      </c>
+      <c r="AC45" s="17">
+        <v>0</v>
+      </c>
+      <c r="AD45" s="17">
+        <v>0</v>
+      </c>
+      <c r="AE45" s="17">
+        <v>1</v>
+      </c>
+      <c r="AF45" s="4"/>
+      <c r="AG45" s="4"/>
+      <c r="AH45" s="4"/>
+      <c r="AI45" s="4"/>
+      <c r="AJ45" s="4"/>
+      <c r="AK45" s="4"/>
+      <c r="AL45" s="28" t="s">
+        <v>131</v>
+      </c>
+      <c r="AM45" s="27" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="46" spans="1:39">
+      <c r="A46" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="B46" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="C46" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="D46" s="24">
+        <v>800</v>
+      </c>
+      <c r="E46" s="25">
+        <v>12</v>
+      </c>
+      <c r="F46" s="24">
+        <v>1</v>
+      </c>
+      <c r="G46" s="24">
+        <v>2</v>
+      </c>
+      <c r="H46" s="24">
+        <v>0</v>
+      </c>
+      <c r="I46" s="24">
+        <v>12</v>
+      </c>
+      <c r="J46" s="5">
+        <v>0</v>
+      </c>
+      <c r="K46" s="5">
+        <v>5</v>
+      </c>
+      <c r="L46" s="17">
+        <v>5</v>
+      </c>
+      <c r="M46" s="17">
+        <v>0</v>
+      </c>
+      <c r="N46" s="17">
+        <v>0</v>
+      </c>
+      <c r="O46" s="17">
+        <v>0</v>
+      </c>
+      <c r="P46" s="17">
+        <v>0</v>
+      </c>
+      <c r="Q46" s="17">
+        <v>0</v>
+      </c>
+      <c r="R46" s="17">
+        <v>0</v>
+      </c>
+      <c r="S46" s="17">
+        <v>0</v>
+      </c>
+      <c r="T46" s="17">
+        <v>0</v>
+      </c>
+      <c r="U46" s="17">
+        <v>0</v>
+      </c>
+      <c r="V46" s="17">
+        <v>0</v>
+      </c>
+      <c r="W46" s="17">
+        <v>0</v>
+      </c>
+      <c r="X46" s="17">
+        <v>0</v>
+      </c>
+      <c r="Y46" s="17">
+        <v>0</v>
+      </c>
+      <c r="Z46" s="17">
+        <v>0</v>
+      </c>
+      <c r="AA46" s="17">
+        <v>0</v>
+      </c>
+      <c r="AB46" s="17">
+        <v>0</v>
+      </c>
+      <c r="AC46" s="17">
+        <v>0</v>
+      </c>
+      <c r="AD46" s="17">
+        <v>0</v>
+      </c>
+      <c r="AE46" s="17">
+        <v>1</v>
+      </c>
+      <c r="AF46" s="26"/>
+      <c r="AG46" s="26"/>
+      <c r="AH46" s="26"/>
+      <c r="AI46" s="26"/>
+      <c r="AJ46" s="26"/>
+      <c r="AK46" s="26"/>
+      <c r="AL46" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="AM46" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="47" spans="1:39">
+      <c r="A47" s="23" t="s">
+        <v>136</v>
+      </c>
+      <c r="B47" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="C47" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="D47" s="24">
+        <v>100</v>
+      </c>
+      <c r="E47" s="25">
+        <v>64</v>
+      </c>
+      <c r="F47" s="24">
+        <v>10</v>
+      </c>
+      <c r="G47" s="24">
+        <v>4</v>
+      </c>
+      <c r="H47" s="24">
+        <v>0</v>
+      </c>
+      <c r="I47" s="24">
+        <v>1</v>
+      </c>
+      <c r="J47" s="5">
+        <v>0</v>
+      </c>
+      <c r="K47" s="5">
+        <v>5</v>
+      </c>
+      <c r="L47" s="17">
+        <v>15</v>
+      </c>
+      <c r="M47" s="17">
+        <v>0</v>
+      </c>
+      <c r="N47" s="17">
+        <v>0</v>
+      </c>
+      <c r="O47" s="17">
+        <v>0</v>
+      </c>
+      <c r="P47" s="17">
+        <v>0</v>
+      </c>
+      <c r="Q47" s="17">
+        <v>0</v>
+      </c>
+      <c r="R47" s="17">
+        <v>0</v>
+      </c>
+      <c r="S47" s="17">
+        <v>0</v>
+      </c>
+      <c r="T47" s="17">
+        <v>0</v>
+      </c>
+      <c r="U47" s="17">
+        <v>0</v>
+      </c>
+      <c r="V47" s="17">
+        <v>0</v>
+      </c>
+      <c r="W47" s="17">
+        <v>0</v>
+      </c>
+      <c r="X47" s="17">
+        <v>0</v>
+      </c>
+      <c r="Y47" s="17">
+        <v>0</v>
+      </c>
+      <c r="Z47" s="17">
+        <v>0</v>
+      </c>
+      <c r="AA47" s="17">
+        <v>0</v>
+      </c>
+      <c r="AB47" s="17">
+        <v>0</v>
+      </c>
+      <c r="AC47" s="17">
+        <v>0</v>
+      </c>
+      <c r="AD47" s="17">
+        <v>0</v>
+      </c>
+      <c r="AE47" s="17">
+        <v>1</v>
+      </c>
+      <c r="AF47" s="26"/>
+      <c r="AG47" s="26"/>
+      <c r="AH47" s="26"/>
+      <c r="AI47" s="26"/>
+      <c r="AJ47" s="26"/>
+      <c r="AK47" s="26"/>
+      <c r="AL47" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="AM47" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="48" spans="1:39">
+      <c r="A48" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="B48" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="C48" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="D48" s="24">
+        <v>300</v>
+      </c>
+      <c r="E48" s="25">
+        <v>16</v>
+      </c>
+      <c r="F48" s="24">
+        <v>10</v>
+      </c>
+      <c r="G48" s="24">
+        <v>4</v>
+      </c>
+      <c r="H48" s="24">
+        <v>0</v>
+      </c>
+      <c r="I48" s="24">
+        <v>1</v>
+      </c>
+      <c r="J48" s="24">
+        <v>1</v>
+      </c>
+      <c r="K48" s="24">
+        <v>5</v>
+      </c>
+      <c r="L48" s="17">
+        <v>3</v>
+      </c>
+      <c r="M48" s="17">
+        <v>0</v>
+      </c>
+      <c r="N48" s="17">
+        <v>0</v>
+      </c>
+      <c r="O48" s="17">
+        <v>0</v>
+      </c>
+      <c r="P48" s="17">
+        <v>0</v>
+      </c>
+      <c r="Q48" s="17">
+        <v>0</v>
+      </c>
+      <c r="R48" s="17">
+        <v>0</v>
+      </c>
+      <c r="S48" s="17">
+        <v>0</v>
+      </c>
+      <c r="T48" s="17">
+        <v>0</v>
+      </c>
+      <c r="U48" s="17">
+        <v>0</v>
+      </c>
+      <c r="V48" s="17">
+        <v>0</v>
+      </c>
+      <c r="W48" s="17">
+        <v>0</v>
+      </c>
+      <c r="X48" s="17">
+        <v>0</v>
+      </c>
+      <c r="Y48" s="17">
+        <v>0</v>
+      </c>
+      <c r="Z48" s="17">
+        <v>0</v>
+      </c>
+      <c r="AA48" s="17">
+        <v>0</v>
+      </c>
+      <c r="AB48" s="17">
+        <v>0</v>
+      </c>
+      <c r="AC48" s="17">
+        <v>0</v>
+      </c>
+      <c r="AD48" s="17">
+        <v>0</v>
+      </c>
+      <c r="AE48" s="17">
+        <v>1</v>
+      </c>
+      <c r="AF48" s="26"/>
+      <c r="AG48" s="26"/>
+      <c r="AH48" s="26"/>
+      <c r="AI48" s="26"/>
+      <c r="AJ48" s="26"/>
+      <c r="AK48" s="26"/>
+      <c r="AL48" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="AM48" s="27" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="49" spans="1:39">
+      <c r="A49" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="B49" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="C49" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="D49" s="24">
+        <v>100</v>
+      </c>
+      <c r="E49" s="25">
+        <v>72</v>
+      </c>
+      <c r="F49" s="24">
+        <v>3</v>
+      </c>
+      <c r="G49" s="24">
+        <v>1</v>
+      </c>
+      <c r="H49" s="24">
+        <v>0</v>
+      </c>
+      <c r="I49" s="24">
+        <v>16</v>
+      </c>
+      <c r="J49" s="24">
+        <v>0</v>
+      </c>
+      <c r="K49" s="24">
+        <v>5</v>
+      </c>
+      <c r="L49" s="17">
+        <v>25</v>
+      </c>
+      <c r="M49" s="17">
+        <v>0</v>
+      </c>
+      <c r="N49" s="17">
+        <v>0</v>
+      </c>
+      <c r="O49" s="17">
+        <v>0</v>
+      </c>
+      <c r="P49" s="17">
+        <v>0</v>
+      </c>
+      <c r="Q49" s="17">
+        <v>0</v>
+      </c>
+      <c r="R49" s="17">
+        <v>0</v>
+      </c>
+      <c r="S49" s="17">
+        <v>0</v>
+      </c>
+      <c r="T49" s="17">
+        <v>0</v>
+      </c>
+      <c r="U49" s="17">
+        <v>0</v>
+      </c>
+      <c r="V49" s="17">
+        <v>0</v>
+      </c>
+      <c r="W49" s="17">
+        <v>0</v>
+      </c>
+      <c r="X49" s="17">
+        <v>0</v>
+      </c>
+      <c r="Y49" s="17">
+        <v>0</v>
+      </c>
+      <c r="Z49" s="17">
+        <v>0</v>
+      </c>
+      <c r="AA49" s="17">
+        <v>0</v>
+      </c>
+      <c r="AB49" s="17">
+        <v>0</v>
+      </c>
+      <c r="AC49" s="17">
+        <v>0</v>
+      </c>
+      <c r="AD49" s="17">
+        <v>0</v>
+      </c>
+      <c r="AE49" s="17">
+        <v>1</v>
+      </c>
+      <c r="AF49" s="26"/>
+      <c r="AG49" s="26"/>
+      <c r="AH49" s="26"/>
+      <c r="AI49" s="26"/>
+      <c r="AJ49" s="26"/>
+      <c r="AK49" s="26"/>
+      <c r="AL49" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="AM49" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="50" spans="1:39">
+      <c r="A50" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="B50" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="C50" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="D50" s="24">
+        <v>50</v>
+      </c>
+      <c r="E50" s="25">
+        <v>48</v>
+      </c>
+      <c r="F50" s="24">
+        <v>1</v>
+      </c>
+      <c r="G50" s="24">
+        <v>2</v>
+      </c>
+      <c r="H50" s="24">
+        <v>0</v>
+      </c>
+      <c r="I50" s="24">
+        <v>12</v>
+      </c>
+      <c r="J50" s="24">
+        <v>0</v>
+      </c>
+      <c r="K50" s="24">
+        <v>5</v>
+      </c>
+      <c r="L50" s="17">
+        <v>5</v>
+      </c>
+      <c r="M50" s="17">
+        <v>0</v>
+      </c>
+      <c r="N50" s="17">
+        <v>0</v>
+      </c>
+      <c r="O50" s="17">
+        <v>0</v>
+      </c>
+      <c r="P50" s="17">
+        <v>0</v>
+      </c>
+      <c r="Q50" s="17">
+        <v>0</v>
+      </c>
+      <c r="R50" s="17">
+        <v>0</v>
+      </c>
+      <c r="S50" s="17">
+        <v>0</v>
+      </c>
+      <c r="T50" s="17">
+        <v>0</v>
+      </c>
+      <c r="U50" s="17">
+        <v>0</v>
+      </c>
+      <c r="V50" s="17">
+        <v>0</v>
+      </c>
+      <c r="W50" s="17">
+        <v>0</v>
+      </c>
+      <c r="X50" s="17">
+        <v>0</v>
+      </c>
+      <c r="Y50" s="17">
+        <v>0</v>
+      </c>
+      <c r="Z50" s="17">
+        <v>0</v>
+      </c>
+      <c r="AA50" s="17">
+        <v>0</v>
+      </c>
+      <c r="AB50" s="17">
+        <v>0</v>
+      </c>
+      <c r="AC50" s="17">
+        <v>0</v>
+      </c>
+      <c r="AD50" s="17">
+        <v>0</v>
+      </c>
+      <c r="AE50" s="17">
+        <v>1</v>
+      </c>
+      <c r="AF50" s="26"/>
+      <c r="AG50" s="26"/>
+      <c r="AH50" s="26"/>
+      <c r="AI50" s="26"/>
+      <c r="AJ50" s="26"/>
+      <c r="AK50" s="26"/>
+      <c r="AL50" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="AM50" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="51" spans="1:39">
+      <c r="A51" s="23" t="s">
+        <v>150</v>
+      </c>
+      <c r="B51" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="C51" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="D51" s="24">
+        <v>80</v>
+      </c>
+      <c r="E51" s="25">
+        <v>120</v>
+      </c>
+      <c r="F51" s="24">
+        <v>1</v>
+      </c>
+      <c r="G51" s="24">
+        <v>1</v>
+      </c>
+      <c r="H51" s="24">
+        <v>0</v>
+      </c>
+      <c r="I51" s="24">
+        <v>12</v>
+      </c>
+      <c r="J51" s="24">
+        <v>0</v>
+      </c>
+      <c r="K51" s="24">
+        <v>5</v>
+      </c>
+      <c r="L51" s="17">
+        <v>40</v>
+      </c>
+      <c r="M51" s="17">
+        <v>0</v>
+      </c>
+      <c r="N51" s="17">
+        <v>0</v>
+      </c>
+      <c r="O51" s="17">
+        <v>0</v>
+      </c>
+      <c r="P51" s="17">
+        <v>0</v>
+      </c>
+      <c r="Q51" s="17">
+        <v>0</v>
+      </c>
+      <c r="R51" s="17">
+        <v>0</v>
+      </c>
+      <c r="S51" s="17">
+        <v>0</v>
+      </c>
+      <c r="T51" s="17">
+        <v>0</v>
+      </c>
+      <c r="U51" s="17">
+        <v>0</v>
+      </c>
+      <c r="V51" s="17">
+        <v>0</v>
+      </c>
+      <c r="W51" s="17">
+        <v>0</v>
+      </c>
+      <c r="X51" s="17">
+        <v>0</v>
+      </c>
+      <c r="Y51" s="17">
+        <v>0</v>
+      </c>
+      <c r="Z51" s="17">
+        <v>0</v>
+      </c>
+      <c r="AA51" s="17">
+        <v>0</v>
+      </c>
+      <c r="AB51" s="17">
+        <v>0</v>
+      </c>
+      <c r="AC51" s="17">
+        <v>0</v>
+      </c>
+      <c r="AD51" s="17">
+        <v>0</v>
+      </c>
+      <c r="AE51" s="17">
+        <v>1</v>
+      </c>
+      <c r="AF51" s="26">
+        <v>1</v>
+      </c>
+      <c r="AG51" s="26"/>
+      <c r="AH51" s="26"/>
+      <c r="AI51" s="26"/>
+      <c r="AJ51" s="26"/>
+      <c r="AK51" s="26"/>
+      <c r="AL51" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="AM51" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="52" spans="1:39">
+      <c r="A52" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D52" s="3">
+        <v>0</v>
+      </c>
+      <c r="E52" s="10">
+        <v>720</v>
+      </c>
+      <c r="F52" s="3">
+        <v>1</v>
+      </c>
+      <c r="G52" s="3">
+        <v>1</v>
+      </c>
+      <c r="H52" s="3">
+        <v>20</v>
+      </c>
+      <c r="I52" s="3">
+        <v>12</v>
+      </c>
+      <c r="J52" s="5">
+        <v>1</v>
+      </c>
+      <c r="K52" s="5">
+        <v>1</v>
+      </c>
+      <c r="L52" s="17">
+        <v>0</v>
+      </c>
+      <c r="M52" s="17">
+        <v>0</v>
+      </c>
+      <c r="N52" s="17">
+        <v>0</v>
+      </c>
+      <c r="O52" s="17">
+        <v>0</v>
+      </c>
+      <c r="P52" s="17">
+        <v>0</v>
+      </c>
+      <c r="Q52" s="17">
+        <v>0</v>
+      </c>
+      <c r="R52" s="17">
+        <v>0</v>
+      </c>
+      <c r="S52" s="17">
+        <v>0</v>
+      </c>
+      <c r="T52" s="17">
+        <v>0</v>
+      </c>
+      <c r="U52" s="17">
+        <v>0</v>
+      </c>
+      <c r="V52" s="17">
+        <v>0</v>
+      </c>
+      <c r="W52" s="17">
+        <v>0</v>
+      </c>
+      <c r="X52" s="17">
+        <v>0</v>
+      </c>
+      <c r="Y52" s="17">
+        <v>0</v>
+      </c>
+      <c r="Z52" s="17">
+        <v>0</v>
+      </c>
+      <c r="AA52" s="17">
+        <v>0</v>
+      </c>
+      <c r="AB52" s="17">
+        <v>0</v>
+      </c>
+      <c r="AC52" s="17">
+        <v>0</v>
+      </c>
+      <c r="AD52" s="17">
+        <v>0</v>
+      </c>
+      <c r="AE52" s="17">
+        <v>1</v>
+      </c>
+      <c r="AF52" s="4"/>
+      <c r="AG52" s="4"/>
+      <c r="AH52" s="4"/>
+      <c r="AI52" s="4"/>
+      <c r="AJ52" s="4"/>
+      <c r="AK52" s="4"/>
+      <c r="AL52" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="AM52" s="20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:39">
+      <c r="A53" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D53" s="5">
+        <v>0</v>
+      </c>
+      <c r="E53" s="11">
+        <v>0</v>
+      </c>
+      <c r="F53" s="5">
+        <v>0</v>
+      </c>
+      <c r="G53" s="5">
+        <v>0</v>
+      </c>
+      <c r="H53" s="5">
+        <v>5</v>
+      </c>
+      <c r="I53" s="5">
+        <v>0</v>
+      </c>
+      <c r="J53" s="5">
+        <v>1</v>
+      </c>
+      <c r="K53" s="5">
+        <v>1</v>
+      </c>
+      <c r="L53" s="17">
+        <v>0</v>
+      </c>
+      <c r="M53" s="17">
+        <v>0</v>
+      </c>
+      <c r="N53" s="17">
+        <v>0</v>
+      </c>
+      <c r="O53" s="17">
+        <v>0</v>
+      </c>
+      <c r="P53" s="17">
+        <v>0</v>
+      </c>
+      <c r="Q53" s="17">
+        <v>0</v>
+      </c>
+      <c r="R53" s="17">
+        <v>0</v>
+      </c>
+      <c r="S53" s="17">
+        <v>0</v>
+      </c>
+      <c r="T53" s="17">
+        <v>0</v>
+      </c>
+      <c r="U53" s="17">
+        <v>0</v>
+      </c>
+      <c r="V53" s="17">
+        <v>0</v>
+      </c>
+      <c r="W53" s="17">
+        <v>0</v>
+      </c>
+      <c r="X53" s="17">
+        <v>0</v>
+      </c>
+      <c r="Y53" s="17">
+        <v>0</v>
+      </c>
+      <c r="Z53" s="17">
+        <v>0</v>
+      </c>
+      <c r="AA53" s="17">
+        <v>0</v>
+      </c>
+      <c r="AB53" s="17">
+        <v>0</v>
+      </c>
+      <c r="AC53" s="17">
+        <v>0</v>
+      </c>
+      <c r="AD53" s="17">
+        <v>0</v>
+      </c>
+      <c r="AE53" s="17">
+        <v>1</v>
+      </c>
+      <c r="AF53" s="4"/>
+      <c r="AG53" s="4"/>
+      <c r="AH53" s="4"/>
+      <c r="AI53" s="4"/>
+      <c r="AJ53" s="4"/>
+      <c r="AK53" s="4"/>
+      <c r="AL53" s="28" t="s">
+        <v>131</v>
+      </c>
+      <c r="AM53" s="20" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="54" spans="1:39">
+      <c r="A54" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D54" s="3">
+        <v>0</v>
+      </c>
+      <c r="E54" s="10">
+        <v>0</v>
+      </c>
+      <c r="F54" s="3">
+        <v>0</v>
+      </c>
+      <c r="G54" s="3">
+        <v>0</v>
+      </c>
+      <c r="H54" s="3">
+        <v>5</v>
+      </c>
+      <c r="I54" s="3">
+        <v>0</v>
+      </c>
+      <c r="J54" s="5">
+        <v>1</v>
+      </c>
+      <c r="K54" s="5">
+        <v>1</v>
+      </c>
+      <c r="L54" s="17">
+        <v>0</v>
+      </c>
+      <c r="M54" s="17">
+        <v>0</v>
+      </c>
+      <c r="N54" s="17">
+        <v>0</v>
+      </c>
+      <c r="O54" s="17">
+        <v>0</v>
+      </c>
+      <c r="P54" s="17">
+        <v>0</v>
+      </c>
+      <c r="Q54" s="17">
+        <v>0</v>
+      </c>
+      <c r="R54" s="17">
+        <v>0</v>
+      </c>
+      <c r="S54" s="17">
+        <v>0</v>
+      </c>
+      <c r="T54" s="17">
+        <v>0</v>
+      </c>
+      <c r="U54" s="17">
+        <v>0</v>
+      </c>
+      <c r="V54" s="17">
+        <v>0</v>
+      </c>
+      <c r="W54" s="17">
+        <v>0</v>
+      </c>
+      <c r="X54" s="17">
+        <v>0</v>
+      </c>
+      <c r="Y54" s="17">
+        <v>0</v>
+      </c>
+      <c r="Z54" s="17">
+        <v>0</v>
+      </c>
+      <c r="AA54" s="17">
+        <v>0</v>
+      </c>
+      <c r="AB54" s="17">
+        <v>0</v>
+      </c>
+      <c r="AC54" s="17">
+        <v>0</v>
+      </c>
+      <c r="AD54" s="17">
+        <v>0</v>
+      </c>
+      <c r="AE54" s="17">
+        <v>1</v>
+      </c>
+      <c r="AF54" s="4"/>
+      <c r="AG54" s="4"/>
+      <c r="AH54" s="4"/>
+      <c r="AI54" s="4"/>
+      <c r="AJ54" s="4"/>
+      <c r="AK54" s="4"/>
+      <c r="AL54" s="28" t="s">
+        <v>131</v>
+      </c>
+      <c r="AM54" s="20" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="55" spans="1:39">
+      <c r="A55" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="B44" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="C44" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="D44" s="7">
+      <c r="B55" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D55" s="3">
+        <v>0</v>
+      </c>
+      <c r="E55" s="10">
+        <v>0</v>
+      </c>
+      <c r="F55" s="3">
+        <v>0</v>
+      </c>
+      <c r="G55" s="3">
+        <v>0</v>
+      </c>
+      <c r="H55" s="3">
+        <v>30</v>
+      </c>
+      <c r="I55" s="3">
+        <v>0</v>
+      </c>
+      <c r="J55" s="5">
+        <v>1</v>
+      </c>
+      <c r="K55" s="5">
+        <v>1</v>
+      </c>
+      <c r="L55" s="17">
+        <v>0</v>
+      </c>
+      <c r="M55" s="17">
+        <v>0</v>
+      </c>
+      <c r="N55" s="17">
+        <v>0</v>
+      </c>
+      <c r="O55" s="17">
+        <v>0</v>
+      </c>
+      <c r="P55" s="17">
+        <v>0</v>
+      </c>
+      <c r="Q55" s="17">
+        <v>0</v>
+      </c>
+      <c r="R55" s="17">
+        <v>0</v>
+      </c>
+      <c r="S55" s="17">
+        <v>0</v>
+      </c>
+      <c r="T55" s="17">
+        <v>0</v>
+      </c>
+      <c r="U55" s="17">
+        <v>0</v>
+      </c>
+      <c r="V55" s="17">
+        <v>0</v>
+      </c>
+      <c r="W55" s="17">
+        <v>0</v>
+      </c>
+      <c r="X55" s="17">
+        <v>0</v>
+      </c>
+      <c r="Y55" s="17">
+        <v>0</v>
+      </c>
+      <c r="Z55" s="17">
+        <v>0</v>
+      </c>
+      <c r="AA55" s="17">
+        <v>0</v>
+      </c>
+      <c r="AB55" s="17">
+        <v>0</v>
+      </c>
+      <c r="AC55" s="17">
+        <v>0</v>
+      </c>
+      <c r="AD55" s="17">
+        <v>0</v>
+      </c>
+      <c r="AE55" s="17">
+        <v>1</v>
+      </c>
+      <c r="AF55" s="4"/>
+      <c r="AG55" s="4"/>
+      <c r="AH55" s="4"/>
+      <c r="AI55" s="4"/>
+      <c r="AJ55" s="4"/>
+      <c r="AK55" s="4"/>
+      <c r="AL55" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="AM55" s="20" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:39">
+      <c r="A56" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D56" s="5">
+        <v>0</v>
+      </c>
+      <c r="E56" s="11">
+        <v>0</v>
+      </c>
+      <c r="F56" s="5">
+        <v>0</v>
+      </c>
+      <c r="G56" s="5">
+        <v>0</v>
+      </c>
+      <c r="H56" s="5">
+        <v>60</v>
+      </c>
+      <c r="I56" s="5">
+        <v>0</v>
+      </c>
+      <c r="J56" s="5">
+        <v>1</v>
+      </c>
+      <c r="K56" s="5">
+        <v>1</v>
+      </c>
+      <c r="L56" s="17">
+        <v>0</v>
+      </c>
+      <c r="M56" s="17">
+        <v>0</v>
+      </c>
+      <c r="N56" s="17">
+        <v>0</v>
+      </c>
+      <c r="O56" s="17">
+        <v>0</v>
+      </c>
+      <c r="P56" s="17">
+        <v>0</v>
+      </c>
+      <c r="Q56" s="17">
+        <v>0</v>
+      </c>
+      <c r="R56" s="17">
+        <v>0</v>
+      </c>
+      <c r="S56" s="17">
+        <v>0</v>
+      </c>
+      <c r="T56" s="17">
+        <v>0</v>
+      </c>
+      <c r="U56" s="17">
+        <v>0</v>
+      </c>
+      <c r="V56" s="17">
+        <v>0</v>
+      </c>
+      <c r="W56" s="17">
+        <v>0</v>
+      </c>
+      <c r="X56" s="17">
+        <v>0</v>
+      </c>
+      <c r="Y56" s="17">
+        <v>0</v>
+      </c>
+      <c r="Z56" s="17">
+        <v>0</v>
+      </c>
+      <c r="AA56" s="17">
+        <v>0</v>
+      </c>
+      <c r="AB56" s="17">
+        <v>0</v>
+      </c>
+      <c r="AC56" s="17">
+        <v>0</v>
+      </c>
+      <c r="AD56" s="17">
+        <v>0</v>
+      </c>
+      <c r="AE56" s="17">
+        <v>1</v>
+      </c>
+      <c r="AF56" s="4"/>
+      <c r="AG56" s="4"/>
+      <c r="AH56" s="4"/>
+      <c r="AI56" s="4"/>
+      <c r="AJ56" s="4"/>
+      <c r="AK56" s="4"/>
+      <c r="AL56" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="AM56" s="20" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:39">
+      <c r="A57" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D57" s="3">
         <v>400</v>
       </c>
-      <c r="E44" s="12">
+      <c r="E57" s="10">
         <v>48</v>
       </c>
-      <c r="F44" s="7">
-        <v>1</v>
-      </c>
-      <c r="G44" s="7">
+      <c r="F57" s="3">
+        <v>1</v>
+      </c>
+      <c r="G57" s="3">
         <v>2</v>
       </c>
-      <c r="H44" s="7">
-        <v>0</v>
-      </c>
-      <c r="I44" s="7">
+      <c r="H57" s="3">
+        <v>0</v>
+      </c>
+      <c r="I57" s="3">
         <v>12</v>
       </c>
-      <c r="J44" s="7">
-        <v>1</v>
-      </c>
-      <c r="K44" s="7">
-        <v>1</v>
-      </c>
-      <c r="L44" s="18">
-        <v>0</v>
-      </c>
-      <c r="M44" s="17">
-        <v>0</v>
-      </c>
-      <c r="N44" s="17">
-        <v>0</v>
-      </c>
-      <c r="O44" s="17">
-        <v>0</v>
-      </c>
-      <c r="P44" s="17">
-        <v>0</v>
-      </c>
-      <c r="Q44" s="17">
-        <v>0</v>
-      </c>
-      <c r="R44" s="17">
-        <v>0</v>
-      </c>
-      <c r="S44" s="17">
-        <v>0</v>
-      </c>
-      <c r="T44" s="17">
-        <v>0</v>
-      </c>
-      <c r="U44" s="17">
-        <v>0</v>
-      </c>
-      <c r="V44" s="17">
-        <v>0</v>
-      </c>
-      <c r="W44" s="17">
-        <v>0</v>
-      </c>
-      <c r="X44" s="17">
-        <v>0</v>
-      </c>
-      <c r="Y44" s="17">
-        <v>0</v>
-      </c>
-      <c r="Z44" s="17">
-        <v>0</v>
-      </c>
-      <c r="AA44" s="17">
-        <v>0</v>
-      </c>
-      <c r="AB44" s="17">
-        <v>0</v>
-      </c>
-      <c r="AC44" s="17">
-        <v>0</v>
-      </c>
-      <c r="AD44" s="17">
-        <v>0</v>
-      </c>
-      <c r="AE44" s="18">
-        <v>1</v>
-      </c>
-      <c r="AF44" s="6"/>
-      <c r="AG44" s="6"/>
-      <c r="AH44" s="6"/>
-      <c r="AI44" s="6"/>
-      <c r="AJ44" s="6"/>
-      <c r="AK44" s="6"/>
-      <c r="AL44" s="6"/>
-      <c r="AM44" s="21" t="s">
-        <v>54</v>
+      <c r="J57" s="5">
+        <v>1</v>
+      </c>
+      <c r="K57" s="5">
+        <v>1</v>
+      </c>
+      <c r="L57" s="17">
+        <v>20</v>
+      </c>
+      <c r="M57" s="17">
+        <v>0</v>
+      </c>
+      <c r="N57" s="17">
+        <v>0</v>
+      </c>
+      <c r="O57" s="17">
+        <v>0</v>
+      </c>
+      <c r="P57" s="17">
+        <v>0</v>
+      </c>
+      <c r="Q57" s="17">
+        <v>0</v>
+      </c>
+      <c r="R57" s="17">
+        <v>0</v>
+      </c>
+      <c r="S57" s="17">
+        <v>0</v>
+      </c>
+      <c r="T57" s="17">
+        <v>0</v>
+      </c>
+      <c r="U57" s="17">
+        <v>0</v>
+      </c>
+      <c r="V57" s="17">
+        <v>0</v>
+      </c>
+      <c r="W57" s="17">
+        <v>0</v>
+      </c>
+      <c r="X57" s="17">
+        <v>0</v>
+      </c>
+      <c r="Y57" s="17">
+        <v>0</v>
+      </c>
+      <c r="Z57" s="17">
+        <v>0</v>
+      </c>
+      <c r="AA57" s="17">
+        <v>0</v>
+      </c>
+      <c r="AB57" s="17">
+        <v>0</v>
+      </c>
+      <c r="AC57" s="17">
+        <v>0</v>
+      </c>
+      <c r="AD57" s="17">
+        <v>0</v>
+      </c>
+      <c r="AE57" s="17">
+        <v>1</v>
+      </c>
+      <c r="AF57" s="4"/>
+      <c r="AG57" s="4"/>
+      <c r="AH57" s="4"/>
+      <c r="AI57" s="4"/>
+      <c r="AJ57" s="4"/>
+      <c r="AK57" s="4"/>
+      <c r="AL57" s="28" t="s">
+        <v>130</v>
+      </c>
+      <c r="AM57" s="20" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="58" spans="1:39">
+      <c r="A58" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B58" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C58" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D58" s="7">
+        <v>400</v>
+      </c>
+      <c r="E58" s="12">
+        <v>48</v>
+      </c>
+      <c r="F58" s="7">
+        <v>1</v>
+      </c>
+      <c r="G58" s="7">
+        <v>2</v>
+      </c>
+      <c r="H58" s="7">
+        <v>0</v>
+      </c>
+      <c r="I58" s="7">
+        <v>12</v>
+      </c>
+      <c r="J58" s="7">
+        <v>1</v>
+      </c>
+      <c r="K58" s="7">
+        <v>1</v>
+      </c>
+      <c r="L58" s="18">
+        <v>40</v>
+      </c>
+      <c r="M58" s="17">
+        <v>0</v>
+      </c>
+      <c r="N58" s="17">
+        <v>0</v>
+      </c>
+      <c r="O58" s="17">
+        <v>0</v>
+      </c>
+      <c r="P58" s="17">
+        <v>0</v>
+      </c>
+      <c r="Q58" s="17">
+        <v>0</v>
+      </c>
+      <c r="R58" s="17">
+        <v>0</v>
+      </c>
+      <c r="S58" s="17">
+        <v>0</v>
+      </c>
+      <c r="T58" s="17">
+        <v>0</v>
+      </c>
+      <c r="U58" s="17">
+        <v>0</v>
+      </c>
+      <c r="V58" s="17">
+        <v>0</v>
+      </c>
+      <c r="W58" s="17">
+        <v>0</v>
+      </c>
+      <c r="X58" s="17">
+        <v>0</v>
+      </c>
+      <c r="Y58" s="17">
+        <v>0</v>
+      </c>
+      <c r="Z58" s="17">
+        <v>0</v>
+      </c>
+      <c r="AA58" s="17">
+        <v>0</v>
+      </c>
+      <c r="AB58" s="17">
+        <v>0</v>
+      </c>
+      <c r="AC58" s="17">
+        <v>0</v>
+      </c>
+      <c r="AD58" s="17">
+        <v>0</v>
+      </c>
+      <c r="AE58" s="18">
+        <v>1</v>
+      </c>
+      <c r="AF58" s="6"/>
+      <c r="AG58" s="6"/>
+      <c r="AH58" s="6"/>
+      <c r="AI58" s="6"/>
+      <c r="AJ58" s="6"/>
+      <c r="AK58" s="6"/>
+      <c r="AL58" s="31" t="s">
+        <v>130</v>
+      </c>
+      <c r="AM58" s="21" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
I kinda just made small random not very important changes.
</commit_message>
<xml_diff>
--- a/xml/Abilities.xlsx
+++ b/xml/Abilities.xlsx
@@ -480,148 +480,148 @@
     <t>Upgrade</t>
   </si>
   <si>
+    <t>Nearby enemies surrounding Cia are slowed for a few seconds.</t>
+  </si>
+  <si>
+    <t>Stuns an enemy for a few seconds.</t>
+  </si>
+  <si>
+    <t>Restores a small amount of HP per second. But really, he stopped doing this a few months ago. REALLY. OMG SHUT UP, YOU HATER.</t>
+  </si>
+  <si>
+    <t>Logic Puzzle</t>
+  </si>
+  <si>
+    <t>Bling Bling</t>
+  </si>
+  <si>
+    <t>Taking Heart</t>
+  </si>
+  <si>
+    <t>Damages enemies in a wave</t>
+  </si>
+  <si>
+    <t>Drain HP from target enemy</t>
+  </si>
+  <si>
+    <t>After channeling, unleash massive damage to nearby enemies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Basic Attack: Shoot down an enemy with rapid gunfire. </t>
+  </si>
+  <si>
+    <t>Creates a ray of solar energy.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gains one solar charge every few seconds. After gaining three charges and activating again, sends forth bursts of solar energy. </t>
+  </si>
+  <si>
+    <t>Teleports Charles and Nate to a point. Afterwards, shoots kunais outward that temporarily stuns nearby enemies.</t>
+  </si>
+  <si>
+    <t>Ananya A.</t>
+  </si>
+  <si>
+    <t>Final Destination</t>
+  </si>
+  <si>
+    <t>Change X's and Ananya's Friendship Finale to Destination Zero.</t>
+  </si>
+  <si>
+    <t>[Aggressive Mediation] Jump up and down violently. Probably does nothing at all. HA TAKE THAT KATA</t>
+  </si>
+  <si>
+    <t>Arrow Control</t>
+  </si>
+  <si>
+    <t>Megaphone Attack</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Throws a random shoe toward a target out of anger. </t>
+  </si>
+  <si>
+    <t>Shoots arrows toward a target.</t>
+  </si>
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>Line</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Circle</t>
+  </si>
+  <si>
+    <t>Cone</t>
+  </si>
+  <si>
+    <t>Point</t>
+  </si>
+  <si>
+    <t>Wall</t>
+  </si>
+  <si>
+    <t>Invis</t>
+  </si>
+  <si>
+    <t>Kunai</t>
+  </si>
+  <si>
+    <t>Shot</t>
+  </si>
+  <si>
+    <t>Heart</t>
+  </si>
+  <si>
+    <t>Shoe</t>
+  </si>
+  <si>
+    <t>Thunder</t>
+  </si>
+  <si>
+    <t>Magic</t>
+  </si>
+  <si>
+    <t>Circles</t>
+  </si>
+  <si>
+    <t>Seal</t>
+  </si>
+  <si>
+    <t>Laser</t>
+  </si>
+  <si>
+    <t>Arrow</t>
+  </si>
+  <si>
+    <t>Aura</t>
+  </si>
+  <si>
+    <t>Set Damage</t>
+  </si>
+  <si>
+    <t>M. Gun Attack</t>
+  </si>
+  <si>
+    <t>Attack</t>
+  </si>
+  <si>
+    <t>AttackNum</t>
+  </si>
+  <si>
+    <t>AttackW</t>
+  </si>
+  <si>
+    <t>AttackH</t>
+  </si>
+  <si>
+    <t>AttackDist</t>
+  </si>
+  <si>
     <t>Downgrade</t>
-  </si>
-  <si>
-    <t>Nearby enemies surrounding Cia are slowed for a few seconds.</t>
-  </si>
-  <si>
-    <t>Stuns an enemy for a few seconds.</t>
-  </si>
-  <si>
-    <t>Restores a small amount of HP per second. But really, he stopped doing this a few months ago. REALLY. OMG SHUT UP, YOU HATER.</t>
-  </si>
-  <si>
-    <t>Logic Puzzle</t>
-  </si>
-  <si>
-    <t>Bling Bling</t>
-  </si>
-  <si>
-    <t>Taking Heart</t>
-  </si>
-  <si>
-    <t>Damages enemies in a wave</t>
-  </si>
-  <si>
-    <t>Drain HP from target enemy</t>
-  </si>
-  <si>
-    <t>After channeling, unleash massive damage to nearby enemies</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Basic Attack: Shoot down an enemy with rapid gunfire. </t>
-  </si>
-  <si>
-    <t>Creates a ray of solar energy.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gains one solar charge every few seconds. After gaining three charges and activating again, sends forth bursts of solar energy. </t>
-  </si>
-  <si>
-    <t>Teleports Charles and Nate to a point. Afterwards, shoots kunais outward that temporarily stuns nearby enemies.</t>
-  </si>
-  <si>
-    <t>Ananya A.</t>
-  </si>
-  <si>
-    <t>Final Destination</t>
-  </si>
-  <si>
-    <t>Change X's and Ananya's Friendship Finale to Destination Zero.</t>
-  </si>
-  <si>
-    <t>[Aggressive Mediation] Jump up and down violently. Probably does nothing at all. HA TAKE THAT KATA</t>
-  </si>
-  <si>
-    <t>Arrow Control</t>
-  </si>
-  <si>
-    <t>Megaphone Attack</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Throws a random shoe toward a target out of anger. </t>
-  </si>
-  <si>
-    <t>Shoots arrows toward a target.</t>
-  </si>
-  <si>
-    <t>Area</t>
-  </si>
-  <si>
-    <t>Line</t>
-  </si>
-  <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t>Circle</t>
-  </si>
-  <si>
-    <t>Cone</t>
-  </si>
-  <si>
-    <t>Point</t>
-  </si>
-  <si>
-    <t>Wall</t>
-  </si>
-  <si>
-    <t>Invis</t>
-  </si>
-  <si>
-    <t>Kunai</t>
-  </si>
-  <si>
-    <t>Shot</t>
-  </si>
-  <si>
-    <t>Heart</t>
-  </si>
-  <si>
-    <t>Shoe</t>
-  </si>
-  <si>
-    <t>Thunder</t>
-  </si>
-  <si>
-    <t>Magic</t>
-  </si>
-  <si>
-    <t>Circles</t>
-  </si>
-  <si>
-    <t>Seal</t>
-  </si>
-  <si>
-    <t>Laser</t>
-  </si>
-  <si>
-    <t>Arrow</t>
-  </si>
-  <si>
-    <t>Aura</t>
-  </si>
-  <si>
-    <t>Set Damage</t>
-  </si>
-  <si>
-    <t>M. Gun Attack</t>
-  </si>
-  <si>
-    <t>Attack</t>
-  </si>
-  <si>
-    <t>AttackNum</t>
-  </si>
-  <si>
-    <t>AttackW</t>
-  </si>
-  <si>
-    <t>AttackH</t>
-  </si>
-  <si>
-    <t>AttackDist</t>
   </si>
 </sst>
 </file>
@@ -648,6 +648,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -833,42 +834,6 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
       <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill patternType="solid">
@@ -1012,6 +977,42 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top/>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor theme="4" tint="0.79998168889431442"/>
@@ -2853,16 +2854,16 @@
     <tableColumn id="35" uniqueName="Bullet" name="Attack" dataDxfId="6">
       <xmlColumnPr mapId="12" xpath="/Abilities/Ability/Bullet" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="36" uniqueName="36" name="AttackNum" dataDxfId="0"/>
-    <tableColumn id="41" uniqueName="41" name="AttackW" dataDxfId="5"/>
-    <tableColumn id="42" uniqueName="42" name="AttackH" dataDxfId="4"/>
-    <tableColumn id="37" uniqueName="BulletRange" name="AttackDist" dataDxfId="3">
+    <tableColumn id="36" uniqueName="36" name="AttackNum" dataDxfId="5"/>
+    <tableColumn id="41" uniqueName="41" name="AttackW" dataDxfId="4"/>
+    <tableColumn id="42" uniqueName="42" name="AttackH" dataDxfId="3"/>
+    <tableColumn id="37" uniqueName="BulletRange" name="AttackDist" dataDxfId="2">
       <xmlColumnPr mapId="12" xpath="/Abilities/Ability/BulletRange" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="38" uniqueName="Target" name="Target" dataDxfId="2">
+    <tableColumn id="38" uniqueName="Target" name="Target" dataDxfId="1">
       <xmlColumnPr mapId="12" xpath="/Abilities/Ability/Target" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="39" uniqueName="Description" name="Description" dataDxfId="1">
+    <tableColumn id="39" uniqueName="Description" name="Description" dataDxfId="0">
       <xmlColumnPr mapId="12" xpath="/Abilities/Ability/Description" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -3157,9 +3158,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AP58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D50" sqref="D50"/>
+      <selection pane="topRight" activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3215,7 +3216,7 @@
         <v>67</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E2" s="15" t="s">
         <v>2</v>
@@ -3311,19 +3312,19 @@
         <v>121</v>
       </c>
       <c r="AJ2" s="19" t="s">
+        <v>196</v>
+      </c>
+      <c r="AK2" s="19" t="s">
         <v>197</v>
       </c>
-      <c r="AK2" s="19" t="s">
+      <c r="AL2" s="19" t="s">
         <v>198</v>
       </c>
-      <c r="AL2" s="19" t="s">
+      <c r="AM2" s="19" t="s">
         <v>199</v>
       </c>
-      <c r="AM2" s="19" t="s">
+      <c r="AN2" s="19" t="s">
         <v>200</v>
-      </c>
-      <c r="AN2" s="19" t="s">
-        <v>201</v>
       </c>
       <c r="AO2" s="19" t="s">
         <v>125</v>
@@ -3343,7 +3344,7 @@
         <v>68</v>
       </c>
       <c r="D3" s="29" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E3" s="3">
         <v>80</v>
@@ -3433,7 +3434,7 @@
       <c r="AH3" s="4"/>
       <c r="AI3" s="4"/>
       <c r="AJ3" s="28" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AK3" s="33">
         <v>1</v>
@@ -3461,7 +3462,7 @@
         <v>68</v>
       </c>
       <c r="D4" s="29" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E4" s="3">
         <v>80</v>
@@ -3553,7 +3554,7 @@
       <c r="AH4" s="4"/>
       <c r="AI4" s="4"/>
       <c r="AJ4" s="28" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="AK4" s="33">
         <v>0</v>
@@ -3581,7 +3582,7 @@
         <v>153</v>
       </c>
       <c r="D5" s="28" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E5" s="5">
         <v>140</v>
@@ -3671,7 +3672,7 @@
       <c r="AH5" s="4"/>
       <c r="AI5" s="4"/>
       <c r="AJ5" s="28" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="AK5" s="33">
         <v>0</v>
@@ -3699,7 +3700,7 @@
         <v>69</v>
       </c>
       <c r="D6" s="29" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E6" s="3">
         <v>30</v>
@@ -3789,7 +3790,7 @@
       <c r="AH6" s="4"/>
       <c r="AI6" s="4"/>
       <c r="AJ6" s="28" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AK6" s="33">
         <v>8</v>
@@ -3803,7 +3804,7 @@
         <v>128</v>
       </c>
       <c r="AP6" s="30" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="7" spans="1:42">
@@ -3817,7 +3818,7 @@
         <v>68</v>
       </c>
       <c r="D7" s="28" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E7" s="3">
         <v>20</v>
@@ -3907,7 +3908,7 @@
       <c r="AH7" s="4"/>
       <c r="AI7" s="4"/>
       <c r="AJ7" s="28" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AK7" s="33">
         <v>1</v>
@@ -3935,7 +3936,7 @@
         <v>153</v>
       </c>
       <c r="D8" s="29" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E8" s="3">
         <v>0</v>
@@ -4025,7 +4026,7 @@
       <c r="AH8" s="4"/>
       <c r="AI8" s="4"/>
       <c r="AJ8" s="28" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="AK8" s="33"/>
       <c r="AL8" s="4"/>
@@ -4051,7 +4052,7 @@
         <v>68</v>
       </c>
       <c r="D9" s="28" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E9" s="3">
         <v>120</v>
@@ -4141,7 +4142,7 @@
       <c r="AH9" s="4"/>
       <c r="AI9" s="4"/>
       <c r="AJ9" s="28" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AK9" s="33"/>
       <c r="AL9" s="4"/>
@@ -4167,7 +4168,7 @@
         <v>153</v>
       </c>
       <c r="D10" s="29" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E10" s="5">
         <v>50</v>
@@ -4257,7 +4258,7 @@
       <c r="AH10" s="4"/>
       <c r="AI10" s="4"/>
       <c r="AJ10" s="28" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="AK10" s="33"/>
       <c r="AL10" s="4"/>
@@ -4283,7 +4284,7 @@
         <v>68</v>
       </c>
       <c r="D11" s="28" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E11" s="3">
         <v>400</v>
@@ -4373,7 +4374,7 @@
       <c r="AH11" s="4"/>
       <c r="AI11" s="4"/>
       <c r="AJ11" s="28" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="AK11" s="33"/>
       <c r="AL11" s="4"/>
@@ -4397,7 +4398,7 @@
         <v>68</v>
       </c>
       <c r="D12" s="29" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E12" s="3">
         <v>500</v>
@@ -4487,7 +4488,7 @@
       <c r="AH12" s="4"/>
       <c r="AI12" s="4"/>
       <c r="AJ12" s="28" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AK12" s="33"/>
       <c r="AL12" s="4"/>
@@ -4497,7 +4498,7 @@
         <v>127</v>
       </c>
       <c r="AP12" s="30" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="13" spans="1:42">
@@ -4511,7 +4512,7 @@
         <v>68</v>
       </c>
       <c r="D13" s="28" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E13" s="3">
         <v>500</v>
@@ -4601,7 +4602,7 @@
       <c r="AH13" s="4"/>
       <c r="AI13" s="4"/>
       <c r="AJ13" s="28" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AK13" s="33"/>
       <c r="AL13" s="4"/>
@@ -4611,7 +4612,7 @@
         <v>127</v>
       </c>
       <c r="AP13" s="30" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="14" spans="1:42">
@@ -4625,7 +4626,7 @@
         <v>68</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E14" s="24">
         <v>200</v>
@@ -4717,7 +4718,7 @@
       <c r="AH14" s="26"/>
       <c r="AI14" s="26"/>
       <c r="AJ14" s="32" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="AK14" s="33"/>
       <c r="AL14" s="26"/>
@@ -4741,7 +4742,7 @@
         <v>68</v>
       </c>
       <c r="D15" s="29" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E15" s="3">
         <v>0</v>
@@ -4831,7 +4832,7 @@
       <c r="AH15" s="4"/>
       <c r="AI15" s="4"/>
       <c r="AJ15" s="28" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AK15" s="33"/>
       <c r="AL15" s="4"/>
@@ -4841,7 +4842,7 @@
         <v>127</v>
       </c>
       <c r="AP15" s="30" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="16" spans="1:42">
@@ -4855,7 +4856,7 @@
         <v>68</v>
       </c>
       <c r="D16" s="28" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E16" s="5">
         <v>400</v>
@@ -4945,7 +4946,7 @@
       <c r="AH16" s="4"/>
       <c r="AI16" s="4"/>
       <c r="AJ16" s="28" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="AK16" s="33"/>
       <c r="AL16" s="4"/>
@@ -4960,7 +4961,7 @@
     </row>
     <row r="17" spans="1:42">
       <c r="A17" s="23" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B17" s="23" t="s">
         <v>86</v>
@@ -4969,7 +4970,7 @@
         <v>68</v>
       </c>
       <c r="D17" s="23" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E17" s="24">
         <v>50</v>
@@ -5059,7 +5060,7 @@
       <c r="AH17" s="26"/>
       <c r="AI17" s="26"/>
       <c r="AJ17" s="32" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AK17" s="33"/>
       <c r="AL17" s="26"/>
@@ -5074,7 +5075,7 @@
     </row>
     <row r="18" spans="1:42">
       <c r="A18" s="23" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B18" s="23" t="s">
         <v>86</v>
@@ -5083,7 +5084,7 @@
         <v>144</v>
       </c>
       <c r="D18" s="23" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E18" s="24">
         <v>800</v>
@@ -5173,7 +5174,7 @@
       <c r="AH18" s="26"/>
       <c r="AI18" s="26"/>
       <c r="AJ18" s="32" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="AK18" s="33"/>
       <c r="AL18" s="26"/>
@@ -5188,16 +5189,16 @@
     </row>
     <row r="19" spans="1:42">
       <c r="A19" s="23" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B19" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="C19" s="23" t="s">
-        <v>154</v>
+      <c r="C19" s="28" t="s">
+        <v>201</v>
       </c>
       <c r="D19" s="23" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E19" s="24">
         <v>100</v>
@@ -5287,7 +5288,7 @@
       <c r="AH19" s="26"/>
       <c r="AI19" s="26"/>
       <c r="AJ19" s="32" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AK19" s="33"/>
       <c r="AL19" s="26"/>
@@ -5297,7 +5298,7 @@
         <v>127</v>
       </c>
       <c r="AP19" s="27" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="20" spans="1:42">
@@ -5311,7 +5312,7 @@
         <v>71</v>
       </c>
       <c r="D20" s="23" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E20" s="24">
         <v>0</v>
@@ -5401,7 +5402,7 @@
       <c r="AH20" s="26"/>
       <c r="AI20" s="26"/>
       <c r="AJ20" s="32" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="AK20" s="33"/>
       <c r="AL20" s="26"/>
@@ -5425,7 +5426,7 @@
         <v>68</v>
       </c>
       <c r="D21" s="28" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E21" s="5">
         <v>80</v>
@@ -5515,7 +5516,7 @@
       <c r="AH21" s="4"/>
       <c r="AI21" s="4"/>
       <c r="AJ21" s="28" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AK21" s="33"/>
       <c r="AL21" s="4"/>
@@ -5539,7 +5540,7 @@
         <v>68</v>
       </c>
       <c r="D22" s="29" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E22" s="3">
         <v>50</v>
@@ -5629,7 +5630,7 @@
       <c r="AH22" s="4"/>
       <c r="AI22" s="4"/>
       <c r="AJ22" s="28" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AK22" s="33"/>
       <c r="AL22" s="4"/>
@@ -5653,7 +5654,7 @@
         <v>68</v>
       </c>
       <c r="D23" s="28" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E23" s="5">
         <v>100</v>
@@ -5743,7 +5744,7 @@
       <c r="AH23" s="4"/>
       <c r="AI23" s="4"/>
       <c r="AJ23" s="28" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AK23" s="33"/>
       <c r="AL23" s="4"/>
@@ -5767,7 +5768,7 @@
         <v>68</v>
       </c>
       <c r="D24" s="29" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E24" s="3">
         <v>100</v>
@@ -5857,7 +5858,7 @@
       <c r="AH24" s="4"/>
       <c r="AI24" s="4"/>
       <c r="AJ24" s="28" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AK24" s="33"/>
       <c r="AL24" s="4"/>
@@ -5881,7 +5882,7 @@
         <v>68</v>
       </c>
       <c r="D25" s="28" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E25" s="5">
         <v>300</v>
@@ -5971,7 +5972,7 @@
       <c r="AH25" s="4"/>
       <c r="AI25" s="4"/>
       <c r="AJ25" s="28" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="AK25" s="33"/>
       <c r="AL25" s="4"/>
@@ -5986,16 +5987,16 @@
     </row>
     <row r="26" spans="1:42">
       <c r="A26" s="28" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C26" s="29" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D26" s="29" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E26" s="5">
         <v>200</v>
@@ -6085,7 +6086,7 @@
       <c r="AH26" s="4"/>
       <c r="AI26" s="4"/>
       <c r="AJ26" s="28" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AK26" s="33"/>
       <c r="AL26" s="4"/>
@@ -6095,7 +6096,7 @@
         <v>127</v>
       </c>
       <c r="AP26" s="30" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="27" spans="1:42">
@@ -6109,7 +6110,7 @@
         <v>68</v>
       </c>
       <c r="D27" s="28" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E27" s="3">
         <v>0</v>
@@ -6201,7 +6202,7 @@
       <c r="AH27" s="4"/>
       <c r="AI27" s="4"/>
       <c r="AJ27" s="28" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="AK27" s="33"/>
       <c r="AL27" s="4"/>
@@ -6210,7 +6211,7 @@
       <c r="AO27" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="AP27" s="20" t="s">
+      <c r="AP27" s="30" t="s">
         <v>17</v>
       </c>
     </row>
@@ -6225,7 +6226,7 @@
         <v>70</v>
       </c>
       <c r="D28" s="29" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E28" s="5">
         <v>300</v>
@@ -6315,7 +6316,7 @@
       <c r="AH28" s="4"/>
       <c r="AI28" s="4"/>
       <c r="AJ28" s="28" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="AK28" s="33"/>
       <c r="AL28" s="4"/>
@@ -6339,7 +6340,7 @@
         <v>71</v>
       </c>
       <c r="D29" s="28" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E29" s="5">
         <v>0</v>
@@ -6429,7 +6430,7 @@
       <c r="AH29" s="4"/>
       <c r="AI29" s="4"/>
       <c r="AJ29" s="28" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="AK29" s="33"/>
       <c r="AL29" s="4"/>
@@ -6439,12 +6440,12 @@
         <v>129</v>
       </c>
       <c r="AP29" s="30" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="30" spans="1:42">
       <c r="A30" s="28" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>97</v>
@@ -6453,7 +6454,7 @@
         <v>68</v>
       </c>
       <c r="D30" s="28" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E30" s="5">
         <v>100</v>
@@ -6565,7 +6566,7 @@
         <v>68</v>
       </c>
       <c r="D31" s="28" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E31" s="5">
         <v>100</v>
@@ -6677,7 +6678,7 @@
         <v>68</v>
       </c>
       <c r="D32" s="28" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E32" s="5">
         <v>150</v>
@@ -6789,7 +6790,7 @@
         <v>72</v>
       </c>
       <c r="D33" s="28" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E33" s="5">
         <v>0</v>
@@ -6901,7 +6902,7 @@
         <v>68</v>
       </c>
       <c r="D34" s="23" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E34" s="24">
         <v>30</v>
@@ -7015,7 +7016,7 @@
         <v>68</v>
       </c>
       <c r="D35" s="23" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E35" s="24">
         <v>50</v>
@@ -7127,7 +7128,7 @@
         <v>72</v>
       </c>
       <c r="D36" s="23" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E36" s="24">
         <v>0</v>
@@ -7239,7 +7240,7 @@
         <v>68</v>
       </c>
       <c r="D37" s="23" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E37" s="24">
         <v>100</v>
@@ -7351,7 +7352,7 @@
         <v>68</v>
       </c>
       <c r="D38" s="29" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E38" s="3">
         <v>60</v>
@@ -7463,7 +7464,7 @@
         <v>72</v>
       </c>
       <c r="D39" s="28" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E39" s="5">
         <v>70</v>
@@ -7575,7 +7576,7 @@
         <v>153</v>
       </c>
       <c r="D40" s="29" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E40" s="3">
         <v>50</v>
@@ -7687,7 +7688,7 @@
         <v>68</v>
       </c>
       <c r="D41" s="28" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E41" s="5">
         <v>80</v>
@@ -7799,7 +7800,7 @@
         <v>71</v>
       </c>
       <c r="D42" s="29" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E42" s="3">
         <v>0</v>
@@ -7911,7 +7912,7 @@
         <v>71</v>
       </c>
       <c r="D43" s="28" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E43" s="5">
         <v>0</v>
@@ -8023,7 +8024,7 @@
         <v>68</v>
       </c>
       <c r="D44" s="29" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E44" s="3">
         <v>30</v>
@@ -8126,16 +8127,16 @@
     </row>
     <row r="45" spans="1:42">
       <c r="A45" s="23" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B45" s="28" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>71</v>
       </c>
       <c r="D45" s="28" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E45" s="5">
         <v>0</v>
@@ -8233,7 +8234,7 @@
         <v>128</v>
       </c>
       <c r="AP45" s="27" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="46" spans="1:42">
@@ -8247,7 +8248,7 @@
         <v>68</v>
       </c>
       <c r="D46" s="23" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E46" s="24">
         <v>800</v>
@@ -8345,7 +8346,7 @@
         <v>127</v>
       </c>
       <c r="AP46" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="47" spans="1:42">
@@ -8359,7 +8360,7 @@
         <v>68</v>
       </c>
       <c r="D47" s="23" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E47" s="24">
         <v>100</v>
@@ -8457,21 +8458,21 @@
         <v>127</v>
       </c>
       <c r="AP47" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="48" spans="1:42">
       <c r="A48" s="28" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B48" s="23" t="s">
         <v>143</v>
       </c>
       <c r="C48" s="28" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D48" s="23" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E48" s="24">
         <v>300</v>
@@ -8569,7 +8570,7 @@
         <v>127</v>
       </c>
       <c r="AP48" s="27" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="49" spans="1:42">
@@ -8583,7 +8584,7 @@
         <v>68</v>
       </c>
       <c r="D49" s="28" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E49" s="24">
         <v>100</v>
@@ -8681,7 +8682,7 @@
         <v>127</v>
       </c>
       <c r="AP49" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="50" spans="1:42">
@@ -8695,7 +8696,7 @@
         <v>144</v>
       </c>
       <c r="D50" s="23" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E50" s="24">
         <v>50</v>
@@ -8793,7 +8794,7 @@
         <v>127</v>
       </c>
       <c r="AP50" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="51" spans="1:42">
@@ -8807,7 +8808,7 @@
         <v>68</v>
       </c>
       <c r="D51" s="23" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E51" s="24">
         <v>80</v>
@@ -8907,7 +8908,7 @@
         <v>127</v>
       </c>
       <c r="AP51" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="52" spans="1:42">
@@ -8921,7 +8922,7 @@
         <v>73</v>
       </c>
       <c r="D52" s="29" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E52" s="3">
         <v>0</v>
@@ -9033,7 +9034,7 @@
         <v>71</v>
       </c>
       <c r="D53" s="28" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E53" s="5">
         <v>0</v>
@@ -9145,7 +9146,7 @@
         <v>71</v>
       </c>
       <c r="D54" s="29" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E54" s="3">
         <v>0</v>
@@ -9257,7 +9258,7 @@
         <v>71</v>
       </c>
       <c r="D55" s="29" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E55" s="3">
         <v>0</v>
@@ -9369,7 +9370,7 @@
         <v>71</v>
       </c>
       <c r="D56" s="28" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E56" s="5">
         <v>0</v>
@@ -9481,7 +9482,7 @@
         <v>68</v>
       </c>
       <c r="D57" s="29" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E57" s="3">
         <v>400</v>
@@ -9593,7 +9594,7 @@
         <v>68</v>
       </c>
       <c r="D58" s="31" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E58" s="7">
         <v>400</v>

</xml_diff>

<commit_message>
Implemented basic z-sorting. Will make more efficient later.
</commit_message>
<xml_diff>
--- a/xml/Abilities.xlsx
+++ b/xml/Abilities.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="223">
   <si>
     <t>Name</t>
   </si>
@@ -682,6 +682,9 @@
   </si>
   <si>
     <t>Basic Attack: Fire a bullet at a target enemy. Hold down for rapid gunfire.</t>
+  </si>
+  <si>
+    <t>0-none 1-move 2-align 3-teleport</t>
   </si>
 </sst>
 </file>
@@ -3511,9 +3514,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AS59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AP1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AS50" sqref="AS50"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3559,6 +3562,9 @@
       <c r="F1" t="s">
         <v>47</v>
       </c>
+      <c r="AH1" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="2" spans="1:45" ht="15.75" thickBot="1">
       <c r="A2" s="1" t="s">
@@ -3798,7 +3804,7 @@
         <v>0</v>
       </c>
       <c r="AH3" s="22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AI3" s="15"/>
       <c r="AJ3" s="15"/>
@@ -3925,7 +3931,7 @@
         <v>0</v>
       </c>
       <c r="AH4" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AI4" s="3">
         <v>1</v>
@@ -4181,7 +4187,7 @@
         <v>0</v>
       </c>
       <c r="AH6" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AI6" s="3"/>
       <c r="AJ6" s="3"/>
@@ -4308,7 +4314,7 @@
         <v>0</v>
       </c>
       <c r="AH7" s="19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AI7" s="18"/>
       <c r="AJ7" s="18"/>

</xml_diff>

<commit_message>
Shinai Attack focus. More mods to Battle system :)
</commit_message>
<xml_diff>
--- a/xml/Abilities.xlsx
+++ b/xml/Abilities.xlsx
@@ -896,7 +896,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1025,59 +1025,12 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="11">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1334,17 +1287,65 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thick">
           <color theme="0"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-      </border>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1432,13 +1433,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:R71" tableType="xml" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" headerRowBorderDxfId="9" tableBorderDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:R71" tableType="xml" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7">
   <autoFilter ref="A2:R71"/>
   <tableColumns count="18">
     <tableColumn id="1" uniqueName="Name" name="Name">
       <xmlColumnPr mapId="33" xpath="/Abilities/Ability/Name" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="Description" name="Description" dataDxfId="8">
+    <tableColumn id="2" uniqueName="Description" name="Description" dataDxfId="6">
       <xmlColumnPr mapId="33" xpath="/Abilities/Ability/Description" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="3" uniqueName="Availability" name="Availability">
@@ -1465,10 +1466,10 @@
     <tableColumn id="10" uniqueName="Exist" name="Exist">
       <xmlColumnPr mapId="33" xpath="/Abilities/Ability/Exist" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="11" uniqueName="Min" name="Min" dataDxfId="7">
+    <tableColumn id="11" uniqueName="Min" name="Min" dataDxfId="5">
       <xmlColumnPr mapId="33" xpath="/Abilities/Ability/Min" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="12" uniqueName="Max" name="Max" dataDxfId="6">
+    <tableColumn id="12" uniqueName="Max" name="Max" dataDxfId="4">
       <xmlColumnPr mapId="33" xpath="/Abilities/Ability/Max" xmlDataType="integer"/>
     </tableColumn>
     <tableColumn id="13" uniqueName="Range" name="Range">
@@ -1477,16 +1478,16 @@
     <tableColumn id="14" uniqueName="Cooldown" name="Cooldown">
       <xmlColumnPr mapId="33" xpath="/Abilities/Ability/Cooldown" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="15" uniqueName="Power" name="Power" dataDxfId="5">
+    <tableColumn id="15" uniqueName="Power" name="Power" dataDxfId="3">
       <xmlColumnPr mapId="33" xpath="/Abilities/Ability/Power" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="16" uniqueName="Power2" name="Power2" dataDxfId="4">
+    <tableColumn id="16" uniqueName="Power2" name="Power2" dataDxfId="2">
       <xmlColumnPr mapId="33" xpath="/Abilities/Ability/Power2" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="17" uniqueName="Power3" name="Power3" dataDxfId="3">
+    <tableColumn id="17" uniqueName="Power3" name="Power3" dataDxfId="1">
       <xmlColumnPr mapId="33" xpath="/Abilities/Ability/Power3" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="18" uniqueName="Correct" name="Correct" dataDxfId="2">
+    <tableColumn id="18" uniqueName="Correct" name="Correct" dataDxfId="0">
       <xmlColumnPr mapId="33" xpath="/Abilities/Ability/Correct" xmlDataType="integer"/>
     </tableColumn>
   </tableColumns>
@@ -1783,7 +1784,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="R71" sqref="R71"/>
+      <selection pane="topRight" activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2158,7 +2159,7 @@
       <c r="X6" s="35"/>
     </row>
     <row r="7" spans="1:24">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="54" t="s">
         <v>53</v>
       </c>
       <c r="B7" s="3" t="s">

</xml_diff>

<commit_message>
Testing out some random attacks.
</commit_message>
<xml_diff>
--- a/xml/Abilities.xlsx
+++ b/xml/Abilities.xlsx
@@ -66,9 +66,6 @@
     <t>Basic Attack: Shoots two guided lasers toward a target.</t>
   </si>
   <si>
-    <t>Apologizing</t>
-  </si>
-  <si>
     <t>Creates a magic and apologetic wall that lasts for four seconds.</t>
   </si>
   <si>
@@ -339,9 +336,6 @@
     <t>Megaphone Attack</t>
   </si>
   <si>
-    <t xml:space="preserve">Throws a random shoe toward a target out of anger. </t>
-  </si>
-  <si>
     <t>Line</t>
   </si>
   <si>
@@ -679,6 +673,12 @@
   </si>
   <si>
     <t>Correct</t>
+  </si>
+  <si>
+    <t>Apologetic</t>
+  </si>
+  <si>
+    <t>Throws a magical shoe to a target out of anger. Each time it hits the wall or an enemy attack, it bounces and gains more damage and speed.</t>
   </si>
 </sst>
 </file>
@@ -896,7 +896,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1026,6 +1026,8 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1784,7 +1786,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B35" sqref="B35"/>
+      <selection pane="topRight" activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1812,28 +1814,28 @@
   <sheetData>
     <row r="1" spans="1:24">
       <c r="C1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D1" t="s">
+        <v>188</v>
+      </c>
+      <c r="E1" t="s">
         <v>189</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>190</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" t="s">
         <v>191</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>192</v>
       </c>
-      <c r="G1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>193</v>
-      </c>
-      <c r="I1" t="s">
-        <v>194</v>
-      </c>
-      <c r="J1" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="2" spans="1:24" ht="15.75" thickBot="1">
@@ -1847,31 +1849,31 @@
         <v>5</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>4</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="H2" s="5" t="s">
         <v>6</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="K2" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="L2" s="5" t="s">
         <v>64</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>65</v>
       </c>
       <c r="M2" s="5" t="s">
         <v>2</v>
@@ -1880,51 +1882,51 @@
         <v>3</v>
       </c>
       <c r="O2" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="P2" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="P2" s="1" t="s">
-        <v>215</v>
-      </c>
       <c r="Q2" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="R2" s="53" t="s">
+        <v>218</v>
+      </c>
+      <c r="S2" s="34" t="s">
         <v>216</v>
       </c>
-      <c r="R2" s="53" t="s">
-        <v>220</v>
-      </c>
-      <c r="S2" s="34" t="s">
-        <v>218</v>
-      </c>
       <c r="T2" s="34" t="s">
+        <v>204</v>
+      </c>
+      <c r="U2" s="34" t="s">
+        <v>205</v>
+      </c>
+      <c r="V2" s="34" t="s">
+        <v>212</v>
+      </c>
+      <c r="W2" s="34" t="s">
         <v>206</v>
       </c>
-      <c r="U2" s="34" t="s">
+      <c r="X2" s="34" t="s">
         <v>207</v>
-      </c>
-      <c r="V2" s="34" t="s">
-        <v>214</v>
-      </c>
-      <c r="W2" s="34" t="s">
-        <v>208</v>
-      </c>
-      <c r="X2" s="34" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="3" spans="1:24" ht="15.75" thickTop="1">
       <c r="A3" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F3" s="18">
         <v>1</v>
@@ -1951,16 +1953,16 @@
         <v>80</v>
       </c>
       <c r="N3" s="12" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="O3" s="17" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="P3" s="17" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="Q3" s="17" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="R3" s="45">
         <v>1</v>
@@ -1974,19 +1976,19 @@
     </row>
     <row r="4" spans="1:24">
       <c r="A4" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F4" s="21">
         <v>1</v>
@@ -2013,16 +2015,16 @@
         <v>80</v>
       </c>
       <c r="N4" s="13" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="O4" s="16" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="P4" s="16" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="Q4" s="16" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="R4" s="46">
         <v>1</v>
@@ -2036,19 +2038,19 @@
     </row>
     <row r="5" spans="1:24">
       <c r="A5" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F5" s="24">
         <v>1</v>
@@ -2075,7 +2077,7 @@
         <v>140</v>
       </c>
       <c r="N5" s="14" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="O5" s="14">
         <v>0</v>
@@ -2098,19 +2100,19 @@
     </row>
     <row r="6" spans="1:24">
       <c r="A6" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>34</v>
-      </c>
       <c r="D6" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F6" s="23">
         <v>1</v>
@@ -2137,16 +2139,16 @@
         <v>30</v>
       </c>
       <c r="N6" s="13" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="O6" s="16" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="P6" s="16" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="Q6" s="16" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="R6" s="46">
         <v>0</v>
@@ -2160,19 +2162,19 @@
     </row>
     <row r="7" spans="1:24">
       <c r="A7" s="54" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F7" s="11">
         <v>1</v>
@@ -2196,19 +2198,19 @@
         <v>10</v>
       </c>
       <c r="M7" s="11">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="N7" s="15" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="O7" s="14" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="P7" s="14" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="Q7" s="14" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="R7" s="45">
         <v>1</v>
@@ -2222,19 +2224,19 @@
     </row>
     <row r="8" spans="1:24">
       <c r="A8" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F8" s="23">
         <v>0</v>
@@ -2284,19 +2286,19 @@
     </row>
     <row r="9" spans="1:24">
       <c r="A9" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F9" s="11">
         <v>1</v>
@@ -2323,16 +2325,16 @@
         <v>120</v>
       </c>
       <c r="N9" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="O9" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="O9" s="14" t="s">
-        <v>128</v>
-      </c>
       <c r="P9" s="14" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="Q9" s="14" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="R9" s="47">
         <v>0</v>
@@ -2346,19 +2348,19 @@
     </row>
     <row r="10" spans="1:24">
       <c r="A10" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="C10" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>57</v>
-      </c>
       <c r="D10" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F10" s="23">
         <v>1</v>
@@ -2385,7 +2387,7 @@
         <v>50</v>
       </c>
       <c r="N10" s="13" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="O10" s="16">
         <v>0</v>
@@ -2408,19 +2410,19 @@
     </row>
     <row r="11" spans="1:24">
       <c r="A11" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F11" s="11">
         <v>3</v>
@@ -2447,16 +2449,16 @@
         <v>20</v>
       </c>
       <c r="N11" s="15" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="O11" s="14" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="P11" s="14" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="Q11" s="14" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="R11" s="47">
         <v>0</v>
@@ -2473,16 +2475,16 @@
         <v>14</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F12" s="11">
         <v>1</v>
@@ -2521,7 +2523,7 @@
         <v>5</v>
       </c>
       <c r="R12" s="48">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="S12" s="35"/>
       <c r="T12" s="35"/>
@@ -2535,16 +2537,16 @@
         <v>7</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>9</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F13" s="23">
         <v>1</v>
@@ -2596,17 +2598,17 @@
       <c r="A14" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>107</v>
+      <c r="B14" s="56" t="s">
+        <v>220</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F14" s="11">
         <v>1</v>
@@ -2656,19 +2658,19 @@
     </row>
     <row r="15" spans="1:24">
       <c r="A15" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F15" s="22">
         <v>1</v>
@@ -2718,19 +2720,19 @@
     </row>
     <row r="16" spans="1:24">
       <c r="A16" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F16" s="11">
         <v>1</v>
@@ -2780,19 +2782,19 @@
     </row>
     <row r="17" spans="1:24">
       <c r="A17" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>61</v>
-      </c>
       <c r="D17" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F17" s="22">
         <v>1</v>
@@ -2842,19 +2844,19 @@
     </row>
     <row r="18" spans="1:24">
       <c r="A18" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F18" s="24">
         <v>1</v>
@@ -2904,19 +2906,19 @@
     </row>
     <row r="19" spans="1:24">
       <c r="A19" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F19" s="22">
         <v>1</v>
@@ -2966,19 +2968,19 @@
     </row>
     <row r="20" spans="1:24">
       <c r="A20" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F20" s="24">
         <v>1</v>
@@ -3028,19 +3030,19 @@
     </row>
     <row r="21" spans="1:24">
       <c r="A21" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F21" s="22">
         <v>0</v>
@@ -3090,19 +3092,19 @@
     </row>
     <row r="22" spans="1:24">
       <c r="A22" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="C22" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F22" s="24">
         <v>1</v>
@@ -3152,19 +3154,19 @@
     </row>
     <row r="23" spans="1:24">
       <c r="A23" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F23" s="23">
         <v>1</v>
@@ -3214,19 +3216,19 @@
     </row>
     <row r="24" spans="1:24">
       <c r="A24" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F24" s="24">
         <v>3</v>
@@ -3276,19 +3278,19 @@
     </row>
     <row r="25" spans="1:24">
       <c r="A25" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C25" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>20</v>
-      </c>
       <c r="D25" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F25" s="23">
         <v>1</v>
@@ -3347,10 +3349,10 @@
         <v>10</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F26" s="24">
         <v>1</v>
@@ -3400,19 +3402,19 @@
     </row>
     <row r="27" spans="1:24">
       <c r="A27" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F27" s="22">
         <v>8</v>
@@ -3465,16 +3467,16 @@
         <v>11</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F28" s="11">
         <v>5</v>
@@ -3527,16 +3529,16 @@
         <v>12</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F29" s="22">
         <v>2</v>
@@ -3585,20 +3587,20 @@
       <c r="X29" s="35"/>
     </row>
     <row r="30" spans="1:24">
-      <c r="A30" s="10" t="s">
-        <v>16</v>
+      <c r="A30" s="55" t="s">
+        <v>219</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C30" s="10" t="s">
         <v>10</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F30" s="24">
         <v>0</v>
@@ -3647,20 +3649,20 @@
       <c r="X30" s="35"/>
     </row>
     <row r="31" spans="1:24">
-      <c r="A31" s="3" t="s">
-        <v>106</v>
+      <c r="A31" s="56" t="s">
+        <v>105</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F31" s="22">
         <v>1</v>
@@ -3710,19 +3712,19 @@
     </row>
     <row r="32" spans="1:24">
       <c r="A32" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F32" s="24">
         <v>1</v>
@@ -3772,19 +3774,19 @@
     </row>
     <row r="33" spans="1:24">
       <c r="A33" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F33" s="22">
         <v>1</v>
@@ -3834,19 +3836,19 @@
     </row>
     <row r="34" spans="1:24">
       <c r="A34" s="10" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F34" s="24">
         <v>1</v>
@@ -3896,19 +3898,19 @@
     </row>
     <row r="35" spans="1:24">
       <c r="A35" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="B35" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="B35" s="3" t="s">
-        <v>198</v>
-      </c>
       <c r="C35" s="6" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F35" s="18">
         <v>1</v>
@@ -3935,16 +3937,16 @@
         <v>80</v>
       </c>
       <c r="N35" s="12" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="O35" s="17" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="P35" s="17" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="Q35" s="17" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="R35" s="50">
         <v>0</v>
@@ -3958,19 +3960,19 @@
     </row>
     <row r="36" spans="1:24">
       <c r="A36" s="25" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B36" s="35" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E36" s="25" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F36" s="26">
         <v>4</v>
@@ -4020,19 +4022,19 @@
     </row>
     <row r="37" spans="1:24">
       <c r="A37" s="25" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B37" s="35" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D37" s="25" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E37" s="25" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F37" s="26">
         <v>1</v>
@@ -4082,19 +4084,19 @@
     </row>
     <row r="38" spans="1:24">
       <c r="A38" s="25" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B38" s="35" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D38" s="25" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E38" s="25" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F38" s="26">
         <v>0</v>
@@ -4144,19 +4146,19 @@
     </row>
     <row r="39" spans="1:24">
       <c r="A39" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F39" s="22">
         <v>1</v>
@@ -4206,19 +4208,19 @@
     </row>
     <row r="40" spans="1:24">
       <c r="A40" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D40" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E40" s="10" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F40" s="24">
         <v>3</v>
@@ -4268,19 +4270,19 @@
     </row>
     <row r="41" spans="1:24">
       <c r="A41" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F41" s="22">
         <v>1</v>
@@ -4330,19 +4332,19 @@
     </row>
     <row r="42" spans="1:24">
       <c r="A42" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D42" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E42" s="10" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F42" s="24">
         <v>3</v>
@@ -4392,19 +4394,19 @@
     </row>
     <row r="43" spans="1:24">
       <c r="A43" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B43" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="B43" s="3" t="s">
-        <v>176</v>
-      </c>
       <c r="C43" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F43" s="24">
         <v>1</v>
@@ -4454,19 +4456,19 @@
     </row>
     <row r="44" spans="1:24">
       <c r="A44" s="25" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B44" s="35" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C44" s="25" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D44" s="25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E44" s="25" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F44" s="26">
         <v>1</v>
@@ -4516,19 +4518,19 @@
     </row>
     <row r="45" spans="1:24">
       <c r="A45" s="25" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B45" s="35" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C45" s="25" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D45" s="25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E45" s="25" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F45" s="26">
         <v>1</v>
@@ -4578,19 +4580,19 @@
     </row>
     <row r="46" spans="1:24">
       <c r="A46" s="25" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B46" s="35" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C46" s="25" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D46" s="25" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E46" s="25" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F46" s="26">
         <v>1</v>
@@ -4640,19 +4642,19 @@
     </row>
     <row r="47" spans="1:24">
       <c r="A47" s="25" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B47" s="35" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C47" s="25" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D47" s="25" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E47" s="25" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F47" s="26">
         <v>1</v>
@@ -4702,19 +4704,19 @@
     </row>
     <row r="48" spans="1:24">
       <c r="A48" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B48" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B48" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="C48" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F48" s="11">
         <v>1</v>
@@ -4764,19 +4766,19 @@
     </row>
     <row r="49" spans="1:24">
       <c r="A49" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B49" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B49" s="3" t="s">
-        <v>29</v>
-      </c>
       <c r="C49" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D49" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E49" s="10" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F49" s="24">
         <v>3</v>
@@ -4826,19 +4828,19 @@
     </row>
     <row r="50" spans="1:24">
       <c r="A50" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F50" s="11">
         <v>3</v>
@@ -4888,19 +4890,19 @@
     </row>
     <row r="51" spans="1:24">
       <c r="A51" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C51" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D51" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E51" s="10" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F51" s="24">
         <v>5</v>
@@ -4950,19 +4952,19 @@
     </row>
     <row r="52" spans="1:24">
       <c r="A52" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C52" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B52" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="D52" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F52" s="11">
         <v>1</v>
@@ -5012,19 +5014,19 @@
     </row>
     <row r="53" spans="1:24">
       <c r="A53" s="25" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B53" s="35" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C53" s="25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D53" s="25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E53" s="25" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F53" s="26">
         <v>1</v>
@@ -5074,19 +5076,19 @@
     </row>
     <row r="54" spans="1:24">
       <c r="A54" s="25" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B54" s="35" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C54" s="25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D54" s="25" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E54" s="25" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F54" s="26">
         <v>1</v>
@@ -5136,19 +5138,19 @@
     </row>
     <row r="55" spans="1:24">
       <c r="A55" s="25" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B55" s="35" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C55" s="25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D55" s="25" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E55" s="25" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F55" s="26">
         <v>1</v>
@@ -5198,19 +5200,19 @@
     </row>
     <row r="56" spans="1:24">
       <c r="A56" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B56" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="B56" s="3" t="s">
-        <v>103</v>
-      </c>
       <c r="C56" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F56" s="22">
         <v>0</v>
@@ -5260,19 +5262,19 @@
     </row>
     <row r="57" spans="1:24">
       <c r="A57" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F57" s="22">
         <v>1</v>
@@ -5322,19 +5324,19 @@
     </row>
     <row r="58" spans="1:24">
       <c r="A58" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F58" s="22">
         <v>10</v>
@@ -5384,19 +5386,19 @@
     </row>
     <row r="59" spans="1:24">
       <c r="A59" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F59" s="22">
         <v>10</v>
@@ -5446,19 +5448,19 @@
     </row>
     <row r="60" spans="1:24">
       <c r="A60" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F60" s="22">
         <v>3</v>
@@ -5508,19 +5510,19 @@
     </row>
     <row r="61" spans="1:24">
       <c r="A61" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C61" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D61" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="D61" s="3" t="s">
-        <v>86</v>
-      </c>
       <c r="E61" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F61" s="22">
         <v>1</v>
@@ -5570,19 +5572,19 @@
     </row>
     <row r="62" spans="1:24">
       <c r="A62" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F62" s="22">
         <v>1</v>
@@ -5632,19 +5634,19 @@
     </row>
     <row r="63" spans="1:24">
       <c r="A63" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="C63" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B63" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="D63" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F63" s="11">
         <v>1</v>
@@ -5694,19 +5696,19 @@
     </row>
     <row r="64" spans="1:24">
       <c r="A64" s="25" t="s">
+        <v>182</v>
+      </c>
+      <c r="B64" s="35" t="s">
         <v>184</v>
       </c>
-      <c r="B64" s="35" t="s">
-        <v>186</v>
-      </c>
       <c r="C64" s="25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D64" s="25" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E64" s="25" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F64" s="26">
         <v>1</v>
@@ -5756,19 +5758,19 @@
     </row>
     <row r="65" spans="1:24">
       <c r="A65" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F65" s="22">
         <v>0</v>
@@ -5818,19 +5820,19 @@
     </row>
     <row r="66" spans="1:24">
       <c r="A66" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F66" s="11">
         <v>0</v>
@@ -5880,19 +5882,19 @@
     </row>
     <row r="67" spans="1:24">
       <c r="A67" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F67" s="11">
         <v>0</v>
@@ -5942,19 +5944,19 @@
     </row>
     <row r="68" spans="1:24">
       <c r="A68" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F68" s="22">
         <v>0</v>
@@ -6004,19 +6006,19 @@
     </row>
     <row r="69" spans="1:24">
       <c r="A69" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C69" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B69" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="D69" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F69" s="11">
         <v>1</v>
@@ -6066,19 +6068,19 @@
     </row>
     <row r="70" spans="1:24">
       <c r="A70" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F70" s="22">
         <v>1</v>
@@ -6128,19 +6130,19 @@
     </row>
     <row r="71" spans="1:24">
       <c r="A71" s="30" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B71" s="37" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C71" s="30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D71" s="30" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E71" s="30" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F71" s="31">
         <v>0</v>

</xml_diff>

<commit_message>
There's a really annoying Ability gameHandler bug that I'm trying to fix now. Apologetic won't quit healing after being unequipped.
</commit_message>
<xml_diff>
--- a/xml/Abilities.xlsx
+++ b/xml/Abilities.xlsx
@@ -678,13 +678,13 @@
     <t>Dashes in a straight line, stunning any enemies in the way. Pick up special gems for extra bonuses!</t>
   </si>
   <si>
-    <t>1+1</t>
-  </si>
-  <si>
-    <t>5-0.2</t>
-  </si>
-  <si>
-    <t>Restores POWER Health per POWER2 seconds. But really, he stopped doing this a few months ago. NO REALLY. OH SCREW YOU MAN.</t>
+    <t>0</t>
+  </si>
+  <si>
+    <t>Restores POWER Health per 5 seconds. But really, he stopped doing this a few months ago. NO REALLY. OH SCREW YOU MAN.</t>
+  </si>
+  <si>
+    <t>1+4</t>
   </si>
 </sst>
 </file>
@@ -1793,9 +1793,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:X71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="O31" sqref="O31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3600,7 +3600,7 @@
         <v>217</v>
       </c>
       <c r="B30" s="56" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C30" s="10" t="s">
         <v>10</v>
@@ -3639,10 +3639,10 @@
         <v>0</v>
       </c>
       <c r="O30" s="57" t="s">
+        <v>222</v>
+      </c>
+      <c r="P30" s="57" t="s">
         <v>220</v>
-      </c>
-      <c r="P30" s="57" t="s">
-        <v>221</v>
       </c>
       <c r="Q30" s="14">
         <v>0</v>
@@ -6202,6 +6202,9 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="P30" numberStoredAsText="1"/>
+  </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>

</xml_diff>

<commit_message>
Arrow Control works now after many failed/stupid attempts. >.>
</commit_message>
<xml_diff>
--- a/xml/Abilities.xlsx
+++ b/xml/Abilities.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="227">
   <si>
     <t>Name</t>
   </si>
@@ -471,9 +471,6 @@
     <t xml:space="preserve">Restores Health to any Unit. </t>
   </si>
   <si>
-    <t>Strengthens Nate with extra Attack and Health restoration over time.</t>
-  </si>
-  <si>
     <t>Reduces Charles' and Nate's Reload Times.</t>
   </si>
   <si>
@@ -549,9 +546,6 @@
     <t>Unleashes a magical elongated surprise from a magical box. ;D</t>
   </si>
   <si>
-    <t>Restores some of Kata's Health every few seconds.</t>
-  </si>
-  <si>
     <t>Creates a happy shield inside a target and makes it expand.</t>
   </si>
   <si>
@@ -684,7 +678,25 @@
     <t>Restores POWER Health per 5 seconds. But really, he stopped doing this a few months ago. NO REALLY. OH SCREW YOU MAN.</t>
   </si>
   <si>
-    <t>1+4</t>
+    <t>2+4</t>
+  </si>
+  <si>
+    <t>Motivates Kata to restore POWER Health and Cia to restore POWER2 Health every 4 seconds.</t>
+  </si>
+  <si>
+    <t>1+3</t>
+  </si>
+  <si>
+    <t>2+3.5</t>
+  </si>
+  <si>
+    <t>Strengthens Nate with POWER extra Attack and restores POWER2 Health every 5 seconds.</t>
+  </si>
+  <si>
+    <t>2+1</t>
+  </si>
+  <si>
+    <t>4+1</t>
   </si>
 </sst>
 </file>
@@ -902,7 +914,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1035,6 +1047,9 @@
     <xf numFmtId="49" fontId="0" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -1793,9 +1808,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:X71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="O31" sqref="O31"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="K1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="R28" sqref="R28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1823,28 +1838,28 @@
   <sheetData>
     <row r="1" spans="1:24">
       <c r="C1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D1" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1" t="s">
         <v>185</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>186</v>
-      </c>
-      <c r="E1" t="s">
-        <v>187</v>
-      </c>
-      <c r="F1" t="s">
-        <v>188</v>
       </c>
       <c r="G1" t="s">
         <v>43</v>
       </c>
       <c r="H1" t="s">
+        <v>187</v>
+      </c>
+      <c r="I1" t="s">
+        <v>188</v>
+      </c>
+      <c r="J1" t="s">
         <v>189</v>
-      </c>
-      <c r="I1" t="s">
-        <v>190</v>
-      </c>
-      <c r="J1" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="2" spans="1:24" ht="15.75" thickBot="1">
@@ -1861,13 +1876,13 @@
         <v>46</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>4</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="H2" s="5" t="s">
         <v>6</v>
@@ -1876,7 +1891,7 @@
         <v>115</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="K2" s="5" t="s">
         <v>63</v>
@@ -1891,34 +1906,34 @@
         <v>3</v>
       </c>
       <c r="O2" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="P2" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="P2" s="1" t="s">
-        <v>211</v>
-      </c>
       <c r="Q2" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="R2" s="53" t="s">
+        <v>214</v>
+      </c>
+      <c r="S2" s="34" t="s">
         <v>212</v>
       </c>
-      <c r="R2" s="53" t="s">
-        <v>216</v>
-      </c>
-      <c r="S2" s="34" t="s">
-        <v>214</v>
-      </c>
       <c r="T2" s="34" t="s">
+        <v>200</v>
+      </c>
+      <c r="U2" s="34" t="s">
+        <v>201</v>
+      </c>
+      <c r="V2" s="34" t="s">
+        <v>208</v>
+      </c>
+      <c r="W2" s="34" t="s">
         <v>202</v>
       </c>
-      <c r="U2" s="34" t="s">
+      <c r="X2" s="34" t="s">
         <v>203</v>
-      </c>
-      <c r="V2" s="34" t="s">
-        <v>210</v>
-      </c>
-      <c r="W2" s="34" t="s">
-        <v>204</v>
-      </c>
-      <c r="X2" s="34" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="3" spans="1:24" ht="15.75" thickTop="1">
@@ -2050,7 +2065,7 @@
         <v>31</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>33</v>
@@ -2235,8 +2250,8 @@
       <c r="A8" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>151</v>
+      <c r="B8" s="56" t="s">
+        <v>224</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>56</v>
@@ -2274,17 +2289,17 @@
       <c r="N8" s="13">
         <v>0</v>
       </c>
-      <c r="O8" s="16">
-        <v>0</v>
-      </c>
-      <c r="P8" s="16">
-        <v>0</v>
+      <c r="O8" s="58" t="s">
+        <v>226</v>
+      </c>
+      <c r="P8" s="58" t="s">
+        <v>225</v>
       </c>
       <c r="Q8" s="16">
         <v>0</v>
       </c>
       <c r="R8" s="46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S8" s="35"/>
       <c r="T8" s="35"/>
@@ -2360,7 +2375,7 @@
         <v>55</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>56</v>
@@ -2419,10 +2434,10 @@
     </row>
     <row r="11" spans="1:24">
       <c r="A11" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>56</v>
@@ -2484,7 +2499,7 @@
         <v>14</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>9</v>
@@ -2608,7 +2623,7 @@
         <v>8</v>
       </c>
       <c r="B14" s="56" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>9</v>
@@ -2856,7 +2871,7 @@
         <v>95</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C18" s="10" t="s">
         <v>60</v>
@@ -3041,8 +3056,8 @@
       <c r="A21" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>177</v>
+      <c r="B21" s="56" t="s">
+        <v>221</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>60</v>
@@ -3080,11 +3095,11 @@
       <c r="N21" s="16">
         <v>0</v>
       </c>
-      <c r="O21" s="16">
-        <v>0</v>
-      </c>
-      <c r="P21" s="16">
-        <v>0</v>
+      <c r="O21" s="58" t="s">
+        <v>222</v>
+      </c>
+      <c r="P21" s="58" t="s">
+        <v>223</v>
       </c>
       <c r="Q21" s="16">
         <v>0</v>
@@ -3420,7 +3435,7 @@
         <v>10</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E27" s="9" t="s">
         <v>106</v>
@@ -3435,7 +3450,7 @@
         <v>0</v>
       </c>
       <c r="I27" s="22">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="J27" s="22">
         <v>0</v>
@@ -3462,7 +3477,7 @@
         <v>3</v>
       </c>
       <c r="R27" s="49">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="S27" s="35"/>
       <c r="T27" s="35"/>
@@ -3476,7 +3491,7 @@
         <v>11</v>
       </c>
       <c r="B28" s="56" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>10</v>
@@ -3597,10 +3612,10 @@
     </row>
     <row r="30" spans="1:24">
       <c r="A30" s="55" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B30" s="56" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C30" s="10" t="s">
         <v>10</v>
@@ -3639,10 +3654,10 @@
         <v>0</v>
       </c>
       <c r="O30" s="57" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="P30" s="57" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="Q30" s="14">
         <v>0</v>
@@ -3845,7 +3860,7 @@
     </row>
     <row r="34" spans="1:24">
       <c r="A34" s="10" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>150</v>
@@ -3907,13 +3922,13 @@
     </row>
     <row r="35" spans="1:24">
       <c r="A35" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="B35" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="B35" s="3" t="s">
-        <v>194</v>
-      </c>
       <c r="C35" s="6" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D35" s="7" t="s">
         <v>47</v>
@@ -3969,13 +3984,13 @@
     </row>
     <row r="36" spans="1:24">
       <c r="A36" s="25" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B36" s="35" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D36" s="7" t="s">
         <v>47</v>
@@ -4031,13 +4046,13 @@
     </row>
     <row r="37" spans="1:24">
       <c r="A37" s="25" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B37" s="35" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D37" s="25" t="s">
         <v>91</v>
@@ -4093,16 +4108,16 @@
     </row>
     <row r="38" spans="1:24">
       <c r="A38" s="25" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B38" s="35" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D38" s="25" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E38" s="25" t="s">
         <v>107</v>
@@ -4403,13 +4418,13 @@
     </row>
     <row r="43" spans="1:24">
       <c r="A43" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>47</v>
@@ -4465,13 +4480,13 @@
     </row>
     <row r="44" spans="1:24">
       <c r="A44" s="25" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B44" s="35" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C44" s="25" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D44" s="25" t="s">
         <v>47</v>
@@ -4527,13 +4542,13 @@
     </row>
     <row r="45" spans="1:24">
       <c r="A45" s="25" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B45" s="35" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C45" s="25" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D45" s="25" t="s">
         <v>47</v>
@@ -4589,13 +4604,13 @@
     </row>
     <row r="46" spans="1:24">
       <c r="A46" s="25" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B46" s="35" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C46" s="25" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D46" s="25" t="s">
         <v>114</v>
@@ -4651,13 +4666,13 @@
     </row>
     <row r="47" spans="1:24">
       <c r="A47" s="25" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B47" s="35" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C47" s="25" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D47" s="25" t="s">
         <v>114</v>
@@ -4902,7 +4917,7 @@
         <v>26</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C51" s="10" t="s">
         <v>22</v>
@@ -5023,10 +5038,10 @@
     </row>
     <row r="53" spans="1:24">
       <c r="A53" s="25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B53" s="35" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C53" s="25" t="s">
         <v>66</v>
@@ -5085,10 +5100,10 @@
     </row>
     <row r="54" spans="1:24">
       <c r="A54" s="25" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B54" s="35" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C54" s="25" t="s">
         <v>66</v>
@@ -5147,10 +5162,10 @@
     </row>
     <row r="55" spans="1:24">
       <c r="A55" s="25" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B55" s="35" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C55" s="25" t="s">
         <v>66</v>
@@ -5398,13 +5413,13 @@
         <v>113</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>84</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>106</v>
@@ -5705,16 +5720,16 @@
     </row>
     <row r="64" spans="1:24">
       <c r="A64" s="25" t="s">
+        <v>178</v>
+      </c>
+      <c r="B64" s="35" t="s">
         <v>180</v>
-      </c>
-      <c r="B64" s="35" t="s">
-        <v>182</v>
       </c>
       <c r="C64" s="25" t="s">
         <v>40</v>
       </c>
       <c r="D64" s="25" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E64" s="25" t="s">
         <v>110</v>
@@ -5894,7 +5909,7 @@
         <v>41</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>40</v>
@@ -5956,7 +5971,7 @@
         <v>42</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C68" s="3" t="s">
         <v>40</v>
@@ -6139,10 +6154,10 @@
     </row>
     <row r="71" spans="1:24">
       <c r="A71" s="30" t="s">
+        <v>164</v>
+      </c>
+      <c r="B71" s="37" t="s">
         <v>165</v>
-      </c>
-      <c r="B71" s="37" t="s">
-        <v>166</v>
       </c>
       <c r="C71" s="30" t="s">
         <v>35</v>

</xml_diff>